<commit_message>
Add unique test data
</commit_message>
<xml_diff>
--- a/src/main/resources/modules/SMOKE.xlsx
+++ b/src/main/resources/modules/SMOKE.xlsx
@@ -1,31 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DSi\Desktop\selemnium1\seleniumTestingFramework\src\main\resources\modules\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ehsan\AMTPublicRipo\AMT-TestFrameWork\src\main\resources\modules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7A2EB36-44D3-4C72-B928-9D3790D78AC7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6F32869-8B2B-4FA1-BAF0-D4A6D9247AEB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="330" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Controller" sheetId="19" r:id="rId1"/>
     <sheet name="TC401_TC500" sheetId="28" r:id="rId2"/>
+    <sheet name="UpdateRevision" sheetId="29" r:id="rId3"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId3"/>
     <externalReference r:id="rId4"/>
+    <externalReference r:id="rId5"/>
+    <externalReference r:id="rId6"/>
+    <externalReference r:id="rId7"/>
   </externalReferences>
   <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="717" uniqueCount="167">
   <si>
     <t>Action</t>
   </si>
@@ -331,13 +334,208 @@
   </si>
   <si>
     <t>Space,$RecurringPayment_spaceInfo_0,Payment/Charge Type,$RecurringPayment_chargeName_0</t>
+  </si>
+  <si>
+    <t>6541329</t>
+  </si>
+  <si>
+    <t>Create</t>
+  </si>
+  <si>
+    <t>#CREATE</t>
+  </si>
+  <si>
+    <t>property,lease,space,recur</t>
+  </si>
+  <si>
+    <t>prequisite handles</t>
+  </si>
+  <si>
+    <t>Preq:102</t>
+  </si>
+  <si>
+    <t>#PREQ</t>
+  </si>
+  <si>
+    <t>$RecurringPayment_LeaseName_0</t>
+  </si>
+  <si>
+    <t>DBA Name,$RecurringPayment_LeaseName_0</t>
+  </si>
+  <si>
+    <t>Click Edit button</t>
+  </si>
+  <si>
+    <t>Edit button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FASB.FIRevisions.btnEdit </t>
+  </si>
+  <si>
+    <t>Calendar - Lessee - Operating - Validate user is able to Update Revision</t>
+  </si>
+  <si>
+    <t>UpdateRevision</t>
+  </si>
+  <si>
+    <t>Set Prepayment</t>
+  </si>
+  <si>
+    <t>Prepayment</t>
+  </si>
+  <si>
+    <t>FASB.FIRevisions.txtPrepayment</t>
+  </si>
+  <si>
+    <t>Set Initial Direct Costs</t>
+  </si>
+  <si>
+    <t>Initial Direct Costs</t>
+  </si>
+  <si>
+    <t>FASB.FIRevisions.txtROU_InitialDirectCosts</t>
+  </si>
+  <si>
+    <t>FASB.FIRevisions.txtROU_LandlordAllowance</t>
+  </si>
+  <si>
+    <t>Set Landlord Allowance</t>
+  </si>
+  <si>
+    <t>Landlord Allowance</t>
+  </si>
+  <si>
+    <t>Click Update button</t>
+  </si>
+  <si>
+    <t>Update button</t>
+  </si>
+  <si>
+    <t>FASB.FIRevisions.btnSave</t>
+  </si>
+  <si>
+    <t>UIBase.WaitingForSuccessfullPopup</t>
+  </si>
+  <si>
+    <t>UIInput.setValue</t>
+  </si>
+  <si>
+    <t>FASB Lease classification</t>
+  </si>
+  <si>
+    <t>Select Lease classification</t>
+  </si>
+  <si>
+    <t>UIDropDown.SelectItem</t>
+  </si>
+  <si>
+    <t>FASB.FIRevisions.FASBClassificationType</t>
+  </si>
+  <si>
+    <t>FASB - Financing</t>
+  </si>
+  <si>
+    <t>FASB/IASB Start Date</t>
+  </si>
+  <si>
+    <t>UIText.SetTextWithoutClear</t>
+  </si>
+  <si>
+    <t>FASB.FIRevisions.level_FASB/IASBStartDate</t>
+  </si>
+  <si>
+    <t>FASB/IASB End Date</t>
+  </si>
+  <si>
+    <t>FASB.FIRevisions.level_FASB/IASBEndDate</t>
+  </si>
+  <si>
+    <t>Add Note</t>
+  </si>
+  <si>
+    <t>Add New</t>
+  </si>
+  <si>
+    <t>FASB.FIRevisions.btnAddNew</t>
+  </si>
+  <si>
+    <t>Set notes</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>FASB.FIRevisions.txtNotes</t>
+  </si>
+  <si>
+    <t>Revision triggered?Revision not triggered</t>
+  </si>
+  <si>
+    <t>FASB.FIRevisions.level_tdPeriods</t>
+  </si>
+  <si>
+    <t>Verify Lease Clasification</t>
+  </si>
+  <si>
+    <t>Lease Clasification</t>
+  </si>
+  <si>
+    <t>FASB.FIRevisions.dpLeaseClasification</t>
+  </si>
+  <si>
+    <t>Update FASB Start Date</t>
+  </si>
+  <si>
+    <t>Update FASB End Date</t>
+  </si>
+  <si>
+    <t>Lease classification verified?Wrong lease classification</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify FASB/IASB Start Date </t>
+  </si>
+  <si>
+    <t xml:space="preserve">FASB/IASB Start Date </t>
+  </si>
+  <si>
+    <t>UIInput.compareValue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify FASB/IASB End Date </t>
+  </si>
+  <si>
+    <t xml:space="preserve">FASB/IASB End Date </t>
+  </si>
+  <si>
+    <t>$RecurringPayment_endDate_0</t>
+  </si>
+  <si>
+    <t>Start Date verified?Wrong start date</t>
+  </si>
+  <si>
+    <t>End Date verified?Wrong start date</t>
+  </si>
+  <si>
+    <t>$RecurringPayment_effDate_0</t>
+  </si>
+  <si>
+    <t>111</t>
+  </si>
+  <si>
+    <t>112</t>
+  </si>
+  <si>
+    <t>113</t>
+  </si>
+  <si>
+    <t>Test unique</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -373,8 +571,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF222222"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF222222"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -408,6 +626,11 @@
       <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
       </patternFill>
     </fill>
   </fills>
@@ -485,11 +708,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -580,12 +804,615 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="1" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="1" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Accent1" xfId="2" builtinId="29"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="105">
+  <dxfs count="179">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1358,6 +2185,32 @@
 </file>
 
 <file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Controller"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Controller"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink4.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -1669,8 +2522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1709,7 +2562,7 @@
         <v>68</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>58</v>
@@ -1729,18 +2582,28 @@
         <v>98</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
+      <c r="A4" s="5">
+        <v>3</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
@@ -3661,340 +4524,340 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H2:H16 H20 H30">
-    <cfRule type="cellIs" dxfId="104" priority="108" operator="equal">
+    <cfRule type="cellIs" dxfId="178" priority="108" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H16 H20 H30">
-    <cfRule type="cellIs" dxfId="103" priority="106" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="102" priority="107" operator="equal">
+    <cfRule type="cellIs" dxfId="177" priority="106" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="176" priority="107" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H17">
-    <cfRule type="cellIs" dxfId="101" priority="104" operator="equal">
+    <cfRule type="cellIs" dxfId="175" priority="104" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H17">
-    <cfRule type="cellIs" dxfId="100" priority="102" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="99" priority="103" operator="equal">
+    <cfRule type="cellIs" dxfId="174" priority="102" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="173" priority="103" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H18">
-    <cfRule type="cellIs" dxfId="98" priority="100" operator="equal">
+    <cfRule type="cellIs" dxfId="172" priority="100" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H18">
-    <cfRule type="cellIs" dxfId="97" priority="98" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="96" priority="99" operator="equal">
+    <cfRule type="cellIs" dxfId="171" priority="98" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="170" priority="99" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H21">
-    <cfRule type="cellIs" dxfId="95" priority="96" operator="equal">
+    <cfRule type="cellIs" dxfId="169" priority="96" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H21">
-    <cfRule type="cellIs" dxfId="94" priority="94" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="93" priority="95" operator="equal">
+    <cfRule type="cellIs" dxfId="168" priority="94" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="167" priority="95" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H28">
-    <cfRule type="cellIs" dxfId="92" priority="88" operator="equal">
+    <cfRule type="cellIs" dxfId="166" priority="88" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H28">
-    <cfRule type="cellIs" dxfId="91" priority="86" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="90" priority="87" operator="equal">
+    <cfRule type="cellIs" dxfId="165" priority="86" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="164" priority="87" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H29">
-    <cfRule type="cellIs" dxfId="89" priority="84" operator="equal">
+    <cfRule type="cellIs" dxfId="163" priority="84" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H29">
-    <cfRule type="cellIs" dxfId="88" priority="82" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="87" priority="83" operator="equal">
+    <cfRule type="cellIs" dxfId="162" priority="82" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="161" priority="83" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H19">
-    <cfRule type="cellIs" dxfId="86" priority="80" operator="equal">
+    <cfRule type="cellIs" dxfId="160" priority="80" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H19">
-    <cfRule type="cellIs" dxfId="85" priority="78" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="84" priority="79" operator="equal">
+    <cfRule type="cellIs" dxfId="159" priority="78" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="158" priority="79" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H26">
-    <cfRule type="cellIs" dxfId="83" priority="76" operator="equal">
+    <cfRule type="cellIs" dxfId="157" priority="76" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H26">
-    <cfRule type="cellIs" dxfId="82" priority="74" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="81" priority="75" operator="equal">
+    <cfRule type="cellIs" dxfId="156" priority="74" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="155" priority="75" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H27">
-    <cfRule type="cellIs" dxfId="80" priority="72" operator="equal">
+    <cfRule type="cellIs" dxfId="154" priority="72" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H27">
-    <cfRule type="cellIs" dxfId="79" priority="70" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="78" priority="71" operator="equal">
+    <cfRule type="cellIs" dxfId="153" priority="70" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="152" priority="71" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H22">
-    <cfRule type="cellIs" dxfId="77" priority="68" operator="equal">
+    <cfRule type="cellIs" dxfId="151" priority="68" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H22">
-    <cfRule type="cellIs" dxfId="76" priority="66" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="75" priority="67" operator="equal">
+    <cfRule type="cellIs" dxfId="150" priority="66" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="149" priority="67" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H23">
-    <cfRule type="cellIs" dxfId="74" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="148" priority="64" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H23">
-    <cfRule type="cellIs" dxfId="73" priority="62" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="63" operator="equal">
+    <cfRule type="cellIs" dxfId="147" priority="62" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="146" priority="63" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H24">
-    <cfRule type="cellIs" dxfId="71" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="145" priority="60" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H24">
-    <cfRule type="cellIs" dxfId="70" priority="58" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="69" priority="59" operator="equal">
+    <cfRule type="cellIs" dxfId="144" priority="58" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="143" priority="59" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H25">
-    <cfRule type="cellIs" dxfId="68" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="142" priority="56" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H25">
-    <cfRule type="cellIs" dxfId="67" priority="54" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="141" priority="54" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="140" priority="55" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H32:H46 H50 H60">
-    <cfRule type="cellIs" dxfId="65" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="139" priority="52" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H32:H46 H50 H60">
-    <cfRule type="cellIs" dxfId="64" priority="50" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="138" priority="50" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="137" priority="51" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H47">
-    <cfRule type="cellIs" dxfId="62" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="136" priority="48" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H47">
-    <cfRule type="cellIs" dxfId="61" priority="46" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="135" priority="46" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="134" priority="47" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H48">
-    <cfRule type="cellIs" dxfId="59" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="133" priority="44" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H48">
-    <cfRule type="cellIs" dxfId="58" priority="42" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="132" priority="42" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="131" priority="43" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H51">
-    <cfRule type="cellIs" dxfId="56" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="130" priority="40" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H51">
-    <cfRule type="cellIs" dxfId="55" priority="38" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="129" priority="38" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="128" priority="39" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H58">
-    <cfRule type="cellIs" dxfId="53" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="127" priority="36" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H58">
-    <cfRule type="cellIs" dxfId="52" priority="34" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="126" priority="34" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="125" priority="35" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H59">
-    <cfRule type="cellIs" dxfId="50" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="124" priority="32" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H59">
-    <cfRule type="cellIs" dxfId="49" priority="30" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="123" priority="30" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="122" priority="31" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H49">
-    <cfRule type="cellIs" dxfId="47" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="121" priority="28" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H49">
-    <cfRule type="cellIs" dxfId="46" priority="26" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="120" priority="26" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="119" priority="27" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H56">
-    <cfRule type="cellIs" dxfId="44" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="118" priority="24" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H56">
-    <cfRule type="cellIs" dxfId="43" priority="22" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="117" priority="22" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="116" priority="23" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H57">
-    <cfRule type="cellIs" dxfId="41" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="115" priority="20" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H57">
-    <cfRule type="cellIs" dxfId="40" priority="18" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="114" priority="18" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="113" priority="19" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H52">
-    <cfRule type="cellIs" dxfId="38" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="112" priority="16" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H52">
-    <cfRule type="cellIs" dxfId="37" priority="14" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="111" priority="14" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="110" priority="15" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H53">
-    <cfRule type="cellIs" dxfId="35" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="109" priority="12" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H53">
-    <cfRule type="cellIs" dxfId="34" priority="10" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="108" priority="10" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="107" priority="11" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H54">
-    <cfRule type="cellIs" dxfId="32" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="106" priority="8" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H54">
-    <cfRule type="cellIs" dxfId="31" priority="6" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="105" priority="6" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="104" priority="7" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H55">
-    <cfRule type="cellIs" dxfId="29" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="103" priority="4" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H55">
-    <cfRule type="cellIs" dxfId="28" priority="2" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="102" priority="2" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="101" priority="3" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4363,4 +5226,1971 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CE87BF7-3C91-45AC-BD7A-97ED35B7B19B}">
+  <dimension ref="A1:L65"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D7" workbookViewId="0">
+      <selection activeCell="H38" sqref="H38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" style="40" customWidth="1"/>
+    <col min="2" max="2" width="11" style="36" customWidth="1"/>
+    <col min="3" max="3" width="55.140625" style="36" customWidth="1"/>
+    <col min="4" max="5" width="50.7109375" style="33" customWidth="1"/>
+    <col min="6" max="6" width="50.7109375" style="36" customWidth="1"/>
+    <col min="7" max="7" width="35.42578125" style="33" customWidth="1"/>
+    <col min="8" max="8" width="14" style="54" customWidth="1"/>
+    <col min="9" max="9" width="16.140625" style="33" customWidth="1"/>
+    <col min="10" max="10" width="17.7109375" style="33" customWidth="1"/>
+    <col min="11" max="11" width="50.42578125" style="36" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="36"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" s="33" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="K1" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="L1" s="33" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="34"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="56" t="s">
+        <v>114</v>
+      </c>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="56"/>
+      <c r="J2" s="56"/>
+      <c r="K2" s="35"/>
+      <c r="L2" s="35"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="B3" s="17">
+        <v>1</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="F3" s="17"/>
+      <c r="G3" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="H3" s="16"/>
+      <c r="I3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" s="17"/>
+      <c r="K3" s="33"/>
+      <c r="L3" s="33"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="B4" s="37">
+        <v>2</v>
+      </c>
+      <c r="C4" s="38" t="s">
+        <v>106</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="F4" s="21"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J4" s="40" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="B5" s="37">
+        <v>1</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="D5" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="F5" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="39"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J5" s="40" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="B6" s="37">
+        <v>2</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="F6" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" s="16"/>
+      <c r="I6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J6" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="L6" s="36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="B7" s="37">
+        <v>3</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="E7" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="F7" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" s="16"/>
+      <c r="I7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J7" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="L7" s="36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="B8" s="37">
+        <v>4</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="F8" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="41" t="s">
+        <v>23</v>
+      </c>
+      <c r="H8" s="16"/>
+      <c r="I8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J8" s="40" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="B9" s="37">
+        <v>5</v>
+      </c>
+      <c r="C9" s="21"/>
+      <c r="D9" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="F9" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="H9" s="16"/>
+      <c r="I9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J9" s="40" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="B10" s="17">
+        <v>6</v>
+      </c>
+      <c r="C10" s="21"/>
+      <c r="D10" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="F10" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" s="25"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="J10" s="40" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="B11" s="17">
+        <v>7</v>
+      </c>
+      <c r="C11" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="F11" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="H11" s="1"/>
+      <c r="I11" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="J11" s="42" t="s">
+        <v>2</v>
+      </c>
+      <c r="L11" s="36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="B12" s="17">
+        <v>8</v>
+      </c>
+      <c r="C12" s="21"/>
+      <c r="D12" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="F12" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="G12" s="25"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="J12" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="L12" s="36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="B13" s="17">
+        <v>9</v>
+      </c>
+      <c r="C13" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="F13" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="G13" s="25"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="J13" s="40" t="s">
+        <v>2</v>
+      </c>
+      <c r="L13" s="36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="B14" s="17">
+        <v>10</v>
+      </c>
+      <c r="C14" s="21"/>
+      <c r="D14" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="E14" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="F14" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="G14" s="25"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="J14" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="L14" s="36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="B15" s="17">
+        <v>11</v>
+      </c>
+      <c r="C15" s="21"/>
+      <c r="D15" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F15" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="G15" s="43" t="s">
+        <v>109</v>
+      </c>
+      <c r="H15" s="1"/>
+      <c r="I15" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="J15" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="L15" s="36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="B16" s="17">
+        <v>12</v>
+      </c>
+      <c r="C16" s="21"/>
+      <c r="D16" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F16" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H16" s="1"/>
+      <c r="I16" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="J16" s="40" t="s">
+        <v>2</v>
+      </c>
+      <c r="L16" s="36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="B17" s="17">
+        <v>13</v>
+      </c>
+      <c r="C17" s="21"/>
+      <c r="D17" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F17" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="H17" s="1"/>
+      <c r="I17" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="J17" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="L17" s="36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="B18" s="17">
+        <v>14</v>
+      </c>
+      <c r="C18" s="21"/>
+      <c r="D18" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F18" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="H18" s="1"/>
+      <c r="I18" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="J18" s="40" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="B19" s="37">
+        <v>16</v>
+      </c>
+      <c r="C19" s="44" t="s">
+        <v>76</v>
+      </c>
+      <c r="D19" s="40" t="s">
+        <v>48</v>
+      </c>
+      <c r="E19" s="33" t="s">
+        <v>72</v>
+      </c>
+      <c r="F19" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="G19" s="45" t="s">
+        <v>70</v>
+      </c>
+      <c r="H19" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J19" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="K19" s="36" t="s">
+        <v>146</v>
+      </c>
+      <c r="L19" s="36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="B20" s="37"/>
+      <c r="C20" s="36" t="s">
+        <v>111</v>
+      </c>
+      <c r="D20" s="42" t="s">
+        <v>112</v>
+      </c>
+      <c r="E20" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="F20" s="46" t="s">
+        <v>113</v>
+      </c>
+      <c r="G20" s="45"/>
+      <c r="H20" s="16"/>
+      <c r="I20" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J20" s="42" t="s">
+        <v>2</v>
+      </c>
+      <c r="L20" s="36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="47"/>
+      <c r="B21" s="48"/>
+      <c r="C21" s="57"/>
+      <c r="D21" s="57"/>
+      <c r="E21" s="57"/>
+      <c r="F21" s="57"/>
+      <c r="G21" s="49"/>
+      <c r="H21" s="16"/>
+      <c r="I21" s="17"/>
+      <c r="J21" s="49"/>
+      <c r="K21" s="50"/>
+      <c r="L21" s="50"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="B22" s="37">
+        <v>19</v>
+      </c>
+      <c r="C22" s="31" t="s">
+        <v>151</v>
+      </c>
+      <c r="D22" s="58" t="s">
+        <v>135</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F22" s="46" t="s">
+        <v>137</v>
+      </c>
+      <c r="G22" s="43" t="s">
+        <v>162</v>
+      </c>
+      <c r="I22" s="51" t="s">
+        <v>2</v>
+      </c>
+      <c r="J22" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="L22" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="B23" s="37"/>
+      <c r="D23" s="42"/>
+      <c r="E23" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="F23" s="46" t="s">
+        <v>147</v>
+      </c>
+      <c r="G23" s="45"/>
+      <c r="H23" s="16"/>
+      <c r="I23" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J23" s="42" t="s">
+        <v>2</v>
+      </c>
+      <c r="L23" s="36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="B24" s="37">
+        <v>20</v>
+      </c>
+      <c r="C24" s="31" t="s">
+        <v>152</v>
+      </c>
+      <c r="D24" s="58" t="s">
+        <v>138</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F24" s="46" t="s">
+        <v>139</v>
+      </c>
+      <c r="G24" s="43" t="s">
+        <v>159</v>
+      </c>
+      <c r="I24" s="51" t="s">
+        <v>2</v>
+      </c>
+      <c r="J24" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="L24" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="B25" s="37"/>
+      <c r="D25" s="42"/>
+      <c r="E25" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="F25" s="46" t="s">
+        <v>147</v>
+      </c>
+      <c r="G25" s="45"/>
+      <c r="H25" s="16"/>
+      <c r="I25" s="51" t="s">
+        <v>2</v>
+      </c>
+      <c r="J25" s="42" t="s">
+        <v>2</v>
+      </c>
+      <c r="L25" s="36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="B26" s="37"/>
+      <c r="C26" s="36" t="s">
+        <v>131</v>
+      </c>
+      <c r="D26" s="42" t="s">
+        <v>130</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F26" s="46" t="s">
+        <v>133</v>
+      </c>
+      <c r="G26" s="52" t="s">
+        <v>134</v>
+      </c>
+      <c r="H26" s="16"/>
+      <c r="I26" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J26" s="42" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="B27" s="37">
+        <v>24</v>
+      </c>
+      <c r="C27" s="36" t="s">
+        <v>140</v>
+      </c>
+      <c r="D27" s="33" t="s">
+        <v>141</v>
+      </c>
+      <c r="E27" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="F27" s="59" t="s">
+        <v>142</v>
+      </c>
+      <c r="I27" s="51" t="s">
+        <v>2</v>
+      </c>
+      <c r="J27" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="L27" s="33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="B28" s="37"/>
+      <c r="C28" s="36" t="s">
+        <v>143</v>
+      </c>
+      <c r="D28" s="42" t="s">
+        <v>144</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F28" s="46" t="s">
+        <v>145</v>
+      </c>
+      <c r="G28" s="55" t="s">
+        <v>166</v>
+      </c>
+      <c r="H28" s="16"/>
+      <c r="I28" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J28" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="L28" s="36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="B29" s="37"/>
+      <c r="C29" s="36" t="s">
+        <v>116</v>
+      </c>
+      <c r="D29" s="42" t="s">
+        <v>117</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="F29" s="46" t="s">
+        <v>118</v>
+      </c>
+      <c r="G29" s="55" t="s">
+        <v>163</v>
+      </c>
+      <c r="H29" s="16"/>
+      <c r="I29" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J29" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="L29" s="36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="B30" s="37"/>
+      <c r="C30" s="36" t="s">
+        <v>119</v>
+      </c>
+      <c r="D30" s="42" t="s">
+        <v>120</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="F30" s="46" t="s">
+        <v>121</v>
+      </c>
+      <c r="G30" s="55" t="s">
+        <v>164</v>
+      </c>
+      <c r="H30" s="16"/>
+      <c r="I30" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J30" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="L30" s="36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="B31" s="37"/>
+      <c r="C31" s="36" t="s">
+        <v>123</v>
+      </c>
+      <c r="D31" s="42" t="s">
+        <v>124</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="F31" s="46" t="s">
+        <v>122</v>
+      </c>
+      <c r="G31" s="55" t="s">
+        <v>165</v>
+      </c>
+      <c r="H31" s="16"/>
+      <c r="I31" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J31" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="L31" s="36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="B32" s="37"/>
+      <c r="C32" s="36" t="s">
+        <v>125</v>
+      </c>
+      <c r="D32" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="E32" s="51" t="s">
+        <v>52</v>
+      </c>
+      <c r="F32" s="46" t="s">
+        <v>127</v>
+      </c>
+      <c r="G32" s="45"/>
+      <c r="H32" s="16"/>
+      <c r="I32" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J32" s="42" t="s">
+        <v>2</v>
+      </c>
+      <c r="L32" s="36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="B33" s="37"/>
+      <c r="D33" s="42"/>
+      <c r="E33" s="51" t="s">
+        <v>128</v>
+      </c>
+      <c r="F33" s="46"/>
+      <c r="G33" s="45"/>
+      <c r="H33" s="16"/>
+      <c r="I33" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J33" s="42" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="B34" s="37"/>
+      <c r="C34" s="36" t="s">
+        <v>111</v>
+      </c>
+      <c r="D34" s="42" t="s">
+        <v>112</v>
+      </c>
+      <c r="E34" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="F34" s="46" t="s">
+        <v>113</v>
+      </c>
+      <c r="G34" s="45"/>
+      <c r="H34" s="16"/>
+      <c r="I34" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J34" s="42" t="s">
+        <v>2</v>
+      </c>
+      <c r="L34" s="36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="B35" s="19">
+        <v>21</v>
+      </c>
+      <c r="C35" s="31" t="s">
+        <v>148</v>
+      </c>
+      <c r="D35" s="60" t="s">
+        <v>149</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F35" s="61" t="s">
+        <v>150</v>
+      </c>
+      <c r="G35" s="52" t="s">
+        <v>134</v>
+      </c>
+      <c r="H35" s="29"/>
+      <c r="I35" s="62" t="s">
+        <v>2</v>
+      </c>
+      <c r="J35" s="63" t="s">
+        <v>12</v>
+      </c>
+      <c r="K35" t="s">
+        <v>153</v>
+      </c>
+      <c r="L35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="C36" s="36" t="s">
+        <v>154</v>
+      </c>
+      <c r="D36" s="33" t="s">
+        <v>155</v>
+      </c>
+      <c r="E36" s="33" t="s">
+        <v>156</v>
+      </c>
+      <c r="F36" s="36" t="s">
+        <v>137</v>
+      </c>
+      <c r="G36" s="43" t="s">
+        <v>162</v>
+      </c>
+      <c r="I36" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="J36" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="K36" s="36" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="B37" s="17"/>
+      <c r="C37" s="21" t="s">
+        <v>157</v>
+      </c>
+      <c r="D37" s="22" t="s">
+        <v>158</v>
+      </c>
+      <c r="E37" s="22" t="s">
+        <v>156</v>
+      </c>
+      <c r="F37" s="24" t="s">
+        <v>139</v>
+      </c>
+      <c r="G37" s="43" t="s">
+        <v>159</v>
+      </c>
+      <c r="H37" s="1"/>
+      <c r="I37" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="J37" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="K37" s="36" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38" s="53"/>
+      <c r="B38" s="17"/>
+      <c r="C38" s="21"/>
+      <c r="D38" s="22"/>
+      <c r="E38" s="25"/>
+      <c r="F38" s="21"/>
+      <c r="G38" s="25"/>
+      <c r="H38" s="1"/>
+      <c r="J38" s="40"/>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39" s="53"/>
+      <c r="B39" s="17"/>
+      <c r="C39" s="21"/>
+      <c r="D39" s="22"/>
+      <c r="E39" s="25"/>
+      <c r="F39" s="21"/>
+      <c r="G39" s="25"/>
+      <c r="H39" s="1"/>
+      <c r="J39" s="40"/>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A40" s="53"/>
+      <c r="B40" s="17"/>
+      <c r="C40" s="21"/>
+      <c r="D40" s="22"/>
+      <c r="E40" s="6"/>
+      <c r="F40" s="24"/>
+      <c r="G40" s="6"/>
+      <c r="H40" s="1"/>
+      <c r="J40" s="40"/>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41" s="53"/>
+      <c r="B41" s="17"/>
+      <c r="C41" s="21"/>
+      <c r="D41" s="22"/>
+      <c r="E41" s="6"/>
+      <c r="F41" s="24"/>
+      <c r="G41" s="6"/>
+      <c r="H41" s="1"/>
+      <c r="J41" s="40"/>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A42" s="53"/>
+      <c r="B42" s="17"/>
+      <c r="C42" s="21"/>
+      <c r="D42" s="22"/>
+      <c r="E42" s="22"/>
+      <c r="F42" s="24"/>
+      <c r="G42" s="25"/>
+      <c r="H42" s="1"/>
+      <c r="J42" s="40"/>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A43" s="53"/>
+      <c r="B43" s="17"/>
+      <c r="C43" s="21"/>
+      <c r="D43" s="22"/>
+      <c r="E43" s="6"/>
+      <c r="F43" s="24"/>
+      <c r="G43" s="6"/>
+      <c r="H43" s="1"/>
+      <c r="I43" s="22"/>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A44" s="53"/>
+      <c r="B44" s="17"/>
+      <c r="C44" s="21"/>
+      <c r="D44" s="22"/>
+      <c r="E44" s="22"/>
+      <c r="F44" s="24"/>
+      <c r="G44" s="25"/>
+      <c r="H44" s="1"/>
+      <c r="I44" s="22"/>
+      <c r="J44" s="40"/>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A45" s="53"/>
+      <c r="B45" s="17"/>
+      <c r="C45" s="21"/>
+      <c r="D45" s="22"/>
+      <c r="E45" s="1"/>
+      <c r="F45" s="24"/>
+      <c r="G45" s="25"/>
+      <c r="H45" s="1"/>
+      <c r="I45" s="22"/>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A46" s="53"/>
+      <c r="B46" s="17"/>
+      <c r="C46" s="21"/>
+      <c r="D46" s="22"/>
+      <c r="E46" s="22"/>
+      <c r="F46" s="24"/>
+      <c r="G46" s="25"/>
+      <c r="H46" s="1"/>
+      <c r="I46" s="22"/>
+      <c r="J46" s="40"/>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A47" s="53"/>
+      <c r="B47" s="17"/>
+      <c r="C47" s="21"/>
+      <c r="D47" s="22"/>
+      <c r="E47" s="1"/>
+      <c r="F47" s="24"/>
+      <c r="G47" s="43"/>
+      <c r="H47" s="1"/>
+      <c r="I47" s="22"/>
+      <c r="J47" s="40"/>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A48" s="53"/>
+      <c r="B48" s="17"/>
+      <c r="C48" s="21"/>
+      <c r="D48" s="22"/>
+      <c r="E48" s="1"/>
+      <c r="F48" s="24"/>
+      <c r="G48" s="6"/>
+      <c r="H48" s="1"/>
+      <c r="I48" s="22"/>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49" s="53"/>
+      <c r="B49" s="17"/>
+      <c r="C49" s="21"/>
+      <c r="D49" s="22"/>
+      <c r="E49" s="1"/>
+      <c r="F49" s="24"/>
+      <c r="G49" s="6"/>
+      <c r="H49" s="1"/>
+      <c r="I49" s="22"/>
+      <c r="J49" s="40"/>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50" s="53"/>
+      <c r="B50" s="17"/>
+      <c r="C50" s="21"/>
+      <c r="D50" s="22"/>
+      <c r="E50" s="1"/>
+      <c r="F50" s="24"/>
+      <c r="G50" s="6"/>
+      <c r="H50" s="1"/>
+      <c r="I50" s="22"/>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A51" s="53"/>
+      <c r="B51" s="17"/>
+      <c r="C51" s="21"/>
+      <c r="D51" s="22"/>
+      <c r="E51" s="1"/>
+      <c r="F51" s="24"/>
+      <c r="G51" s="6"/>
+      <c r="H51" s="1"/>
+      <c r="I51" s="22"/>
+      <c r="J51" s="40"/>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A52" s="53"/>
+      <c r="B52" s="17"/>
+      <c r="C52" s="31"/>
+      <c r="D52" s="25"/>
+      <c r="E52" s="1"/>
+      <c r="F52" s="24"/>
+      <c r="G52" s="5"/>
+      <c r="H52" s="1"/>
+      <c r="I52" s="22"/>
+      <c r="J52" s="40"/>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A53" s="53"/>
+      <c r="B53" s="17"/>
+      <c r="C53" s="31"/>
+      <c r="D53" s="25"/>
+      <c r="E53" s="1"/>
+      <c r="F53" s="24"/>
+      <c r="G53" s="5"/>
+      <c r="H53" s="1"/>
+      <c r="I53" s="22"/>
+      <c r="J53" s="40"/>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A54" s="53"/>
+      <c r="B54" s="17"/>
+      <c r="C54" s="31"/>
+      <c r="D54" s="25"/>
+      <c r="E54" s="1"/>
+      <c r="F54" s="24"/>
+      <c r="G54" s="5"/>
+      <c r="H54" s="1"/>
+      <c r="I54" s="22"/>
+      <c r="J54" s="40"/>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A55" s="53"/>
+      <c r="B55" s="17"/>
+      <c r="C55" s="31"/>
+      <c r="D55" s="25"/>
+      <c r="E55" s="1"/>
+      <c r="F55" s="24"/>
+      <c r="G55" s="5"/>
+      <c r="H55" s="1"/>
+      <c r="I55" s="22"/>
+      <c r="J55" s="40"/>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A56" s="53"/>
+      <c r="B56" s="17"/>
+      <c r="C56" s="31"/>
+      <c r="D56" s="25"/>
+      <c r="E56" s="1"/>
+      <c r="F56" s="24"/>
+      <c r="G56" s="5"/>
+      <c r="H56" s="1"/>
+      <c r="I56" s="22"/>
+      <c r="J56" s="40"/>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A57" s="53"/>
+      <c r="B57" s="17"/>
+      <c r="C57" s="31"/>
+      <c r="D57" s="25"/>
+      <c r="E57" s="1"/>
+      <c r="F57" s="24"/>
+      <c r="G57" s="5"/>
+      <c r="H57" s="1"/>
+      <c r="I57" s="22"/>
+      <c r="J57" s="40"/>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A58" s="53"/>
+      <c r="B58" s="17"/>
+      <c r="C58" s="31"/>
+      <c r="D58" s="25"/>
+      <c r="E58" s="1"/>
+      <c r="F58" s="24"/>
+      <c r="G58" s="5"/>
+      <c r="H58" s="1"/>
+      <c r="I58" s="22"/>
+      <c r="J58" s="40"/>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A59" s="53"/>
+      <c r="B59" s="17"/>
+      <c r="C59" s="31"/>
+      <c r="D59" s="25"/>
+      <c r="E59" s="1"/>
+      <c r="F59" s="24"/>
+      <c r="G59" s="5"/>
+      <c r="H59" s="1"/>
+      <c r="I59" s="22"/>
+      <c r="J59" s="40"/>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A60" s="53"/>
+      <c r="B60" s="17"/>
+      <c r="C60" s="31"/>
+      <c r="D60" s="25"/>
+      <c r="E60" s="1"/>
+      <c r="F60" s="24"/>
+      <c r="G60" s="5"/>
+      <c r="H60" s="1"/>
+      <c r="I60" s="22"/>
+      <c r="J60" s="40"/>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A61" s="53"/>
+      <c r="B61" s="17"/>
+      <c r="C61" s="31"/>
+      <c r="D61" s="25"/>
+      <c r="E61" s="1"/>
+      <c r="F61" s="24"/>
+      <c r="G61" s="5"/>
+      <c r="H61" s="1"/>
+      <c r="I61" s="22"/>
+      <c r="J61" s="40"/>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A62" s="53"/>
+      <c r="B62" s="17"/>
+      <c r="C62" s="31"/>
+      <c r="D62" s="25"/>
+      <c r="E62" s="1"/>
+      <c r="F62" s="24"/>
+      <c r="G62" s="5"/>
+      <c r="H62" s="1"/>
+      <c r="I62" s="22"/>
+      <c r="J62" s="40"/>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A63" s="53"/>
+      <c r="B63" s="17"/>
+      <c r="C63" s="31"/>
+      <c r="D63" s="25"/>
+      <c r="E63" s="1"/>
+      <c r="F63" s="24"/>
+      <c r="G63" s="5"/>
+      <c r="H63" s="1"/>
+      <c r="I63" s="22"/>
+      <c r="J63" s="40"/>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A64" s="53"/>
+      <c r="B64" s="17"/>
+      <c r="C64" s="31"/>
+      <c r="D64" s="25"/>
+      <c r="E64" s="1"/>
+      <c r="F64" s="24"/>
+      <c r="G64" s="5"/>
+      <c r="H64" s="1"/>
+      <c r="I64" s="22"/>
+      <c r="J64" s="40"/>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A65" s="53"/>
+      <c r="B65" s="17"/>
+      <c r="C65" s="44"/>
+      <c r="D65" s="22"/>
+      <c r="E65" s="22"/>
+      <c r="F65" s="44"/>
+      <c r="G65" s="40"/>
+      <c r="H65" s="1"/>
+      <c r="I65" s="22"/>
+      <c r="J65" s="40"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C2:J2"/>
+    <mergeCell ref="C21:F21"/>
+  </mergeCells>
+  <conditionalFormatting sqref="H37:H51 H55 H65">
+    <cfRule type="cellIs" dxfId="70" priority="75" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H37:H51 H55 H65">
+    <cfRule type="cellIs" dxfId="69" priority="73" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="68" priority="74" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H52">
+    <cfRule type="cellIs" dxfId="67" priority="71" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H52">
+    <cfRule type="cellIs" dxfId="66" priority="69" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="65" priority="70" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H53">
+    <cfRule type="cellIs" dxfId="64" priority="67" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H53">
+    <cfRule type="cellIs" dxfId="63" priority="65" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="62" priority="66" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H56">
+    <cfRule type="cellIs" dxfId="61" priority="63" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H56">
+    <cfRule type="cellIs" dxfId="60" priority="61" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="59" priority="62" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H63">
+    <cfRule type="cellIs" dxfId="58" priority="59" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H63">
+    <cfRule type="cellIs" dxfId="57" priority="57" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="56" priority="58" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H64">
+    <cfRule type="cellIs" dxfId="55" priority="55" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H64">
+    <cfRule type="cellIs" dxfId="54" priority="53" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="53" priority="54" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H54">
+    <cfRule type="cellIs" dxfId="52" priority="51" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H54">
+    <cfRule type="cellIs" dxfId="51" priority="49" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="50" priority="50" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H61">
+    <cfRule type="cellIs" dxfId="49" priority="47" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H61">
+    <cfRule type="cellIs" dxfId="48" priority="45" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="47" priority="46" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H62">
+    <cfRule type="cellIs" dxfId="46" priority="43" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H62">
+    <cfRule type="cellIs" dxfId="45" priority="41" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="44" priority="42" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H57">
+    <cfRule type="cellIs" dxfId="43" priority="39" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H57">
+    <cfRule type="cellIs" dxfId="42" priority="37" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="41" priority="38" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H58">
+    <cfRule type="cellIs" dxfId="40" priority="35" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H58">
+    <cfRule type="cellIs" dxfId="39" priority="33" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="38" priority="34" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H59">
+    <cfRule type="cellIs" dxfId="37" priority="31" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H59">
+    <cfRule type="cellIs" dxfId="36" priority="29" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="35" priority="30" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H60">
+    <cfRule type="cellIs" dxfId="34" priority="27" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H60">
+    <cfRule type="cellIs" dxfId="33" priority="25" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="32" priority="26" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H10:H18">
+    <cfRule type="cellIs" dxfId="31" priority="22" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H10:H18">
+    <cfRule type="cellIs" dxfId="30" priority="20" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="29" priority="21" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H37:H65 H10:H18" xr:uid="{9C714141-7DE7-49DA-A661-FCE85EC1A298}">
+      <formula1>#REF!</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="88" operator="equal" id="{AC584969-8ED5-494A-82D1-FD30706166EE}">
+            <xm:f>'\Users\DSi\Documents\Users\DSi\Desktop\backuo\src\main\resources\modules\[sample.xlsx]Controller'!#REF!</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="5" tint="0.39994506668294322"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>H1</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="72" operator="equal" id="{8E2C6DA8-A3C1-45B3-9794-468ADF79D851}">
+            <xm:f>'\Users\DSi\Documents\Users\naveeng\Documents\Builds\AMTDirectAutomationSuite11\AMTDirectAutomationSuite\Framework\Modules\[PortFolioInsight.xlsx]Controller'!#REF!</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="5" tint="0.39994506668294322"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>H37:H51 H55 H65</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="68" operator="equal" id="{676A36EB-3DF3-4A9E-B344-1544F770C7A2}">
+            <xm:f>'\Users\DSi\Documents\Users\naveeng\Documents\Builds\AMTDirectAutomationSuite11\AMTDirectAutomationSuite\Framework\Modules\[PortFolioInsight.xlsx]Controller'!#REF!</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="5" tint="0.39994506668294322"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>H52</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="64" operator="equal" id="{7EA5D274-53AB-4DF7-983D-63FB8F42560A}">
+            <xm:f>'\Users\DSi\Documents\Users\naveeng\Documents\Builds\AMTDirectAutomationSuite11\AMTDirectAutomationSuite\Framework\Modules\[PortFolioInsight.xlsx]Controller'!#REF!</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="5" tint="0.39994506668294322"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>H53</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="60" operator="equal" id="{12A6CF38-7B92-43E2-ABD8-24703CF66017}">
+            <xm:f>'\Users\DSi\Documents\Users\naveeng\Documents\Builds\AMTDirectAutomationSuite11\AMTDirectAutomationSuite\Framework\Modules\[PortFolioInsight.xlsx]Controller'!#REF!</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="5" tint="0.39994506668294322"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>H56</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="56" operator="equal" id="{4F16A991-16DF-4053-AE09-0ED47F6677AE}">
+            <xm:f>'\Users\DSi\Documents\Users\naveeng\Documents\Builds\AMTDirectAutomationSuite11\AMTDirectAutomationSuite\Framework\Modules\[PortFolioInsight.xlsx]Controller'!#REF!</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="5" tint="0.39994506668294322"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>H63</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="52" operator="equal" id="{63E7DCA0-0E2A-45A7-9F8B-FA25967D4489}">
+            <xm:f>'\Users\DSi\Documents\Users\naveeng\Documents\Builds\AMTDirectAutomationSuite11\AMTDirectAutomationSuite\Framework\Modules\[PortFolioInsight.xlsx]Controller'!#REF!</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="5" tint="0.39994506668294322"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>H64</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="48" operator="equal" id="{C9A447BB-BE12-4A63-9B15-39220806C8E2}">
+            <xm:f>'\Users\DSi\Documents\Users\naveeng\Documents\Builds\AMTDirectAutomationSuite11\AMTDirectAutomationSuite\Framework\Modules\[PortFolioInsight.xlsx]Controller'!#REF!</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="5" tint="0.39994506668294322"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>H54</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="44" operator="equal" id="{61D4B09B-99F3-4441-A57A-09EB2E5050D6}">
+            <xm:f>'\Users\DSi\Documents\Users\naveeng\Documents\Builds\AMTDirectAutomationSuite11\AMTDirectAutomationSuite\Framework\Modules\[PortFolioInsight.xlsx]Controller'!#REF!</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="5" tint="0.39994506668294322"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>H61</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="40" operator="equal" id="{5A87A78C-98C5-4648-96B9-D8362A21BB1C}">
+            <xm:f>'\Users\DSi\Documents\Users\naveeng\Documents\Builds\AMTDirectAutomationSuite11\AMTDirectAutomationSuite\Framework\Modules\[PortFolioInsight.xlsx]Controller'!#REF!</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="5" tint="0.39994506668294322"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>H62</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="36" operator="equal" id="{82D9DE22-A6C3-41BA-B973-4A53362F5E92}">
+            <xm:f>'\Users\DSi\Documents\Users\naveeng\Documents\Builds\AMTDirectAutomationSuite11\AMTDirectAutomationSuite\Framework\Modules\[PortFolioInsight.xlsx]Controller'!#REF!</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="5" tint="0.39994506668294322"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>H57</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="32" operator="equal" id="{0215D699-028F-4112-AF73-51E9D18905B1}">
+            <xm:f>'\Users\DSi\Documents\Users\naveeng\Documents\Builds\AMTDirectAutomationSuite11\AMTDirectAutomationSuite\Framework\Modules\[PortFolioInsight.xlsx]Controller'!#REF!</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="5" tint="0.39994506668294322"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>H58</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="28" operator="equal" id="{E4517FB0-F1C2-4BC3-8CED-C8584589B3B7}">
+            <xm:f>'\Users\DSi\Documents\Users\naveeng\Documents\Builds\AMTDirectAutomationSuite11\AMTDirectAutomationSuite\Framework\Modules\[PortFolioInsight.xlsx]Controller'!#REF!</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="5" tint="0.39994506668294322"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>H59</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="24" operator="equal" id="{4C7ADB0E-686E-44DC-89CE-AF09146385E1}">
+            <xm:f>'\Users\DSi\Documents\Users\naveeng\Documents\Builds\AMTDirectAutomationSuite11\AMTDirectAutomationSuite\Framework\Modules\[PortFolioInsight.xlsx]Controller'!#REF!</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="5" tint="0.39994506668294322"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>H60</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="23" operator="equal" id="{405BAF02-FB5D-45A8-A810-A24E6C8DC018}">
+            <xm:f>'\Users\DSi\Documents\Users\DSi\Desktop\backuo\src\main\resources\modules\[sample.xlsx]Controller'!#REF!</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="5" tint="0.39994506668294322"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>H3:H9 H19:H21</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="19" operator="equal" id="{A0D0E590-80F7-4052-8ECA-43A425414079}">
+            <xm:f>'\Users\DSi\Documents\Users\naveeng\Documents\Builds\AMTDirectAutomationSuite11\AMTDirectAutomationSuite\Framework\Modules\[PortFolioInsight.xlsx]Controller'!#REF!</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="5" tint="0.39994506668294322"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>H10:H18</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="12" operator="equal" id="{D95833B8-28CE-4218-9432-718E358F0DEB}">
+            <xm:f>'\Users\DSi\Documents\Users\DSi\Desktop\backuo\src\main\resources\modules\[sample.xlsx]Controller'!#REF!</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="5" tint="0.39994506668294322"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>H29</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="11" operator="equal" id="{3F180771-AB84-471A-A2DB-3FF3A8781118}">
+            <xm:f>'\Users\DSi\Documents\Users\DSi\Desktop\backuo\src\main\resources\modules\[sample.xlsx]Controller'!#REF!</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="5" tint="0.39994506668294322"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>H30</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="10" operator="equal" id="{A19297AE-E58C-4E7A-A726-423D420F3B57}">
+            <xm:f>'\Users\DSi\Documents\Users\DSi\Desktop\backuo\src\main\resources\modules\[sample.xlsx]Controller'!#REF!</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="5" tint="0.39994506668294322"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>H31</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="9" operator="equal" id="{24FAECC6-86D6-4752-A8FB-527CA2946952}">
+            <xm:f>'\Users\DSi\Documents\Users\DSi\Desktop\backuo\src\main\resources\modules\[sample.xlsx]Controller'!#REF!</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="5" tint="0.39994506668294322"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>H32</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="8" operator="equal" id="{30916333-4FD0-4DB4-8722-C19598E52425}">
+            <xm:f>'\Users\DSi\Documents\Users\DSi\Desktop\backuo\src\main\resources\modules\[sample.xlsx]Controller'!#REF!</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="5" tint="0.39994506668294322"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>H33</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="7" operator="equal" id="{60D88BE3-49B5-431F-8963-4DB0D1A6C9BA}">
+            <xm:f>'\Users\DSi\Documents\Users\DSi\Desktop\backuo\src\main\resources\modules\[sample.xlsx]Controller'!#REF!</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="5" tint="0.39994506668294322"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>H34</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="6" operator="equal" id="{2F163E15-011A-480A-926C-C4A51611ED9B}">
+            <xm:f>'\Users\DSi\Documents\Users\DSi\Desktop\backuo\src\main\resources\modules\[sample.xlsx]Controller'!#REF!</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="5" tint="0.39994506668294322"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>H26</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="4" operator="equal" id="{FDCEF14C-0760-4F83-BC4D-33428F4CA25F}">
+            <xm:f>'\Users\DSi\Documents\Users\DSi\Desktop\backuo\src\main\resources\modules\[sample.xlsx]Controller'!#REF!</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="5" tint="0.39994506668294322"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>H28</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="2" operator="equal" id="{C7113A6B-D844-47A1-B1FA-F5239D87A51A}">
+            <xm:f>'\Users\DSi\Documents\Users\DSi\Desktop\backuo\src\main\resources\modules\[sample.xlsx]Controller'!#REF!</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="5" tint="0.39994506668294322"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>H23</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="1" operator="equal" id="{34468DF2-664C-493D-97F3-591E289332FB}">
+            <xm:f>'\Users\DSi\Documents\Users\DSi\Desktop\backuo\src\main\resources\modules\[sample.xlsx]Controller'!#REF!</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="5" tint="0.39994506668294322"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>H25</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add smoke test case for update revision
</commit_message>
<xml_diff>
--- a/src/main/resources/modules/SMOKE.xlsx
+++ b/src/main/resources/modules/SMOKE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ehsan\AMTPublicRipo\AMT-TestFrameWork\src\main\resources\modules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6F32869-8B2B-4FA1-BAF0-D4A6D9247AEB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EBE2E98-E292-478C-9B37-6F50F231428B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="330" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="717" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="717" uniqueCount="165">
   <si>
     <t>Action</t>
   </si>
@@ -519,16 +519,10 @@
     <t>$RecurringPayment_effDate_0</t>
   </si>
   <si>
-    <t>111</t>
-  </si>
-  <si>
-    <t>112</t>
-  </si>
-  <si>
-    <t>113</t>
-  </si>
-  <si>
-    <t>Test unique</t>
+    <t>1000</t>
+  </si>
+  <si>
+    <t>Test$Unq</t>
   </si>
 </sst>
 </file>
@@ -713,7 +707,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -888,220 +882,184 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Accent1" xfId="2" builtinId="29"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="179">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
+  <dxfs count="173">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4524,340 +4482,340 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H2:H16 H20 H30">
-    <cfRule type="cellIs" dxfId="178" priority="108" operator="equal">
+    <cfRule type="cellIs" dxfId="172" priority="108" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H16 H20 H30">
-    <cfRule type="cellIs" dxfId="177" priority="106" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="176" priority="107" operator="equal">
+    <cfRule type="cellIs" dxfId="171" priority="106" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="170" priority="107" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H17">
-    <cfRule type="cellIs" dxfId="175" priority="104" operator="equal">
+    <cfRule type="cellIs" dxfId="169" priority="104" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H17">
-    <cfRule type="cellIs" dxfId="174" priority="102" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="173" priority="103" operator="equal">
+    <cfRule type="cellIs" dxfId="168" priority="102" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="167" priority="103" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H18">
-    <cfRule type="cellIs" dxfId="172" priority="100" operator="equal">
+    <cfRule type="cellIs" dxfId="166" priority="100" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H18">
-    <cfRule type="cellIs" dxfId="171" priority="98" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="170" priority="99" operator="equal">
+    <cfRule type="cellIs" dxfId="165" priority="98" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="164" priority="99" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H21">
-    <cfRule type="cellIs" dxfId="169" priority="96" operator="equal">
+    <cfRule type="cellIs" dxfId="163" priority="96" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H21">
-    <cfRule type="cellIs" dxfId="168" priority="94" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="167" priority="95" operator="equal">
+    <cfRule type="cellIs" dxfId="162" priority="94" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="161" priority="95" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H28">
-    <cfRule type="cellIs" dxfId="166" priority="88" operator="equal">
+    <cfRule type="cellIs" dxfId="160" priority="88" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H28">
-    <cfRule type="cellIs" dxfId="165" priority="86" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="164" priority="87" operator="equal">
+    <cfRule type="cellIs" dxfId="159" priority="86" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="158" priority="87" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H29">
-    <cfRule type="cellIs" dxfId="163" priority="84" operator="equal">
+    <cfRule type="cellIs" dxfId="157" priority="84" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H29">
-    <cfRule type="cellIs" dxfId="162" priority="82" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="161" priority="83" operator="equal">
+    <cfRule type="cellIs" dxfId="156" priority="82" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="155" priority="83" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H19">
-    <cfRule type="cellIs" dxfId="160" priority="80" operator="equal">
+    <cfRule type="cellIs" dxfId="154" priority="80" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H19">
-    <cfRule type="cellIs" dxfId="159" priority="78" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="158" priority="79" operator="equal">
+    <cfRule type="cellIs" dxfId="153" priority="78" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="152" priority="79" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H26">
-    <cfRule type="cellIs" dxfId="157" priority="76" operator="equal">
+    <cfRule type="cellIs" dxfId="151" priority="76" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H26">
-    <cfRule type="cellIs" dxfId="156" priority="74" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="155" priority="75" operator="equal">
+    <cfRule type="cellIs" dxfId="150" priority="74" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="149" priority="75" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H27">
-    <cfRule type="cellIs" dxfId="154" priority="72" operator="equal">
+    <cfRule type="cellIs" dxfId="148" priority="72" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H27">
-    <cfRule type="cellIs" dxfId="153" priority="70" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="152" priority="71" operator="equal">
+    <cfRule type="cellIs" dxfId="147" priority="70" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="146" priority="71" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H22">
-    <cfRule type="cellIs" dxfId="151" priority="68" operator="equal">
+    <cfRule type="cellIs" dxfId="145" priority="68" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H22">
-    <cfRule type="cellIs" dxfId="150" priority="66" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="149" priority="67" operator="equal">
+    <cfRule type="cellIs" dxfId="144" priority="66" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="143" priority="67" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H23">
-    <cfRule type="cellIs" dxfId="148" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="142" priority="64" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H23">
-    <cfRule type="cellIs" dxfId="147" priority="62" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="146" priority="63" operator="equal">
+    <cfRule type="cellIs" dxfId="141" priority="62" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="140" priority="63" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H24">
-    <cfRule type="cellIs" dxfId="145" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="139" priority="60" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H24">
-    <cfRule type="cellIs" dxfId="144" priority="58" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="143" priority="59" operator="equal">
+    <cfRule type="cellIs" dxfId="138" priority="58" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="137" priority="59" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H25">
-    <cfRule type="cellIs" dxfId="142" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="136" priority="56" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H25">
-    <cfRule type="cellIs" dxfId="141" priority="54" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="140" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="135" priority="54" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="134" priority="55" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H32:H46 H50 H60">
-    <cfRule type="cellIs" dxfId="139" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="133" priority="52" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H32:H46 H50 H60">
-    <cfRule type="cellIs" dxfId="138" priority="50" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="137" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="132" priority="50" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="131" priority="51" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H47">
-    <cfRule type="cellIs" dxfId="136" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="130" priority="48" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H47">
-    <cfRule type="cellIs" dxfId="135" priority="46" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="134" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="129" priority="46" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="128" priority="47" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H48">
-    <cfRule type="cellIs" dxfId="133" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="127" priority="44" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H48">
-    <cfRule type="cellIs" dxfId="132" priority="42" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="131" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="126" priority="42" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="125" priority="43" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H51">
-    <cfRule type="cellIs" dxfId="130" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="124" priority="40" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H51">
-    <cfRule type="cellIs" dxfId="129" priority="38" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="128" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="123" priority="38" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="122" priority="39" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H58">
-    <cfRule type="cellIs" dxfId="127" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="121" priority="36" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H58">
-    <cfRule type="cellIs" dxfId="126" priority="34" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="125" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="120" priority="34" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="119" priority="35" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H59">
-    <cfRule type="cellIs" dxfId="124" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="118" priority="32" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H59">
-    <cfRule type="cellIs" dxfId="123" priority="30" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="122" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="117" priority="30" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="116" priority="31" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H49">
-    <cfRule type="cellIs" dxfId="121" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="115" priority="28" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H49">
-    <cfRule type="cellIs" dxfId="120" priority="26" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="119" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="114" priority="26" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="113" priority="27" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H56">
-    <cfRule type="cellIs" dxfId="118" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="112" priority="24" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H56">
-    <cfRule type="cellIs" dxfId="117" priority="22" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="116" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="111" priority="22" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="110" priority="23" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H57">
-    <cfRule type="cellIs" dxfId="115" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="109" priority="20" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H57">
-    <cfRule type="cellIs" dxfId="114" priority="18" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="113" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="108" priority="18" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="107" priority="19" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H52">
-    <cfRule type="cellIs" dxfId="112" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="106" priority="16" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H52">
-    <cfRule type="cellIs" dxfId="111" priority="14" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="110" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="105" priority="14" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="104" priority="15" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H53">
-    <cfRule type="cellIs" dxfId="109" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="103" priority="12" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H53">
-    <cfRule type="cellIs" dxfId="108" priority="10" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="107" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="102" priority="10" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="101" priority="11" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H54">
-    <cfRule type="cellIs" dxfId="106" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="100" priority="8" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H54">
-    <cfRule type="cellIs" dxfId="105" priority="6" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="104" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="99" priority="6" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="98" priority="7" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H55">
-    <cfRule type="cellIs" dxfId="103" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="97" priority="4" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H55">
-    <cfRule type="cellIs" dxfId="102" priority="2" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="101" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="2" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="95" priority="3" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5232,8 +5190,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CE87BF7-3C91-45AC-BD7A-97ED35B7B19B}">
   <dimension ref="A1:L65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D7" workbookViewId="0">
-      <selection activeCell="H38" sqref="H38"/>
+    <sheetView tabSelected="1" topLeftCell="D4" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5248,7 +5206,8 @@
     <col min="9" max="9" width="16.140625" style="33" customWidth="1"/>
     <col min="10" max="10" width="17.7109375" style="33" customWidth="1"/>
     <col min="11" max="11" width="50.42578125" style="36" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="36"/>
+    <col min="12" max="12" width="9.140625" style="33"/>
+    <col min="13" max="16384" width="9.140625" style="36"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="33" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -5292,18 +5251,18 @@
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="34"/>
       <c r="B2" s="35"/>
-      <c r="C2" s="56" t="s">
+      <c r="C2" s="64" t="s">
         <v>114</v>
       </c>
-      <c r="D2" s="56"/>
-      <c r="E2" s="56"/>
-      <c r="F2" s="56"/>
-      <c r="G2" s="56"/>
-      <c r="H2" s="56"/>
-      <c r="I2" s="56"/>
-      <c r="J2" s="56"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="64"/>
+      <c r="I2" s="64"/>
+      <c r="J2" s="64"/>
       <c r="K2" s="35"/>
-      <c r="L2" s="35"/>
+      <c r="L2" s="56"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
@@ -5331,7 +5290,6 @@
       </c>
       <c r="J3" s="17"/>
       <c r="K3" s="33"/>
-      <c r="L3" s="33"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
@@ -5416,7 +5374,7 @@
       <c r="J6" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="L6" s="36">
+      <c r="L6" s="33">
         <v>0</v>
       </c>
     </row>
@@ -5449,7 +5407,7 @@
       <c r="J7" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="L7" s="36">
+      <c r="L7" s="33">
         <v>2</v>
       </c>
     </row>
@@ -5483,7 +5441,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>102</v>
       </c>
@@ -5566,7 +5524,7 @@
       <c r="J11" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="L11" s="36">
+      <c r="L11" s="33">
         <v>0</v>
       </c>
     </row>
@@ -5595,7 +5553,7 @@
       <c r="J12" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="L12" s="36">
+      <c r="L12" s="33">
         <v>1</v>
       </c>
     </row>
@@ -5626,7 +5584,7 @@
       <c r="J13" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="L13" s="36">
+      <c r="L13" s="33">
         <v>1</v>
       </c>
     </row>
@@ -5655,7 +5613,7 @@
       <c r="J14" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="L14" s="36">
+      <c r="L14" s="33">
         <v>1</v>
       </c>
     </row>
@@ -5686,7 +5644,7 @@
       <c r="J15" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="L15" s="36">
+      <c r="L15" s="33">
         <v>1</v>
       </c>
     </row>
@@ -5717,7 +5675,7 @@
       <c r="J16" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="L16" s="36">
+      <c r="L16" s="33">
         <v>1</v>
       </c>
     </row>
@@ -5748,7 +5706,7 @@
       <c r="J17" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="L17" s="36">
+      <c r="L17" s="33">
         <v>2</v>
       </c>
     </row>
@@ -5814,7 +5772,7 @@
       <c r="K19" s="36" t="s">
         <v>146</v>
       </c>
-      <c r="L19" s="36">
+      <c r="L19" s="33">
         <v>1</v>
       </c>
     </row>
@@ -5843,23 +5801,23 @@
       <c r="J20" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="L20" s="36">
+      <c r="L20" s="33">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="47"/>
       <c r="B21" s="48"/>
-      <c r="C21" s="57"/>
-      <c r="D21" s="57"/>
-      <c r="E21" s="57"/>
-      <c r="F21" s="57"/>
+      <c r="C21" s="65"/>
+      <c r="D21" s="65"/>
+      <c r="E21" s="65"/>
+      <c r="F21" s="65"/>
       <c r="G21" s="49"/>
       <c r="H21" s="16"/>
       <c r="I21" s="17"/>
       <c r="J21" s="49"/>
       <c r="K21" s="50"/>
-      <c r="L21" s="50"/>
+      <c r="L21" s="57"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
@@ -5913,7 +5871,7 @@
       <c r="J23" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="L23" s="36">
+      <c r="L23" s="33">
         <v>0</v>
       </c>
     </row>
@@ -5969,7 +5927,7 @@
       <c r="J25" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="L25" s="36">
+      <c r="L25" s="33">
         <v>0</v>
       </c>
     </row>
@@ -6048,7 +6006,7 @@
         <v>145</v>
       </c>
       <c r="G28" s="55" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="H28" s="16"/>
       <c r="I28" s="1" t="s">
@@ -6057,7 +6015,7 @@
       <c r="J28" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="L28" s="36">
+      <c r="L28" s="33">
         <v>1</v>
       </c>
     </row>
@@ -6088,7 +6046,7 @@
       <c r="J29" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="L29" s="36">
+      <c r="L29" s="33">
         <v>1</v>
       </c>
     </row>
@@ -6110,7 +6068,7 @@
         <v>121</v>
       </c>
       <c r="G30" s="55" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H30" s="16"/>
       <c r="I30" s="1" t="s">
@@ -6119,7 +6077,7 @@
       <c r="J30" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="L30" s="36">
+      <c r="L30" s="33">
         <v>1</v>
       </c>
     </row>
@@ -6141,7 +6099,7 @@
         <v>122</v>
       </c>
       <c r="G31" s="55" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="H31" s="16"/>
       <c r="I31" s="1" t="s">
@@ -6150,7 +6108,7 @@
       <c r="J31" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="L31" s="36">
+      <c r="L31" s="33">
         <v>1</v>
       </c>
     </row>
@@ -6179,7 +6137,7 @@
       <c r="J32" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="L32" s="36">
+      <c r="L32" s="33">
         <v>0</v>
       </c>
     </row>
@@ -6227,7 +6185,7 @@
       <c r="J34" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="L34" s="36">
+      <c r="L34" s="33">
         <v>1</v>
       </c>
     </row>
@@ -6263,7 +6221,7 @@
       <c r="K35" t="s">
         <v>153</v>
       </c>
-      <c r="L35">
+      <c r="L35" s="3">
         <v>1</v>
       </c>
     </row>
@@ -6660,184 +6618,184 @@
     <mergeCell ref="C21:F21"/>
   </mergeCells>
   <conditionalFormatting sqref="H37:H51 H55 H65">
-    <cfRule type="cellIs" dxfId="70" priority="75" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="75" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H37:H51 H55 H65">
-    <cfRule type="cellIs" dxfId="69" priority="73" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="74" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="73" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="65" priority="74" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H52">
-    <cfRule type="cellIs" dxfId="67" priority="71" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="71" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H52">
-    <cfRule type="cellIs" dxfId="66" priority="69" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="65" priority="70" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="69" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="62" priority="70" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H53">
-    <cfRule type="cellIs" dxfId="64" priority="67" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="67" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H53">
-    <cfRule type="cellIs" dxfId="63" priority="65" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="66" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="65" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="59" priority="66" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H56">
-    <cfRule type="cellIs" dxfId="61" priority="63" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="63" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H56">
-    <cfRule type="cellIs" dxfId="60" priority="61" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="59" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="61" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="56" priority="62" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H63">
-    <cfRule type="cellIs" dxfId="58" priority="59" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="59" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H63">
-    <cfRule type="cellIs" dxfId="57" priority="57" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="58" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="57" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="53" priority="58" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H64">
-    <cfRule type="cellIs" dxfId="55" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="55" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H64">
-    <cfRule type="cellIs" dxfId="54" priority="53" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="53" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="50" priority="54" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H54">
-    <cfRule type="cellIs" dxfId="52" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="51" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H54">
-    <cfRule type="cellIs" dxfId="51" priority="49" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="49" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="47" priority="50" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H61">
-    <cfRule type="cellIs" dxfId="49" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="47" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H61">
-    <cfRule type="cellIs" dxfId="48" priority="45" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="45" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="44" priority="46" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H62">
-    <cfRule type="cellIs" dxfId="46" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="43" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H62">
-    <cfRule type="cellIs" dxfId="45" priority="41" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="41" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="41" priority="42" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H57">
-    <cfRule type="cellIs" dxfId="43" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="39" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H57">
-    <cfRule type="cellIs" dxfId="42" priority="37" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="37" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="38" priority="38" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H58">
-    <cfRule type="cellIs" dxfId="40" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="35" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H58">
-    <cfRule type="cellIs" dxfId="39" priority="33" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="33" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="35" priority="34" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H59">
-    <cfRule type="cellIs" dxfId="37" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="31" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H59">
-    <cfRule type="cellIs" dxfId="36" priority="29" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="29" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="32" priority="30" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H60">
-    <cfRule type="cellIs" dxfId="34" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="27" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H60">
-    <cfRule type="cellIs" dxfId="33" priority="25" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="25" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="29" priority="26" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10:H18">
-    <cfRule type="cellIs" dxfId="31" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="22" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10:H18">
-    <cfRule type="cellIs" dxfId="30" priority="20" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="20" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="26" priority="21" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Update smoke and commonTc for lease classification verity
</commit_message>
<xml_diff>
--- a/src/main/resources/modules/SMOKE.xlsx
+++ b/src/main/resources/modules/SMOKE.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DSi\Desktop\selemnium1\seleniumTestingFramework\src\main\resources\modules\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ehsan\AMTPublicRipo\AMT-TestFrameWork\src\main\resources\modules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0651E7A0-FD71-4F41-94C3-EF338B080182}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9FBD0D0-26C6-4348-BE7E-FC9F1BE440D1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="4575" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Controller" sheetId="19" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1010" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1052" uniqueCount="132">
   <si>
     <t>Action</t>
   </si>
@@ -669,7 +669,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="107">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -903,9 +903,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -929,9 +926,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -955,6 +949,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -4042,7 +4039,7 @@
   <dimension ref="A1:S39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="J38" sqref="J38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4105,6 +4102,9 @@
       <c r="E3" s="5" t="s">
         <v>97</v>
       </c>
+      <c r="F3" s="5" t="s">
+        <v>97</v>
+      </c>
       <c r="S3" s="2" t="s">
         <v>2</v>
       </c>
@@ -4123,6 +4123,9 @@
         <v>11</v>
       </c>
       <c r="E4" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>97</v>
       </c>
     </row>
@@ -4142,6 +4145,9 @@
       <c r="E5" s="5" t="s">
         <v>102</v>
       </c>
+      <c r="F5" s="5" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
@@ -4154,9 +4160,12 @@
         <v>104</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="E6" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="F6" s="5" t="s">
         <v>102</v>
       </c>
     </row>
@@ -4171,9 +4180,12 @@
         <v>111</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="E7" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="F7" s="5" t="s">
         <v>102</v>
       </c>
     </row>
@@ -4188,9 +4200,12 @@
         <v>119</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="E8" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="F8" s="5" t="s">
         <v>102</v>
       </c>
     </row>
@@ -4205,9 +4220,12 @@
         <v>31</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="E9" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" s="5" t="s">
         <v>32</v>
       </c>
     </row>
@@ -4222,9 +4240,12 @@
         <v>38</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="E10" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" s="5" t="s">
         <v>32</v>
       </c>
     </row>
@@ -4239,9 +4260,12 @@
         <v>39</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="E11" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" s="5" t="s">
         <v>32</v>
       </c>
     </row>
@@ -4255,10 +4279,13 @@
       <c r="C12" t="s">
         <v>40</v>
       </c>
-      <c r="D12" s="50" t="s">
-        <v>11</v>
+      <c r="D12" s="5" t="s">
+        <v>2</v>
       </c>
       <c r="E12" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" s="5" t="s">
         <v>32</v>
       </c>
     </row>
@@ -4272,7 +4299,7 @@
       <c r="E15" s="46"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A16" s="87">
+      <c r="A16" s="5">
         <v>1</v>
       </c>
       <c r="B16" s="59">
@@ -4281,12 +4308,18 @@
       <c r="C16" t="s">
         <v>96</v>
       </c>
+      <c r="D16" s="50" t="s">
+        <v>44</v>
+      </c>
       <c r="E16" s="5" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="87">
+      <c r="F16" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="5">
         <v>2</v>
       </c>
       <c r="B17" s="59">
@@ -4295,58 +4328,99 @@
       <c r="C17" t="s">
         <v>98</v>
       </c>
+      <c r="D17" s="50" t="s">
+        <v>44</v>
+      </c>
       <c r="E17" s="5" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="87"/>
+      <c r="F17" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="5">
+        <v>3</v>
+      </c>
       <c r="B18" s="59">
         <v>6530927</v>
       </c>
       <c r="C18" t="s">
         <v>107</v>
       </c>
+      <c r="D18" s="50" t="s">
+        <v>44</v>
+      </c>
       <c r="E18" s="5" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F18" s="5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="5">
+        <v>4</v>
+      </c>
       <c r="B19" s="3">
         <v>6530966</v>
       </c>
       <c r="C19" t="s">
         <v>108</v>
       </c>
+      <c r="D19" s="50" t="s">
+        <v>44</v>
+      </c>
       <c r="E19" s="5" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F19" s="5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="5">
+        <v>5</v>
+      </c>
       <c r="B20" s="3">
         <v>6530960</v>
       </c>
       <c r="C20" t="s">
         <v>130</v>
       </c>
+      <c r="D20" s="50" t="s">
+        <v>44</v>
+      </c>
       <c r="E20" s="5" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F20" s="5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="5">
+        <v>6</v>
+      </c>
       <c r="B21" s="3">
         <v>6530959</v>
       </c>
       <c r="C21" t="s">
         <v>131</v>
       </c>
+      <c r="D21" s="50" t="s">
+        <v>44</v>
+      </c>
       <c r="E21" s="5" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F21" s="5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B22" s="51" t="s">
         <v>42</v>
@@ -4360,10 +4434,13 @@
       <c r="E22" s="5" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F22" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B23" s="49">
         <v>6558241</v>
@@ -4377,10 +4454,13 @@
       <c r="E23" s="5" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F23" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B24" s="49">
         <v>6558243</v>
@@ -4394,10 +4474,13 @@
       <c r="E24" s="5" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F24" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B25" s="49">
         <v>6558245</v>
@@ -4411,8 +4494,11 @@
       <c r="E25" s="5" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F25" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="44"/>
       <c r="B29" s="45"/>
       <c r="C29" s="44" t="s">
@@ -4421,8 +4507,8 @@
       <c r="D29" s="44"/>
       <c r="E29" s="46"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="87">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="5">
         <v>1</v>
       </c>
       <c r="B30" s="59">
@@ -4431,12 +4517,18 @@
       <c r="C30" t="s">
         <v>99</v>
       </c>
+      <c r="D30" s="50" t="s">
+        <v>11</v>
+      </c>
       <c r="E30" s="5" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="87">
+      <c r="F30" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="5">
         <v>2</v>
       </c>
       <c r="B31" s="59">
@@ -4445,12 +4537,18 @@
       <c r="C31" t="s">
         <v>100</v>
       </c>
+      <c r="D31" s="50" t="s">
+        <v>11</v>
+      </c>
       <c r="E31" s="5" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" s="86" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="87">
+      <c r="F31" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" s="85" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="5">
         <v>3</v>
       </c>
       <c r="B32" s="13" t="s">
@@ -4459,55 +4557,79 @@
       <c r="C32" t="s">
         <v>95</v>
       </c>
-      <c r="D32" s="85"/>
+      <c r="D32" s="50" t="s">
+        <v>11</v>
+      </c>
       <c r="E32" s="5" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" s="86" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="87">
+      <c r="F32" s="5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" s="85" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="5">
         <v>4</v>
       </c>
-      <c r="B33" s="88" t="s">
+      <c r="B33" s="87" t="s">
         <v>106</v>
       </c>
       <c r="C33" t="s">
         <v>105</v>
       </c>
-      <c r="D33" s="85"/>
+      <c r="D33" s="50" t="s">
+        <v>11</v>
+      </c>
       <c r="E33" s="5" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" s="86" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="87"/>
-      <c r="B34" s="88" t="s">
+      <c r="F33" s="5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" s="85" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="5">
+        <v>5</v>
+      </c>
+      <c r="B34" s="87" t="s">
         <v>128</v>
       </c>
       <c r="C34" t="s">
         <v>126</v>
       </c>
-      <c r="D34" s="85"/>
+      <c r="D34" s="50" t="s">
+        <v>11</v>
+      </c>
       <c r="E34" s="5" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" s="86" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="87"/>
-      <c r="B35" s="88" t="s">
+      <c r="F34" s="5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" s="85" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="5">
+        <v>6</v>
+      </c>
+      <c r="B35" s="87" t="s">
         <v>129</v>
       </c>
       <c r="C35" t="s">
         <v>127</v>
       </c>
-      <c r="D35" s="85"/>
+      <c r="D35" s="50" t="s">
+        <v>11</v>
+      </c>
       <c r="E35" s="5" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="87">
-        <v>5</v>
+      <c r="F35" s="5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="5">
+        <v>7</v>
       </c>
       <c r="B36" s="49">
         <v>6541329</v>
@@ -4521,10 +4643,13 @@
       <c r="E36" s="5" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="87">
-        <v>6</v>
+      <c r="F36" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="5">
+        <v>8</v>
       </c>
       <c r="B37" s="49">
         <v>6558247</v>
@@ -4538,10 +4663,13 @@
       <c r="E37" s="5" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="87">
-        <v>7</v>
+      <c r="F37" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="5">
+        <v>9</v>
       </c>
       <c r="B38" s="49">
         <v>6558248</v>
@@ -4555,10 +4683,13 @@
       <c r="E38" s="5" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="87">
-        <v>8</v>
+      <c r="F38" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="86">
+        <v>10</v>
       </c>
       <c r="B39" s="3">
         <v>6558250</v>
@@ -4570,6 +4701,9 @@
         <v>11</v>
       </c>
       <c r="E39" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F39" s="5" t="s">
         <v>32</v>
       </c>
     </row>
@@ -4583,8 +4717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3BEFDB9-89D3-4BD7-BCAC-3A5ECC5CDE8F}">
   <dimension ref="A1:L115"/>
   <sheetViews>
-    <sheetView topLeftCell="G27" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G110" sqref="G110"/>
+    <sheetView topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4640,12 +4774,12 @@
     </row>
     <row r="2" spans="1:12" s="80" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="82"/>
-      <c r="B2" s="97" t="s">
+      <c r="B2" s="95" t="s">
         <v>94</v>
       </c>
-      <c r="C2" s="98"/>
-      <c r="D2" s="98"/>
-      <c r="E2" s="99"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="96"/>
+      <c r="E2" s="97"/>
       <c r="F2" s="84"/>
       <c r="G2" s="83"/>
       <c r="H2" s="82"/>
@@ -4709,13 +4843,13 @@
       <c r="D5" s="70" t="s">
         <v>115</v>
       </c>
-      <c r="E5" s="91" t="s">
+      <c r="E5" s="90" t="s">
         <v>120</v>
       </c>
       <c r="F5" s="69" t="s">
         <v>121</v>
       </c>
-      <c r="G5" s="91" t="s">
+      <c r="G5" s="90" t="s">
         <v>116</v>
       </c>
       <c r="I5" s="60" t="s">
@@ -4774,12 +4908,12 @@
     </row>
     <row r="8" spans="1:12" s="67" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="74"/>
-      <c r="B8" s="100" t="s">
+      <c r="B8" s="98" t="s">
         <v>92</v>
       </c>
-      <c r="C8" s="100"/>
-      <c r="D8" s="100"/>
-      <c r="E8" s="100"/>
+      <c r="C8" s="98"/>
+      <c r="D8" s="98"/>
+      <c r="E8" s="98"/>
       <c r="H8" s="68"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -4955,13 +5089,13 @@
       <c r="D15" s="70" t="s">
         <v>115</v>
       </c>
-      <c r="E15" s="91" t="s">
+      <c r="E15" s="90" t="s">
         <v>120</v>
       </c>
       <c r="F15" s="69" t="s">
         <v>121</v>
       </c>
-      <c r="G15" s="91" t="s">
+      <c r="G15" s="90" t="s">
         <v>116</v>
       </c>
       <c r="I15" s="60" t="s">
@@ -5020,12 +5154,12 @@
     </row>
     <row r="18" spans="1:12" s="67" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="74"/>
-      <c r="B18" s="101" t="s">
+      <c r="B18" s="99" t="s">
         <v>91</v>
       </c>
-      <c r="C18" s="96"/>
-      <c r="D18" s="96"/>
-      <c r="E18" s="96"/>
+      <c r="C18" s="94"/>
+      <c r="D18" s="94"/>
+      <c r="E18" s="94"/>
       <c r="H18" s="68"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -5085,13 +5219,13 @@
       <c r="D21" s="70" t="s">
         <v>115</v>
       </c>
-      <c r="E21" s="91" t="s">
+      <c r="E21" s="90" t="s">
         <v>120</v>
       </c>
       <c r="F21" s="69" t="s">
         <v>121</v>
       </c>
-      <c r="G21" s="91" t="s">
+      <c r="G21" s="90" t="s">
         <v>116</v>
       </c>
       <c r="I21" s="60" t="s">
@@ -5150,12 +5284,12 @@
     </row>
     <row r="24" spans="1:12" s="67" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="79"/>
-      <c r="B24" s="102" t="s">
+      <c r="B24" s="100" t="s">
         <v>89</v>
       </c>
-      <c r="C24" s="103"/>
-      <c r="D24" s="103"/>
-      <c r="E24" s="103"/>
+      <c r="C24" s="101"/>
+      <c r="D24" s="101"/>
+      <c r="E24" s="101"/>
       <c r="F24" s="78"/>
       <c r="G24" s="77"/>
       <c r="H24" s="76"/>
@@ -5335,13 +5469,13 @@
       <c r="D31" s="70" t="s">
         <v>115</v>
       </c>
-      <c r="E31" s="91" t="s">
+      <c r="E31" s="90" t="s">
         <v>120</v>
       </c>
       <c r="F31" s="69" t="s">
         <v>121</v>
       </c>
-      <c r="G31" s="91" t="s">
+      <c r="G31" s="90" t="s">
         <v>116</v>
       </c>
       <c r="I31" s="60" t="s">
@@ -5400,12 +5534,12 @@
     </row>
     <row r="34" spans="1:12" s="67" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="74"/>
-      <c r="B34" s="96" t="s">
+      <c r="B34" s="94" t="s">
         <v>88</v>
       </c>
-      <c r="C34" s="96"/>
-      <c r="D34" s="96"/>
-      <c r="E34" s="96"/>
+      <c r="C34" s="94"/>
+      <c r="D34" s="94"/>
+      <c r="E34" s="94"/>
       <c r="H34" s="68"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
@@ -5465,13 +5599,13 @@
       <c r="D37" s="70" t="s">
         <v>115</v>
       </c>
-      <c r="E37" s="91" t="s">
+      <c r="E37" s="90" t="s">
         <v>120</v>
       </c>
       <c r="F37" s="69" t="s">
         <v>121</v>
       </c>
-      <c r="G37" s="91" t="s">
+      <c r="G37" s="90" t="s">
         <v>116</v>
       </c>
       <c r="I37" s="60" t="s">
@@ -5530,12 +5664,12 @@
     </row>
     <row r="40" spans="1:12" s="67" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="74"/>
-      <c r="B40" s="96" t="s">
+      <c r="B40" s="94" t="s">
         <v>85</v>
       </c>
-      <c r="C40" s="96"/>
-      <c r="D40" s="96"/>
-      <c r="E40" s="96"/>
+      <c r="C40" s="94"/>
+      <c r="D40" s="94"/>
+      <c r="E40" s="94"/>
       <c r="H40" s="68"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
@@ -5711,13 +5845,13 @@
       <c r="D47" s="70" t="s">
         <v>115</v>
       </c>
-      <c r="E47" s="91" t="s">
+      <c r="E47" s="90" t="s">
         <v>120</v>
       </c>
       <c r="F47" s="69" t="s">
         <v>121</v>
       </c>
-      <c r="G47" s="91" t="s">
+      <c r="G47" s="90" t="s">
         <v>116</v>
       </c>
       <c r="I47" s="60" t="s">
@@ -5775,13 +5909,13 @@
       </c>
     </row>
     <row r="50" spans="1:12" s="67" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="89"/>
-      <c r="B50" s="96" t="s">
+      <c r="A50" s="88"/>
+      <c r="B50" s="94" t="s">
         <v>109</v>
       </c>
-      <c r="C50" s="96"/>
-      <c r="D50" s="96"/>
-      <c r="E50" s="96"/>
+      <c r="C50" s="94"/>
+      <c r="D50" s="94"/>
+      <c r="E50" s="94"/>
       <c r="H50" s="68"/>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
@@ -5989,7 +6123,7 @@
       <c r="D58" s="70" t="s">
         <v>115</v>
       </c>
-      <c r="E58" s="91" t="s">
+      <c r="E58" s="90" t="s">
         <v>120</v>
       </c>
       <c r="F58" s="69" t="s">
@@ -6057,13 +6191,13 @@
       </c>
     </row>
     <row r="61" spans="1:12" s="67" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="90"/>
-      <c r="B61" s="96" t="s">
+      <c r="A61" s="89"/>
+      <c r="B61" s="94" t="s">
         <v>112</v>
       </c>
-      <c r="C61" s="96"/>
-      <c r="D61" s="96"/>
-      <c r="E61" s="96"/>
+      <c r="C61" s="94"/>
+      <c r="D61" s="94"/>
+      <c r="E61" s="94"/>
       <c r="H61" s="68"/>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.25">
@@ -6271,7 +6405,7 @@
       <c r="D69" s="70" t="s">
         <v>115</v>
       </c>
-      <c r="E69" s="91" t="s">
+      <c r="E69" s="90" t="s">
         <v>120</v>
       </c>
       <c r="F69" s="69" t="s">
@@ -6338,14 +6472,14 @@
         <v>11</v>
       </c>
     </row>
-    <row r="72" spans="1:12" s="93" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="92"/>
-      <c r="B72" s="95" t="s">
+    <row r="72" spans="1:12" s="92" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="91"/>
+      <c r="B72" s="102" t="s">
         <v>122</v>
       </c>
-      <c r="C72" s="95"/>
-      <c r="D72" s="95"/>
-      <c r="H72" s="94"/>
+      <c r="C72" s="102"/>
+      <c r="D72" s="102"/>
+      <c r="H72" s="93"/>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73" s="3">
@@ -6552,7 +6686,7 @@
       <c r="D80" s="70" t="s">
         <v>115</v>
       </c>
-      <c r="E80" s="91" t="s">
+      <c r="E80" s="90" t="s">
         <v>120</v>
       </c>
       <c r="F80" s="69" t="s">
@@ -6619,14 +6753,14 @@
         <v>11</v>
       </c>
     </row>
-    <row r="83" spans="1:12" s="93" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="92"/>
-      <c r="B83" s="95" t="s">
+    <row r="83" spans="1:12" s="92" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="91"/>
+      <c r="B83" s="102" t="s">
         <v>123</v>
       </c>
-      <c r="C83" s="95"/>
-      <c r="D83" s="95"/>
-      <c r="H83" s="94"/>
+      <c r="C83" s="102"/>
+      <c r="D83" s="102"/>
+      <c r="H83" s="93"/>
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A84" s="3">
@@ -6833,7 +6967,7 @@
       <c r="D91" s="70" t="s">
         <v>115</v>
       </c>
-      <c r="E91" s="91" t="s">
+      <c r="E91" s="90" t="s">
         <v>120</v>
       </c>
       <c r="F91" s="69" t="s">
@@ -6900,14 +7034,14 @@
         <v>11</v>
       </c>
     </row>
-    <row r="94" spans="1:12" s="93" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="92"/>
-      <c r="B94" s="95" t="s">
+    <row r="94" spans="1:12" s="92" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="91"/>
+      <c r="B94" s="102" t="s">
         <v>124</v>
       </c>
-      <c r="C94" s="95"/>
-      <c r="D94" s="95"/>
-      <c r="H94" s="94"/>
+      <c r="C94" s="102"/>
+      <c r="D94" s="102"/>
+      <c r="H94" s="93"/>
     </row>
     <row r="95" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A95" s="3">
@@ -7114,7 +7248,7 @@
       <c r="D102" s="70" t="s">
         <v>115</v>
       </c>
-      <c r="E102" s="91" t="s">
+      <c r="E102" s="90" t="s">
         <v>120</v>
       </c>
       <c r="F102" s="69" t="s">
@@ -7181,14 +7315,14 @@
         <v>11</v>
       </c>
     </row>
-    <row r="105" spans="1:12" s="93" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="92"/>
-      <c r="B105" s="95" t="s">
+    <row r="105" spans="1:12" s="92" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="91"/>
+      <c r="B105" s="102" t="s">
         <v>125</v>
       </c>
-      <c r="C105" s="95"/>
-      <c r="D105" s="95"/>
-      <c r="H105" s="94"/>
+      <c r="C105" s="102"/>
+      <c r="D105" s="102"/>
+      <c r="H105" s="93"/>
     </row>
     <row r="106" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A106" s="3">
@@ -7395,7 +7529,7 @@
       <c r="D113" s="70" t="s">
         <v>115</v>
       </c>
-      <c r="E113" s="91" t="s">
+      <c r="E113" s="90" t="s">
         <v>120</v>
       </c>
       <c r="F113" s="69" t="s">
@@ -7464,6 +7598,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B72:D72"/>
+    <mergeCell ref="B83:D83"/>
+    <mergeCell ref="B94:D94"/>
+    <mergeCell ref="B105:D105"/>
+    <mergeCell ref="B61:E61"/>
     <mergeCell ref="B50:E50"/>
     <mergeCell ref="B40:E40"/>
     <mergeCell ref="B2:E2"/>
@@ -7471,11 +7610,6 @@
     <mergeCell ref="B18:E18"/>
     <mergeCell ref="B34:E34"/>
     <mergeCell ref="B24:E24"/>
-    <mergeCell ref="B72:D72"/>
-    <mergeCell ref="B83:D83"/>
-    <mergeCell ref="B94:D94"/>
-    <mergeCell ref="B105:D105"/>
-    <mergeCell ref="B61:E61"/>
   </mergeCells>
   <conditionalFormatting sqref="H3">
     <cfRule type="cellIs" dxfId="384" priority="314" operator="equal">
@@ -9401,11 +9535,11 @@
   <sheetData>
     <row r="1" spans="1:12" s="63" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="65"/>
-      <c r="B1" s="104" t="s">
+      <c r="B1" s="103" t="s">
         <v>69</v>
       </c>
-      <c r="C1" s="104"/>
-      <c r="D1" s="104"/>
+      <c r="C1" s="103"/>
+      <c r="D1" s="103"/>
       <c r="H1" s="64"/>
     </row>
     <row r="2" spans="1:12" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -9496,11 +9630,11 @@
     </row>
     <row r="6" spans="1:12" s="67" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="65"/>
-      <c r="B6" s="105" t="s">
+      <c r="B6" s="104" t="s">
         <v>68</v>
       </c>
-      <c r="C6" s="105"/>
-      <c r="D6" s="105"/>
+      <c r="C6" s="104"/>
+      <c r="D6" s="104"/>
       <c r="H6" s="68"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -9559,11 +9693,11 @@
     </row>
     <row r="10" spans="1:12" s="63" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="65"/>
-      <c r="B10" s="104" t="s">
+      <c r="B10" s="103" t="s">
         <v>66</v>
       </c>
-      <c r="C10" s="104"/>
-      <c r="D10" s="104"/>
+      <c r="C10" s="103"/>
+      <c r="D10" s="103"/>
       <c r="H10" s="64"/>
     </row>
     <row r="11" spans="1:12" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -9654,11 +9788,11 @@
     </row>
     <row r="15" spans="1:12" s="63" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="65"/>
-      <c r="B15" s="104" t="s">
+      <c r="B15" s="103" t="s">
         <v>65</v>
       </c>
-      <c r="C15" s="104"/>
-      <c r="D15" s="104"/>
+      <c r="C15" s="103"/>
+      <c r="D15" s="103"/>
       <c r="H15" s="64"/>
     </row>
     <row r="16" spans="1:12" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -9749,11 +9883,11 @@
     </row>
     <row r="20" spans="1:12" s="63" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="65"/>
-      <c r="B20" s="104" t="s">
+      <c r="B20" s="103" t="s">
         <v>64</v>
       </c>
-      <c r="C20" s="104"/>
-      <c r="D20" s="104"/>
+      <c r="C20" s="103"/>
+      <c r="D20" s="103"/>
       <c r="H20" s="64"/>
     </row>
     <row r="21" spans="1:12" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -9844,11 +9978,11 @@
     </row>
     <row r="25" spans="1:12" s="63" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="65"/>
-      <c r="B25" s="104" t="s">
+      <c r="B25" s="103" t="s">
         <v>63</v>
       </c>
-      <c r="C25" s="104"/>
-      <c r="D25" s="104"/>
+      <c r="C25" s="103"/>
+      <c r="D25" s="103"/>
       <c r="H25" s="64"/>
     </row>
     <row r="26" spans="1:12" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -10619,8 +10753,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CE87BF7-3C91-45AC-BD7A-97ED35B7B19B}">
   <dimension ref="A1:L65"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C22" sqref="C22:J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10680,16 +10814,16 @@
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="31"/>
       <c r="B2" s="32"/>
-      <c r="C2" s="106" t="s">
+      <c r="C2" s="105" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="106"/>
-      <c r="E2" s="106"/>
-      <c r="F2" s="106"/>
-      <c r="G2" s="106"/>
-      <c r="H2" s="106"/>
-      <c r="I2" s="106"/>
-      <c r="J2" s="106"/>
+      <c r="D2" s="105"/>
+      <c r="E2" s="105"/>
+      <c r="F2" s="105"/>
+      <c r="G2" s="105"/>
+      <c r="H2" s="105"/>
+      <c r="I2" s="105"/>
+      <c r="J2" s="105"/>
       <c r="K2" s="32"/>
       <c r="L2" s="43"/>
     </row>
@@ -10789,16 +10923,16 @@
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="31"/>
       <c r="B7" s="32"/>
-      <c r="C7" s="106" t="s">
+      <c r="C7" s="105" t="s">
         <v>38</v>
       </c>
-      <c r="D7" s="106"/>
-      <c r="E7" s="106"/>
-      <c r="F7" s="106"/>
-      <c r="G7" s="106"/>
-      <c r="H7" s="106"/>
-      <c r="I7" s="106"/>
-      <c r="J7" s="106"/>
+      <c r="D7" s="105"/>
+      <c r="E7" s="105"/>
+      <c r="F7" s="105"/>
+      <c r="G7" s="105"/>
+      <c r="H7" s="105"/>
+      <c r="I7" s="105"/>
+      <c r="J7" s="105"/>
       <c r="K7" s="32"/>
       <c r="L7" s="43"/>
     </row>
@@ -10889,16 +11023,16 @@
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="31"/>
       <c r="B12" s="32"/>
-      <c r="C12" s="106" t="s">
+      <c r="C12" s="105" t="s">
         <v>39</v>
       </c>
-      <c r="D12" s="106"/>
-      <c r="E12" s="106"/>
-      <c r="F12" s="106"/>
-      <c r="G12" s="106"/>
-      <c r="H12" s="106"/>
-      <c r="I12" s="106"/>
-      <c r="J12" s="106"/>
+      <c r="D12" s="105"/>
+      <c r="E12" s="105"/>
+      <c r="F12" s="105"/>
+      <c r="G12" s="105"/>
+      <c r="H12" s="105"/>
+      <c r="I12" s="105"/>
+      <c r="J12" s="105"/>
       <c r="K12" s="32"/>
       <c r="L12" s="43"/>
     </row>
@@ -10989,16 +11123,16 @@
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="31"/>
       <c r="B17" s="32"/>
-      <c r="C17" s="106" t="s">
+      <c r="C17" s="105" t="s">
         <v>40</v>
       </c>
-      <c r="D17" s="106"/>
-      <c r="E17" s="106"/>
-      <c r="F17" s="106"/>
-      <c r="G17" s="106"/>
-      <c r="H17" s="106"/>
-      <c r="I17" s="106"/>
-      <c r="J17" s="106"/>
+      <c r="D17" s="105"/>
+      <c r="E17" s="105"/>
+      <c r="F17" s="105"/>
+      <c r="G17" s="105"/>
+      <c r="H17" s="105"/>
+      <c r="I17" s="105"/>
+      <c r="J17" s="105"/>
       <c r="K17" s="32"/>
       <c r="L17" s="43"/>
     </row>
@@ -11089,16 +11223,16 @@
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="31"/>
       <c r="B22" s="32"/>
-      <c r="C22" s="106" t="s">
+      <c r="C22" s="105" t="s">
         <v>43</v>
       </c>
-      <c r="D22" s="106"/>
-      <c r="E22" s="106"/>
-      <c r="F22" s="106"/>
-      <c r="G22" s="106"/>
-      <c r="H22" s="106"/>
-      <c r="I22" s="106"/>
-      <c r="J22" s="106"/>
+      <c r="D22" s="105"/>
+      <c r="E22" s="105"/>
+      <c r="F22" s="105"/>
+      <c r="G22" s="105"/>
+      <c r="H22" s="105"/>
+      <c r="I22" s="105"/>
+      <c r="J22" s="105"/>
       <c r="K22" s="32"/>
       <c r="L22" s="43"/>
     </row>
@@ -11200,16 +11334,16 @@
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="31"/>
       <c r="B27" s="32"/>
-      <c r="C27" s="106" t="s">
+      <c r="C27" s="105" t="s">
         <v>45</v>
       </c>
-      <c r="D27" s="106"/>
-      <c r="E27" s="106"/>
-      <c r="F27" s="106"/>
-      <c r="G27" s="106"/>
-      <c r="H27" s="106"/>
-      <c r="I27" s="106"/>
-      <c r="J27" s="106"/>
+      <c r="D27" s="105"/>
+      <c r="E27" s="105"/>
+      <c r="F27" s="105"/>
+      <c r="G27" s="105"/>
+      <c r="H27" s="105"/>
+      <c r="I27" s="105"/>
+      <c r="J27" s="105"/>
       <c r="K27" s="32"/>
       <c r="L27" s="43"/>
     </row>
@@ -11300,16 +11434,16 @@
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="31"/>
       <c r="B32" s="32"/>
-      <c r="C32" s="106" t="s">
+      <c r="C32" s="105" t="s">
         <v>46</v>
       </c>
-      <c r="D32" s="106"/>
-      <c r="E32" s="106"/>
-      <c r="F32" s="106"/>
-      <c r="G32" s="106"/>
-      <c r="H32" s="106"/>
-      <c r="I32" s="106"/>
-      <c r="J32" s="106"/>
+      <c r="D32" s="105"/>
+      <c r="E32" s="105"/>
+      <c r="F32" s="105"/>
+      <c r="G32" s="105"/>
+      <c r="H32" s="105"/>
+      <c r="I32" s="105"/>
+      <c r="J32" s="105"/>
       <c r="K32" s="32"/>
       <c r="L32" s="43"/>
     </row>
@@ -11400,16 +11534,16 @@
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="31"/>
       <c r="B37" s="32"/>
-      <c r="C37" s="106" t="s">
+      <c r="C37" s="105" t="s">
         <v>47</v>
       </c>
-      <c r="D37" s="106"/>
-      <c r="E37" s="106"/>
-      <c r="F37" s="106"/>
-      <c r="G37" s="106"/>
-      <c r="H37" s="106"/>
-      <c r="I37" s="106"/>
-      <c r="J37" s="106"/>
+      <c r="D37" s="105"/>
+      <c r="E37" s="105"/>
+      <c r="F37" s="105"/>
+      <c r="G37" s="105"/>
+      <c r="H37" s="105"/>
+      <c r="I37" s="105"/>
+      <c r="J37" s="105"/>
       <c r="K37" s="32"/>
       <c r="L37" s="43"/>
     </row>
@@ -11500,16 +11634,16 @@
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="31"/>
       <c r="B42" s="32"/>
-      <c r="C42" s="106" t="s">
+      <c r="C42" s="105" t="s">
         <v>49</v>
       </c>
-      <c r="D42" s="106"/>
-      <c r="E42" s="106"/>
-      <c r="F42" s="106"/>
-      <c r="G42" s="106"/>
-      <c r="H42" s="106"/>
-      <c r="I42" s="106"/>
-      <c r="J42" s="106"/>
+      <c r="D42" s="105"/>
+      <c r="E42" s="105"/>
+      <c r="F42" s="105"/>
+      <c r="G42" s="105"/>
+      <c r="H42" s="105"/>
+      <c r="I42" s="105"/>
+      <c r="J42" s="105"/>
       <c r="K42" s="32"/>
       <c r="L42" s="43"/>
     </row>
@@ -11600,16 +11734,16 @@
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="31"/>
       <c r="B47" s="32"/>
-      <c r="C47" s="106" t="s">
+      <c r="C47" s="105" t="s">
         <v>50</v>
       </c>
-      <c r="D47" s="106"/>
-      <c r="E47" s="106"/>
-      <c r="F47" s="106"/>
-      <c r="G47" s="106"/>
-      <c r="H47" s="106"/>
-      <c r="I47" s="106"/>
-      <c r="J47" s="106"/>
+      <c r="D47" s="105"/>
+      <c r="E47" s="105"/>
+      <c r="F47" s="105"/>
+      <c r="G47" s="105"/>
+      <c r="H47" s="105"/>
+      <c r="I47" s="105"/>
+      <c r="J47" s="105"/>
       <c r="K47" s="32"/>
       <c r="L47" s="43"/>
     </row>
@@ -11700,16 +11834,16 @@
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="31"/>
       <c r="B52" s="32"/>
-      <c r="C52" s="106" t="s">
+      <c r="C52" s="105" t="s">
         <v>51</v>
       </c>
-      <c r="D52" s="106"/>
-      <c r="E52" s="106"/>
-      <c r="F52" s="106"/>
-      <c r="G52" s="106"/>
-      <c r="H52" s="106"/>
-      <c r="I52" s="106"/>
-      <c r="J52" s="106"/>
+      <c r="D52" s="105"/>
+      <c r="E52" s="105"/>
+      <c r="F52" s="105"/>
+      <c r="G52" s="105"/>
+      <c r="H52" s="105"/>
+      <c r="I52" s="105"/>
+      <c r="J52" s="105"/>
       <c r="K52" s="32"/>
       <c r="L52" s="43"/>
     </row>
@@ -11800,16 +11934,16 @@
     <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" s="31"/>
       <c r="B57" s="32"/>
-      <c r="C57" s="106" t="s">
+      <c r="C57" s="105" t="s">
         <v>52</v>
       </c>
-      <c r="D57" s="106"/>
-      <c r="E57" s="106"/>
-      <c r="F57" s="106"/>
-      <c r="G57" s="106"/>
-      <c r="H57" s="106"/>
-      <c r="I57" s="106"/>
-      <c r="J57" s="106"/>
+      <c r="D57" s="105"/>
+      <c r="E57" s="105"/>
+      <c r="F57" s="105"/>
+      <c r="G57" s="105"/>
+      <c r="H57" s="105"/>
+      <c r="I57" s="105"/>
+      <c r="J57" s="105"/>
       <c r="K57" s="32"/>
       <c r="L57" s="43"/>
     </row>
@@ -11956,6 +12090,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="C2:J2"/>
+    <mergeCell ref="C7:J7"/>
+    <mergeCell ref="C12:J12"/>
+    <mergeCell ref="C17:J17"/>
+    <mergeCell ref="C47:J47"/>
     <mergeCell ref="C52:J52"/>
     <mergeCell ref="C57:J57"/>
     <mergeCell ref="C22:J22"/>
@@ -11963,11 +12102,6 @@
     <mergeCell ref="C32:J32"/>
     <mergeCell ref="C37:J37"/>
     <mergeCell ref="C42:J42"/>
-    <mergeCell ref="C2:J2"/>
-    <mergeCell ref="C7:J7"/>
-    <mergeCell ref="C12:J12"/>
-    <mergeCell ref="C17:J17"/>
-    <mergeCell ref="C47:J47"/>
   </mergeCells>
   <conditionalFormatting sqref="H65">
     <cfRule type="cellIs" dxfId="42" priority="98" operator="equal">

</xml_diff>

<commit_message>
work for demo asap
</commit_message>
<xml_diff>
--- a/src/main/resources/modules/SMOKE.xlsx
+++ b/src/main/resources/modules/SMOKE.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="5400" windowWidth="20490" windowHeight="7485"/>
+    <workbookView xWindow="0" yWindow="7200" windowWidth="20490" windowHeight="5250"/>
   </bookViews>
   <sheets>
     <sheet name="Controller" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4218" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4220" uniqueCount="241">
   <si>
     <t>TC_ID</t>
   </si>
@@ -743,6 +743,12 @@
   </si>
   <si>
     <t>13th Period - Lessor - Operating - Validate user is able to Add Revision</t>
+  </si>
+  <si>
+    <t>TCEnv105</t>
+  </si>
+  <si>
+    <t>TCEnv106</t>
   </si>
 </sst>
 </file>
@@ -1531,6 +1537,11 @@
     <xf numFmtId="0" fontId="19" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1569,11 +1580,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -4988,8 +4994,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1005"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44:D48"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -5093,7 +5099,7 @@
         <v>25</v>
       </c>
       <c r="D3" s="99" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="E3" s="62" t="s">
         <v>27</v>
@@ -5365,10 +5371,10 @@
       <c r="A15" s="63">
         <v>13</v>
       </c>
-      <c r="B15" s="152">
+      <c r="B15" s="132">
         <v>6579744</v>
       </c>
-      <c r="C15" s="152" t="s">
+      <c r="C15" s="132" t="s">
         <v>224</v>
       </c>
       <c r="D15" s="99" t="s">
@@ -5390,10 +5396,10 @@
       <c r="A16" s="63">
         <v>13</v>
       </c>
-      <c r="B16" s="152">
+      <c r="B16" s="132">
         <v>6579785</v>
       </c>
-      <c r="C16" s="152" t="s">
+      <c r="C16" s="132" t="s">
         <v>228</v>
       </c>
       <c r="D16" s="99" t="s">
@@ -5452,13 +5458,16 @@
         <v>71</v>
       </c>
       <c r="D19" s="99" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E19" s="62" t="s">
         <v>27</v>
       </c>
       <c r="F19" s="62" t="s">
         <v>27</v>
+      </c>
+      <c r="I19" s="118" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="20" spans="1:26">
@@ -5669,7 +5678,7 @@
       <c r="B30" s="124">
         <v>6591989</v>
       </c>
-      <c r="C30" s="152" t="s">
+      <c r="C30" s="132" t="s">
         <v>220</v>
       </c>
       <c r="D30" s="99" t="s">
@@ -5690,7 +5699,7 @@
       <c r="B31" s="124">
         <v>6591990</v>
       </c>
-      <c r="C31" s="152" t="s">
+      <c r="C31" s="132" t="s">
         <v>236</v>
       </c>
       <c r="D31" s="99" t="s">
@@ -5711,7 +5720,7 @@
       <c r="B32" s="124">
         <v>6591991</v>
       </c>
-      <c r="C32" s="152" t="s">
+      <c r="C32" s="132" t="s">
         <v>237</v>
       </c>
       <c r="D32" s="99" t="s">
@@ -5725,10 +5734,10 @@
       </c>
       <c r="I32" s="125"/>
     </row>
-    <row r="33" spans="1:26" s="153" customFormat="1" ht="15.75" customHeight="1">
-      <c r="B33" s="154"/>
-      <c r="E33" s="154"/>
-      <c r="F33" s="154"/>
+    <row r="33" spans="1:26" s="133" customFormat="1" ht="15.75" customHeight="1">
+      <c r="B33" s="134"/>
+      <c r="E33" s="134"/>
+      <c r="F33" s="134"/>
     </row>
     <row r="34" spans="1:26" ht="15.75" customHeight="1">
       <c r="A34" s="113"/>
@@ -5779,6 +5788,9 @@
       <c r="F35" s="62" t="s">
         <v>27</v>
       </c>
+      <c r="I35" s="118" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="36" spans="1:26" ht="15.75" customHeight="1">
       <c r="A36" s="62">
@@ -6068,7 +6080,7 @@
       <c r="B46" s="124">
         <v>6591993</v>
       </c>
-      <c r="C46" s="152" t="s">
+      <c r="C46" s="132" t="s">
         <v>238</v>
       </c>
       <c r="D46" s="99" t="s">
@@ -6089,7 +6101,7 @@
       <c r="B47" s="127">
         <v>6591994</v>
       </c>
-      <c r="C47" s="152" t="s">
+      <c r="C47" s="132" t="s">
         <v>231</v>
       </c>
       <c r="D47" s="99" t="s">
@@ -6110,7 +6122,7 @@
       <c r="B48" s="124">
         <v>6591995</v>
       </c>
-      <c r="C48" s="152" t="s">
+      <c r="C48" s="132" t="s">
         <v>232</v>
       </c>
       <c r="D48" s="99" t="s">
@@ -7091,7 +7103,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A64" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -7099,7 +7113,7 @@
     <col min="2" max="2" width="11" customWidth="1"/>
     <col min="3" max="3" width="69.7109375" customWidth="1"/>
     <col min="4" max="6" width="50.7109375" customWidth="1"/>
-    <col min="7" max="7" width="111.28515625" customWidth="1"/>
+    <col min="7" max="7" width="43.7109375" customWidth="1"/>
     <col min="8" max="8" width="14" customWidth="1"/>
     <col min="9" max="9" width="16.140625" customWidth="1"/>
     <col min="10" max="10" width="17.7109375" customWidth="1"/>
@@ -7161,12 +7175,12 @@
     </row>
     <row r="2" spans="1:26" ht="19.5" customHeight="1">
       <c r="A2" s="7"/>
-      <c r="B2" s="138" t="s">
+      <c r="B2" s="141" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="133"/>
-      <c r="D2" s="133"/>
-      <c r="E2" s="139"/>
+      <c r="C2" s="136"/>
+      <c r="D2" s="136"/>
+      <c r="E2" s="142"/>
       <c r="F2" s="13"/>
       <c r="G2" s="15"/>
       <c r="H2" s="7"/>
@@ -7435,12 +7449,12 @@
     </row>
     <row r="11" spans="1:26">
       <c r="A11" s="8"/>
-      <c r="B11" s="140" t="s">
+      <c r="B11" s="143" t="s">
         <v>108</v>
       </c>
-      <c r="C11" s="141"/>
-      <c r="D11" s="141"/>
-      <c r="E11" s="142"/>
+      <c r="C11" s="144"/>
+      <c r="D11" s="144"/>
+      <c r="E11" s="145"/>
       <c r="F11" s="9"/>
       <c r="G11" s="9"/>
       <c r="H11" s="10"/>
@@ -7794,12 +7808,12 @@
     </row>
     <row r="23" spans="1:26" ht="15.75" customHeight="1">
       <c r="A23" s="8"/>
-      <c r="B23" s="143" t="s">
+      <c r="B23" s="146" t="s">
         <v>131</v>
       </c>
-      <c r="C23" s="136"/>
-      <c r="D23" s="136"/>
-      <c r="E23" s="137"/>
+      <c r="C23" s="139"/>
+      <c r="D23" s="139"/>
+      <c r="E23" s="140"/>
       <c r="F23" s="9"/>
       <c r="G23" s="9"/>
       <c r="H23" s="10"/>
@@ -8068,12 +8082,12 @@
     </row>
     <row r="32" spans="1:26" ht="15.75" customHeight="1">
       <c r="A32" s="38"/>
-      <c r="B32" s="144" t="s">
+      <c r="B32" s="147" t="s">
         <v>133</v>
       </c>
-      <c r="C32" s="133"/>
-      <c r="D32" s="133"/>
-      <c r="E32" s="134"/>
+      <c r="C32" s="136"/>
+      <c r="D32" s="136"/>
+      <c r="E32" s="137"/>
       <c r="F32" s="39"/>
       <c r="G32" s="40"/>
       <c r="H32" s="17"/>
@@ -8427,12 +8441,12 @@
     </row>
     <row r="44" spans="1:26" ht="15.75" customHeight="1">
       <c r="A44" s="8"/>
-      <c r="B44" s="135" t="s">
+      <c r="B44" s="138" t="s">
         <v>134</v>
       </c>
-      <c r="C44" s="136"/>
-      <c r="D44" s="136"/>
-      <c r="E44" s="137"/>
+      <c r="C44" s="139"/>
+      <c r="D44" s="139"/>
+      <c r="E44" s="140"/>
       <c r="F44" s="9"/>
       <c r="G44" s="9"/>
       <c r="H44" s="10"/>
@@ -8701,12 +8715,12 @@
     </row>
     <row r="53" spans="1:26" ht="15.75" customHeight="1">
       <c r="A53" s="8"/>
-      <c r="B53" s="135" t="s">
+      <c r="B53" s="138" t="s">
         <v>136</v>
       </c>
-      <c r="C53" s="136"/>
-      <c r="D53" s="136"/>
-      <c r="E53" s="137"/>
+      <c r="C53" s="139"/>
+      <c r="D53" s="139"/>
+      <c r="E53" s="140"/>
       <c r="F53" s="9"/>
       <c r="G53" s="9"/>
       <c r="H53" s="10"/>
@@ -9060,12 +9074,12 @@
     </row>
     <row r="65" spans="1:26" ht="15.75" customHeight="1">
       <c r="A65" s="8"/>
-      <c r="B65" s="135" t="s">
+      <c r="B65" s="138" t="s">
         <v>138</v>
       </c>
-      <c r="C65" s="136"/>
-      <c r="D65" s="136"/>
-      <c r="E65" s="137"/>
+      <c r="C65" s="139"/>
+      <c r="D65" s="139"/>
+      <c r="E65" s="140"/>
       <c r="F65" s="9"/>
       <c r="G65" s="9"/>
       <c r="H65" s="10"/>
@@ -9455,12 +9469,12 @@
     </row>
     <row r="78" spans="1:26" ht="15.75" customHeight="1">
       <c r="A78" s="8"/>
-      <c r="B78" s="135" t="s">
+      <c r="B78" s="138" t="s">
         <v>147</v>
       </c>
-      <c r="C78" s="136"/>
-      <c r="D78" s="136"/>
-      <c r="E78" s="137"/>
+      <c r="C78" s="139"/>
+      <c r="D78" s="139"/>
+      <c r="E78" s="140"/>
       <c r="F78" s="9"/>
       <c r="G78" s="9"/>
       <c r="H78" s="10"/>
@@ -9850,11 +9864,11 @@
     </row>
     <row r="91" spans="1:26" ht="15.75" customHeight="1">
       <c r="A91" s="55"/>
-      <c r="B91" s="132" t="s">
+      <c r="B91" s="135" t="s">
         <v>152</v>
       </c>
-      <c r="C91" s="133"/>
-      <c r="D91" s="134"/>
+      <c r="C91" s="136"/>
+      <c r="D91" s="137"/>
       <c r="E91" s="56"/>
       <c r="F91" s="56"/>
       <c r="G91" s="56"/>
@@ -10245,11 +10259,11 @@
     </row>
     <row r="104" spans="1:26" ht="15.75" customHeight="1">
       <c r="A104" s="55"/>
-      <c r="B104" s="132" t="s">
+      <c r="B104" s="135" t="s">
         <v>154</v>
       </c>
-      <c r="C104" s="133"/>
-      <c r="D104" s="134"/>
+      <c r="C104" s="136"/>
+      <c r="D104" s="137"/>
       <c r="E104" s="56"/>
       <c r="F104" s="56"/>
       <c r="G104" s="56"/>
@@ -10640,11 +10654,11 @@
     </row>
     <row r="117" spans="1:26" ht="15.75" customHeight="1">
       <c r="A117" s="55"/>
-      <c r="B117" s="132" t="s">
+      <c r="B117" s="135" t="s">
         <v>155</v>
       </c>
-      <c r="C117" s="133"/>
-      <c r="D117" s="134"/>
+      <c r="C117" s="136"/>
+      <c r="D117" s="137"/>
       <c r="E117" s="56"/>
       <c r="F117" s="56"/>
       <c r="G117" s="56"/>
@@ -11035,11 +11049,11 @@
     </row>
     <row r="130" spans="1:26" ht="15.75" customHeight="1">
       <c r="A130" s="55"/>
-      <c r="B130" s="132" t="s">
+      <c r="B130" s="135" t="s">
         <v>156</v>
       </c>
-      <c r="C130" s="133"/>
-      <c r="D130" s="134"/>
+      <c r="C130" s="136"/>
+      <c r="D130" s="137"/>
       <c r="E130" s="56"/>
       <c r="F130" s="56"/>
       <c r="G130" s="56"/>
@@ -16086,11 +16100,11 @@
     </row>
     <row r="2" spans="1:26">
       <c r="A2" s="8"/>
-      <c r="B2" s="145" t="s">
+      <c r="B2" s="148" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="146"/>
-      <c r="D2" s="147"/>
+      <c r="C2" s="149"/>
+      <c r="D2" s="150"/>
       <c r="E2" s="9"/>
       <c r="F2" s="9"/>
       <c r="G2" s="9"/>
@@ -16302,11 +16316,11 @@
     </row>
     <row r="10" spans="1:26">
       <c r="A10" s="8"/>
-      <c r="B10" s="145" t="s">
+      <c r="B10" s="148" t="s">
         <v>49</v>
       </c>
-      <c r="C10" s="146"/>
-      <c r="D10" s="147"/>
+      <c r="C10" s="149"/>
+      <c r="D10" s="150"/>
       <c r="E10" s="9"/>
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
@@ -16518,11 +16532,11 @@
     </row>
     <row r="18" spans="1:26">
       <c r="A18" s="8"/>
-      <c r="B18" s="145" t="s">
+      <c r="B18" s="148" t="s">
         <v>64</v>
       </c>
-      <c r="C18" s="146"/>
-      <c r="D18" s="147"/>
+      <c r="C18" s="149"/>
+      <c r="D18" s="150"/>
       <c r="E18" s="9"/>
       <c r="F18" s="9"/>
       <c r="G18" s="9"/>
@@ -16734,11 +16748,11 @@
     </row>
     <row r="26" spans="1:26" ht="15.75" customHeight="1">
       <c r="A26" s="8"/>
-      <c r="B26" s="145" t="s">
+      <c r="B26" s="148" t="s">
         <v>70</v>
       </c>
-      <c r="C26" s="146"/>
-      <c r="D26" s="147"/>
+      <c r="C26" s="149"/>
+      <c r="D26" s="150"/>
       <c r="E26" s="9"/>
       <c r="F26" s="9"/>
       <c r="G26" s="9"/>
@@ -16950,11 +16964,11 @@
     </row>
     <row r="34" spans="1:26" ht="15.75" customHeight="1">
       <c r="A34" s="8"/>
-      <c r="B34" s="145" t="s">
+      <c r="B34" s="148" t="s">
         <v>95</v>
       </c>
-      <c r="C34" s="146"/>
-      <c r="D34" s="147"/>
+      <c r="C34" s="149"/>
+      <c r="D34" s="150"/>
       <c r="E34" s="9"/>
       <c r="F34" s="9"/>
       <c r="G34" s="9"/>
@@ -17160,11 +17174,11 @@
     </row>
     <row r="42" spans="1:26" ht="15.75" customHeight="1">
       <c r="A42" s="8"/>
-      <c r="B42" s="145" t="s">
+      <c r="B42" s="148" t="s">
         <v>110</v>
       </c>
-      <c r="C42" s="146"/>
-      <c r="D42" s="147"/>
+      <c r="C42" s="149"/>
+      <c r="D42" s="150"/>
       <c r="E42" s="9"/>
       <c r="F42" s="9"/>
       <c r="G42" s="9"/>
@@ -21628,16 +21642,16 @@
     <row r="2" spans="1:26">
       <c r="A2" s="44"/>
       <c r="B2" s="45"/>
-      <c r="C2" s="148" t="s">
+      <c r="C2" s="151" t="s">
         <v>61</v>
       </c>
-      <c r="D2" s="133"/>
-      <c r="E2" s="133"/>
-      <c r="F2" s="133"/>
-      <c r="G2" s="133"/>
-      <c r="H2" s="133"/>
-      <c r="I2" s="133"/>
-      <c r="J2" s="139"/>
+      <c r="D2" s="136"/>
+      <c r="E2" s="136"/>
+      <c r="F2" s="136"/>
+      <c r="G2" s="136"/>
+      <c r="H2" s="136"/>
+      <c r="I2" s="136"/>
+      <c r="J2" s="142"/>
       <c r="K2" s="45"/>
       <c r="L2" s="46"/>
       <c r="M2" s="47"/>
@@ -21812,16 +21826,16 @@
     <row r="7" spans="1:26">
       <c r="A7" s="44"/>
       <c r="B7" s="45"/>
-      <c r="C7" s="148" t="s">
+      <c r="C7" s="151" t="s">
         <v>65</v>
       </c>
-      <c r="D7" s="133"/>
-      <c r="E7" s="133"/>
-      <c r="F7" s="133"/>
-      <c r="G7" s="133"/>
-      <c r="H7" s="133"/>
-      <c r="I7" s="133"/>
-      <c r="J7" s="139"/>
+      <c r="D7" s="136"/>
+      <c r="E7" s="136"/>
+      <c r="F7" s="136"/>
+      <c r="G7" s="136"/>
+      <c r="H7" s="136"/>
+      <c r="I7" s="136"/>
+      <c r="J7" s="142"/>
       <c r="K7" s="45"/>
       <c r="L7" s="46"/>
       <c r="M7" s="47"/>
@@ -21996,16 +22010,16 @@
     <row r="12" spans="1:26">
       <c r="A12" s="44"/>
       <c r="B12" s="45"/>
-      <c r="C12" s="148" t="s">
+      <c r="C12" s="151" t="s">
         <v>66</v>
       </c>
-      <c r="D12" s="133"/>
-      <c r="E12" s="133"/>
-      <c r="F12" s="133"/>
-      <c r="G12" s="133"/>
-      <c r="H12" s="133"/>
-      <c r="I12" s="133"/>
-      <c r="J12" s="139"/>
+      <c r="D12" s="136"/>
+      <c r="E12" s="136"/>
+      <c r="F12" s="136"/>
+      <c r="G12" s="136"/>
+      <c r="H12" s="136"/>
+      <c r="I12" s="136"/>
+      <c r="J12" s="142"/>
       <c r="K12" s="45"/>
       <c r="L12" s="46"/>
       <c r="M12" s="47"/>
@@ -22180,16 +22194,16 @@
     <row r="17" spans="1:26">
       <c r="A17" s="44"/>
       <c r="B17" s="45"/>
-      <c r="C17" s="148" t="s">
+      <c r="C17" s="151" t="s">
         <v>69</v>
       </c>
-      <c r="D17" s="133"/>
-      <c r="E17" s="133"/>
-      <c r="F17" s="133"/>
-      <c r="G17" s="133"/>
-      <c r="H17" s="133"/>
-      <c r="I17" s="133"/>
-      <c r="J17" s="139"/>
+      <c r="D17" s="136"/>
+      <c r="E17" s="136"/>
+      <c r="F17" s="136"/>
+      <c r="G17" s="136"/>
+      <c r="H17" s="136"/>
+      <c r="I17" s="136"/>
+      <c r="J17" s="142"/>
       <c r="K17" s="45"/>
       <c r="L17" s="46"/>
       <c r="M17" s="47"/>
@@ -22364,16 +22378,16 @@
     <row r="22" spans="1:26" ht="15.75" customHeight="1">
       <c r="A22" s="44"/>
       <c r="B22" s="45"/>
-      <c r="C22" s="148" t="s">
+      <c r="C22" s="151" t="s">
         <v>79</v>
       </c>
-      <c r="D22" s="133"/>
-      <c r="E22" s="133"/>
-      <c r="F22" s="133"/>
-      <c r="G22" s="133"/>
-      <c r="H22" s="133"/>
-      <c r="I22" s="133"/>
-      <c r="J22" s="139"/>
+      <c r="D22" s="136"/>
+      <c r="E22" s="136"/>
+      <c r="F22" s="136"/>
+      <c r="G22" s="136"/>
+      <c r="H22" s="136"/>
+      <c r="I22" s="136"/>
+      <c r="J22" s="142"/>
       <c r="K22" s="45"/>
       <c r="L22" s="46"/>
       <c r="M22" s="47"/>
@@ -22538,16 +22552,16 @@
     <row r="27" spans="1:26" ht="15.75" customHeight="1">
       <c r="A27" s="44"/>
       <c r="B27" s="45"/>
-      <c r="C27" s="148" t="s">
+      <c r="C27" s="151" t="s">
         <v>83</v>
       </c>
-      <c r="D27" s="133"/>
-      <c r="E27" s="133"/>
-      <c r="F27" s="133"/>
-      <c r="G27" s="133"/>
-      <c r="H27" s="133"/>
-      <c r="I27" s="133"/>
-      <c r="J27" s="139"/>
+      <c r="D27" s="136"/>
+      <c r="E27" s="136"/>
+      <c r="F27" s="136"/>
+      <c r="G27" s="136"/>
+      <c r="H27" s="136"/>
+      <c r="I27" s="136"/>
+      <c r="J27" s="142"/>
       <c r="K27" s="45"/>
       <c r="L27" s="46"/>
       <c r="M27" s="47"/>
@@ -22722,16 +22736,16 @@
     <row r="32" spans="1:26" ht="15.75" customHeight="1">
       <c r="A32" s="44"/>
       <c r="B32" s="45"/>
-      <c r="C32" s="148" t="s">
+      <c r="C32" s="151" t="s">
         <v>84</v>
       </c>
-      <c r="D32" s="133"/>
-      <c r="E32" s="133"/>
-      <c r="F32" s="133"/>
-      <c r="G32" s="133"/>
-      <c r="H32" s="133"/>
-      <c r="I32" s="133"/>
-      <c r="J32" s="139"/>
+      <c r="D32" s="136"/>
+      <c r="E32" s="136"/>
+      <c r="F32" s="136"/>
+      <c r="G32" s="136"/>
+      <c r="H32" s="136"/>
+      <c r="I32" s="136"/>
+      <c r="J32" s="142"/>
       <c r="K32" s="45"/>
       <c r="L32" s="46"/>
       <c r="M32" s="47"/>
@@ -22906,16 +22920,16 @@
     <row r="37" spans="1:26" ht="15.75" customHeight="1">
       <c r="A37" s="44"/>
       <c r="B37" s="45"/>
-      <c r="C37" s="148" t="s">
+      <c r="C37" s="151" t="s">
         <v>87</v>
       </c>
-      <c r="D37" s="133"/>
-      <c r="E37" s="133"/>
-      <c r="F37" s="133"/>
-      <c r="G37" s="133"/>
-      <c r="H37" s="133"/>
-      <c r="I37" s="133"/>
-      <c r="J37" s="139"/>
+      <c r="D37" s="136"/>
+      <c r="E37" s="136"/>
+      <c r="F37" s="136"/>
+      <c r="G37" s="136"/>
+      <c r="H37" s="136"/>
+      <c r="I37" s="136"/>
+      <c r="J37" s="142"/>
       <c r="K37" s="45"/>
       <c r="L37" s="46"/>
       <c r="M37" s="47"/>
@@ -23090,16 +23104,16 @@
     <row r="42" spans="1:26" ht="15.75" customHeight="1">
       <c r="A42" s="44"/>
       <c r="B42" s="45"/>
-      <c r="C42" s="148" t="s">
+      <c r="C42" s="151" t="s">
         <v>112</v>
       </c>
-      <c r="D42" s="133"/>
-      <c r="E42" s="133"/>
-      <c r="F42" s="133"/>
-      <c r="G42" s="133"/>
-      <c r="H42" s="133"/>
-      <c r="I42" s="133"/>
-      <c r="J42" s="139"/>
+      <c r="D42" s="136"/>
+      <c r="E42" s="136"/>
+      <c r="F42" s="136"/>
+      <c r="G42" s="136"/>
+      <c r="H42" s="136"/>
+      <c r="I42" s="136"/>
+      <c r="J42" s="142"/>
       <c r="K42" s="45"/>
       <c r="L42" s="46"/>
       <c r="M42" s="47"/>
@@ -23274,16 +23288,16 @@
     <row r="47" spans="1:26" ht="15.75" customHeight="1">
       <c r="A47" s="44"/>
       <c r="B47" s="45"/>
-      <c r="C47" s="148" t="s">
+      <c r="C47" s="151" t="s">
         <v>113</v>
       </c>
-      <c r="D47" s="133"/>
-      <c r="E47" s="133"/>
-      <c r="F47" s="133"/>
-      <c r="G47" s="133"/>
-      <c r="H47" s="133"/>
-      <c r="I47" s="133"/>
-      <c r="J47" s="139"/>
+      <c r="D47" s="136"/>
+      <c r="E47" s="136"/>
+      <c r="F47" s="136"/>
+      <c r="G47" s="136"/>
+      <c r="H47" s="136"/>
+      <c r="I47" s="136"/>
+      <c r="J47" s="142"/>
       <c r="K47" s="45"/>
       <c r="L47" s="46"/>
       <c r="M47" s="47"/>
@@ -23458,16 +23472,16 @@
     <row r="52" spans="1:26" ht="15.75" customHeight="1">
       <c r="A52" s="44"/>
       <c r="B52" s="45"/>
-      <c r="C52" s="148" t="s">
+      <c r="C52" s="151" t="s">
         <v>114</v>
       </c>
-      <c r="D52" s="133"/>
-      <c r="E52" s="133"/>
-      <c r="F52" s="133"/>
-      <c r="G52" s="133"/>
-      <c r="H52" s="133"/>
-      <c r="I52" s="133"/>
-      <c r="J52" s="139"/>
+      <c r="D52" s="136"/>
+      <c r="E52" s="136"/>
+      <c r="F52" s="136"/>
+      <c r="G52" s="136"/>
+      <c r="H52" s="136"/>
+      <c r="I52" s="136"/>
+      <c r="J52" s="142"/>
       <c r="K52" s="45"/>
       <c r="L52" s="46"/>
       <c r="M52" s="47"/>
@@ -23642,16 +23656,16 @@
     <row r="57" spans="1:26" ht="15.75" customHeight="1">
       <c r="A57" s="44"/>
       <c r="B57" s="45"/>
-      <c r="C57" s="148" t="s">
+      <c r="C57" s="151" t="s">
         <v>116</v>
       </c>
-      <c r="D57" s="133"/>
-      <c r="E57" s="133"/>
-      <c r="F57" s="133"/>
-      <c r="G57" s="133"/>
-      <c r="H57" s="133"/>
-      <c r="I57" s="133"/>
-      <c r="J57" s="139"/>
+      <c r="D57" s="136"/>
+      <c r="E57" s="136"/>
+      <c r="F57" s="136"/>
+      <c r="G57" s="136"/>
+      <c r="H57" s="136"/>
+      <c r="I57" s="136"/>
+      <c r="J57" s="142"/>
       <c r="K57" s="45"/>
       <c r="L57" s="46"/>
       <c r="M57" s="47"/>
@@ -50309,16 +50323,16 @@
     <row r="2" spans="1:26" s="99" customFormat="1">
       <c r="A2" s="94"/>
       <c r="B2" s="95"/>
-      <c r="C2" s="149" t="s">
+      <c r="C2" s="152" t="s">
         <v>209</v>
       </c>
-      <c r="D2" s="150"/>
-      <c r="E2" s="150"/>
-      <c r="F2" s="150"/>
-      <c r="G2" s="150"/>
-      <c r="H2" s="150"/>
-      <c r="I2" s="150"/>
-      <c r="J2" s="150"/>
+      <c r="D2" s="153"/>
+      <c r="E2" s="153"/>
+      <c r="F2" s="153"/>
+      <c r="G2" s="153"/>
+      <c r="H2" s="153"/>
+      <c r="I2" s="153"/>
+      <c r="J2" s="153"/>
       <c r="K2" s="96"/>
       <c r="L2" s="97"/>
       <c r="M2" s="98"/>
@@ -51299,16 +51313,16 @@
     <row r="36" spans="1:12" ht="15" customHeight="1">
       <c r="A36" s="94"/>
       <c r="B36" s="95"/>
-      <c r="C36" s="149" t="s">
+      <c r="C36" s="152" t="s">
         <v>213</v>
       </c>
-      <c r="D36" s="150"/>
-      <c r="E36" s="150"/>
-      <c r="F36" s="150"/>
-      <c r="G36" s="150"/>
-      <c r="H36" s="150"/>
-      <c r="I36" s="150"/>
-      <c r="J36" s="150"/>
+      <c r="D36" s="153"/>
+      <c r="E36" s="153"/>
+      <c r="F36" s="153"/>
+      <c r="G36" s="153"/>
+      <c r="H36" s="153"/>
+      <c r="I36" s="153"/>
+      <c r="J36" s="153"/>
       <c r="K36" s="96"/>
       <c r="L36" s="97"/>
     </row>
@@ -52316,16 +52330,16 @@
     <row r="70" spans="1:26" ht="15" customHeight="1">
       <c r="A70" s="94"/>
       <c r="B70" s="95"/>
-      <c r="C70" s="149" t="s">
+      <c r="C70" s="152" t="s">
         <v>224</v>
       </c>
-      <c r="D70" s="150"/>
-      <c r="E70" s="150"/>
-      <c r="F70" s="150"/>
-      <c r="G70" s="150"/>
-      <c r="H70" s="150"/>
-      <c r="I70" s="150"/>
-      <c r="J70" s="150"/>
+      <c r="D70" s="153"/>
+      <c r="E70" s="153"/>
+      <c r="F70" s="153"/>
+      <c r="G70" s="153"/>
+      <c r="H70" s="153"/>
+      <c r="I70" s="153"/>
+      <c r="J70" s="153"/>
       <c r="K70" s="96"/>
       <c r="L70" s="97"/>
     </row>
@@ -53367,16 +53381,16 @@
     <row r="106" spans="1:26" ht="15" customHeight="1">
       <c r="A106" s="94"/>
       <c r="B106" s="95"/>
-      <c r="C106" s="149" t="s">
+      <c r="C106" s="152" t="s">
         <v>228</v>
       </c>
-      <c r="D106" s="150"/>
-      <c r="E106" s="150"/>
-      <c r="F106" s="150"/>
-      <c r="G106" s="150"/>
-      <c r="H106" s="150"/>
-      <c r="I106" s="150"/>
-      <c r="J106" s="150"/>
+      <c r="D106" s="153"/>
+      <c r="E106" s="153"/>
+      <c r="F106" s="153"/>
+      <c r="G106" s="153"/>
+      <c r="H106" s="153"/>
+      <c r="I106" s="153"/>
+      <c r="J106" s="153"/>
       <c r="K106" s="96"/>
       <c r="L106" s="97"/>
     </row>
@@ -54418,16 +54432,16 @@
     <row r="142" spans="1:12" ht="15" customHeight="1">
       <c r="A142" s="94"/>
       <c r="B142" s="95"/>
-      <c r="C142" s="151" t="s">
+      <c r="C142" s="154" t="s">
         <v>218</v>
       </c>
-      <c r="D142" s="150"/>
-      <c r="E142" s="150"/>
-      <c r="F142" s="150"/>
-      <c r="G142" s="150"/>
-      <c r="H142" s="150"/>
-      <c r="I142" s="150"/>
-      <c r="J142" s="150"/>
+      <c r="D142" s="153"/>
+      <c r="E142" s="153"/>
+      <c r="F142" s="153"/>
+      <c r="G142" s="153"/>
+      <c r="H142" s="153"/>
+      <c r="I142" s="153"/>
+      <c r="J142" s="153"/>
       <c r="K142" s="96"/>
       <c r="L142" s="97"/>
     </row>
@@ -55392,16 +55406,16 @@
     <row r="177" spans="1:12" ht="15" customHeight="1">
       <c r="A177" s="94"/>
       <c r="B177" s="95"/>
-      <c r="C177" s="151" t="s">
+      <c r="C177" s="154" t="s">
         <v>220</v>
       </c>
-      <c r="D177" s="150"/>
-      <c r="E177" s="150"/>
-      <c r="F177" s="150"/>
-      <c r="G177" s="150"/>
-      <c r="H177" s="150"/>
-      <c r="I177" s="150"/>
-      <c r="J177" s="150"/>
+      <c r="D177" s="153"/>
+      <c r="E177" s="153"/>
+      <c r="F177" s="153"/>
+      <c r="G177" s="153"/>
+      <c r="H177" s="153"/>
+      <c r="I177" s="153"/>
+      <c r="J177" s="153"/>
       <c r="K177" s="96"/>
       <c r="L177" s="97"/>
     </row>
@@ -56364,16 +56378,16 @@
     <row r="213" spans="1:12" ht="15" customHeight="1">
       <c r="A213" s="94"/>
       <c r="B213" s="95"/>
-      <c r="C213" s="149" t="s">
+      <c r="C213" s="152" t="s">
         <v>233</v>
       </c>
-      <c r="D213" s="150"/>
-      <c r="E213" s="150"/>
-      <c r="F213" s="150"/>
-      <c r="G213" s="150"/>
-      <c r="H213" s="150"/>
-      <c r="I213" s="150"/>
-      <c r="J213" s="150"/>
+      <c r="D213" s="153"/>
+      <c r="E213" s="153"/>
+      <c r="F213" s="153"/>
+      <c r="G213" s="153"/>
+      <c r="H213" s="153"/>
+      <c r="I213" s="153"/>
+      <c r="J213" s="153"/>
       <c r="K213" s="96"/>
       <c r="L213" s="97"/>
     </row>
@@ -57402,16 +57416,16 @@
     <row r="250" spans="1:12" ht="15" customHeight="1">
       <c r="A250" s="94"/>
       <c r="B250" s="95"/>
-      <c r="C250" s="149" t="s">
+      <c r="C250" s="152" t="s">
         <v>234</v>
       </c>
-      <c r="D250" s="150"/>
-      <c r="E250" s="150"/>
-      <c r="F250" s="150"/>
-      <c r="G250" s="150"/>
-      <c r="H250" s="150"/>
-      <c r="I250" s="150"/>
-      <c r="J250" s="150"/>
+      <c r="D250" s="153"/>
+      <c r="E250" s="153"/>
+      <c r="F250" s="153"/>
+      <c r="G250" s="153"/>
+      <c r="H250" s="153"/>
+      <c r="I250" s="153"/>
+      <c r="J250" s="153"/>
       <c r="K250" s="96"/>
       <c r="L250" s="97"/>
     </row>
@@ -58445,16 +58459,16 @@
     <row r="323" spans="1:12" ht="15" customHeight="1">
       <c r="A323" s="94"/>
       <c r="B323" s="95"/>
-      <c r="C323" s="151" t="s">
+      <c r="C323" s="154" t="s">
         <v>221</v>
       </c>
-      <c r="D323" s="150"/>
-      <c r="E323" s="150"/>
-      <c r="F323" s="150"/>
-      <c r="G323" s="150"/>
-      <c r="H323" s="150"/>
-      <c r="I323" s="150"/>
-      <c r="J323" s="150"/>
+      <c r="D323" s="153"/>
+      <c r="E323" s="153"/>
+      <c r="F323" s="153"/>
+      <c r="G323" s="153"/>
+      <c r="H323" s="153"/>
+      <c r="I323" s="153"/>
+      <c r="J323" s="153"/>
       <c r="K323" s="96"/>
       <c r="L323" s="97"/>
     </row>
@@ -59419,16 +59433,16 @@
     <row r="359" spans="1:12" ht="15" customHeight="1">
       <c r="A359" s="94"/>
       <c r="B359" s="95"/>
-      <c r="C359" s="151" t="s">
+      <c r="C359" s="154" t="s">
         <v>222</v>
       </c>
-      <c r="D359" s="150"/>
-      <c r="E359" s="150"/>
-      <c r="F359" s="150"/>
-      <c r="G359" s="150"/>
-      <c r="H359" s="150"/>
-      <c r="I359" s="150"/>
-      <c r="J359" s="150"/>
+      <c r="D359" s="153"/>
+      <c r="E359" s="153"/>
+      <c r="F359" s="153"/>
+      <c r="G359" s="153"/>
+      <c r="H359" s="153"/>
+      <c r="I359" s="153"/>
+      <c r="J359" s="153"/>
       <c r="K359" s="96"/>
       <c r="L359" s="97"/>
     </row>
@@ -60390,16 +60404,16 @@
     <row r="395" spans="1:12" ht="15" customHeight="1">
       <c r="A395" s="94"/>
       <c r="B395" s="95"/>
-      <c r="C395" s="149" t="s">
+      <c r="C395" s="152" t="s">
         <v>231</v>
       </c>
-      <c r="D395" s="150"/>
-      <c r="E395" s="150"/>
-      <c r="F395" s="150"/>
-      <c r="G395" s="150"/>
-      <c r="H395" s="150"/>
-      <c r="I395" s="150"/>
-      <c r="J395" s="150"/>
+      <c r="D395" s="153"/>
+      <c r="E395" s="153"/>
+      <c r="F395" s="153"/>
+      <c r="G395" s="153"/>
+      <c r="H395" s="153"/>
+      <c r="I395" s="153"/>
+      <c r="J395" s="153"/>
       <c r="K395" s="96"/>
       <c r="L395" s="97"/>
     </row>
@@ -61427,16 +61441,16 @@
     <row r="431" spans="1:12" ht="15" customHeight="1">
       <c r="A431" s="94"/>
       <c r="B431" s="95"/>
-      <c r="C431" s="149" t="s">
+      <c r="C431" s="152" t="s">
         <v>232</v>
       </c>
-      <c r="D431" s="150"/>
-      <c r="E431" s="150"/>
-      <c r="F431" s="150"/>
-      <c r="G431" s="150"/>
-      <c r="H431" s="150"/>
-      <c r="I431" s="150"/>
-      <c r="J431" s="150"/>
+      <c r="D431" s="153"/>
+      <c r="E431" s="153"/>
+      <c r="F431" s="153"/>
+      <c r="G431" s="153"/>
+      <c r="H431" s="153"/>
+      <c r="I431" s="153"/>
+      <c r="J431" s="153"/>
       <c r="K431" s="96"/>
       <c r="L431" s="97"/>
     </row>

</xml_diff>

<commit_message>
Work for 30 smoke test cases on App
</commit_message>
<xml_diff>
--- a/src/main/resources/modules/SMOKE.xlsx
+++ b/src/main/resources/modules/SMOKE.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="7200" windowWidth="20490" windowHeight="5250"/>
+    <workbookView xWindow="0" yWindow="7650" windowWidth="20490" windowHeight="4800"/>
   </bookViews>
   <sheets>
     <sheet name="Controller" sheetId="1" r:id="rId1"/>
@@ -20,13 +20,14 @@
   </sheets>
   <externalReferences>
     <externalReference r:id="rId6"/>
+    <externalReference r:id="rId7"/>
   </externalReferences>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4220" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4300" uniqueCount="241">
   <si>
     <t>TC_ID</t>
   </si>
@@ -874,7 +875,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="20">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -961,6 +962,29 @@
       <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor rgb="FF4472C4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
       </patternFill>
     </fill>
   </fills>
@@ -1185,7 +1209,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="155">
+  <cellXfs count="164">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1542,19 +1566,10 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1564,8 +1579,17 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1582,12 +1606,184 @@
     <xf numFmtId="0" fontId="16" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="16" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="19" borderId="20" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="399">
+  <dxfs count="420">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -4729,6 +4925,19 @@
 </externalLink>
 </file>
 
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Controller"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -4995,7 +5204,7 @@
   <dimension ref="A1:Z1005"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="A44" sqref="A44:XFD44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -5099,7 +5308,7 @@
         <v>25</v>
       </c>
       <c r="D3" s="99" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E3" s="62" t="s">
         <v>27</v>
@@ -5122,7 +5331,7 @@
         <v>47</v>
       </c>
       <c r="D4" s="99" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E4" s="62" t="s">
         <v>27</v>
@@ -5148,7 +5357,7 @@
         <v>54</v>
       </c>
       <c r="D5" s="99" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E5" s="62" t="s">
         <v>55</v>
@@ -5171,7 +5380,7 @@
         <v>57</v>
       </c>
       <c r="D6" s="99" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E6" s="62" t="s">
         <v>55</v>
@@ -5194,7 +5403,7 @@
         <v>58</v>
       </c>
       <c r="D7" s="99" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E7" s="62" t="s">
         <v>55</v>
@@ -5217,7 +5426,7 @@
         <v>59</v>
       </c>
       <c r="D8" s="99" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E8" s="62" t="s">
         <v>55</v>
@@ -5240,7 +5449,7 @@
         <v>61</v>
       </c>
       <c r="D9" s="99" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E9" s="62" t="s">
         <v>62</v>
@@ -5263,7 +5472,7 @@
         <v>65</v>
       </c>
       <c r="D10" s="99" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E10" s="62" t="s">
         <v>62</v>
@@ -5286,7 +5495,7 @@
         <v>66</v>
       </c>
       <c r="D11" s="99" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E11" s="62" t="s">
         <v>62</v>
@@ -5309,7 +5518,7 @@
         <v>69</v>
       </c>
       <c r="D12" s="99" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E12" s="62" t="s">
         <v>62</v>
@@ -5481,13 +5690,16 @@
         <v>72</v>
       </c>
       <c r="D20" s="99" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E20" s="62" t="s">
         <v>27</v>
       </c>
       <c r="F20" s="62" t="s">
         <v>27</v>
+      </c>
+      <c r="I20" s="118" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="21" spans="1:26">
@@ -5501,13 +5713,16 @@
         <v>73</v>
       </c>
       <c r="D21" s="99" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E21" s="62" t="s">
         <v>55</v>
       </c>
       <c r="F21" s="62" t="s">
         <v>55</v>
+      </c>
+      <c r="I21" s="118" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="22" spans="1:26">
@@ -5521,13 +5736,16 @@
         <v>74</v>
       </c>
       <c r="D22" s="99" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E22" s="62" t="s">
         <v>55</v>
       </c>
       <c r="F22" s="62" t="s">
         <v>55</v>
+      </c>
+      <c r="I22" s="118" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="23" spans="1:26">
@@ -5541,13 +5759,16 @@
         <v>75</v>
       </c>
       <c r="D23" s="99" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E23" s="62" t="s">
         <v>55</v>
       </c>
       <c r="F23" s="62" t="s">
         <v>55</v>
+      </c>
+      <c r="I23" s="118" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="24" spans="1:26" ht="15.75" customHeight="1">
@@ -5561,13 +5782,16 @@
         <v>76</v>
       </c>
       <c r="D24" s="99" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E24" s="62" t="s">
         <v>55</v>
       </c>
       <c r="F24" s="62" t="s">
         <v>55</v>
+      </c>
+      <c r="I24" s="118" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="25" spans="1:26" ht="15.75" customHeight="1">
@@ -5581,13 +5805,16 @@
         <v>79</v>
       </c>
       <c r="D25" s="99" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E25" s="62" t="s">
         <v>62</v>
       </c>
       <c r="F25" s="62" t="s">
         <v>62</v>
+      </c>
+      <c r="I25" s="118" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="26" spans="1:26" ht="15.75" customHeight="1">
@@ -5601,13 +5828,16 @@
         <v>83</v>
       </c>
       <c r="D26" s="99" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E26" s="62" t="s">
         <v>62</v>
       </c>
       <c r="F26" s="62" t="s">
         <v>62</v>
+      </c>
+      <c r="I26" s="118" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="27" spans="1:26" ht="15.75" customHeight="1">
@@ -5621,13 +5851,16 @@
         <v>84</v>
       </c>
       <c r="D27" s="99" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E27" s="62" t="s">
         <v>62</v>
       </c>
       <c r="F27" s="62" t="s">
         <v>62</v>
+      </c>
+      <c r="I27" s="118" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="28" spans="1:26" ht="15.75" customHeight="1">
@@ -5641,13 +5874,16 @@
         <v>87</v>
       </c>
       <c r="D28" s="99" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E28" s="62" t="s">
         <v>62</v>
       </c>
       <c r="F28" s="62" t="s">
         <v>62</v>
+      </c>
+      <c r="I28" s="118" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="29" spans="1:26" s="79" customFormat="1">
@@ -5669,7 +5905,9 @@
       <c r="F29" s="93" t="s">
         <v>210</v>
       </c>
-      <c r="I29" s="125"/>
+      <c r="I29" s="118" t="s">
+        <v>239</v>
+      </c>
     </row>
     <row r="30" spans="1:26" s="79" customFormat="1">
       <c r="A30" s="63">
@@ -5690,7 +5928,9 @@
       <c r="F30" s="93" t="s">
         <v>210</v>
       </c>
-      <c r="I30" s="125"/>
+      <c r="I30" s="118" t="s">
+        <v>239</v>
+      </c>
     </row>
     <row r="31" spans="1:26" s="79" customFormat="1">
       <c r="A31" s="63">
@@ -5711,7 +5951,9 @@
       <c r="F31" s="93" t="s">
         <v>210</v>
       </c>
-      <c r="I31" s="125"/>
+      <c r="I31" s="118" t="s">
+        <v>239</v>
+      </c>
     </row>
     <row r="32" spans="1:26" s="79" customFormat="1">
       <c r="A32" s="63">
@@ -5732,7 +5974,9 @@
       <c r="F32" s="93" t="s">
         <v>210</v>
       </c>
-      <c r="I32" s="125"/>
+      <c r="I32" s="118" t="s">
+        <v>239</v>
+      </c>
     </row>
     <row r="33" spans="1:26" s="133" customFormat="1" ht="15.75" customHeight="1">
       <c r="B33" s="134"/>
@@ -5780,7 +6024,7 @@
         <v>89</v>
       </c>
       <c r="D35" s="99" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E35" s="62" t="s">
         <v>27</v>
@@ -5803,13 +6047,16 @@
         <v>91</v>
       </c>
       <c r="D36" s="99" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E36" s="62" t="s">
         <v>27</v>
       </c>
       <c r="F36" s="62" t="s">
         <v>27</v>
+      </c>
+      <c r="I36" s="118" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="37" spans="1:26" ht="15.75" customHeight="1">
@@ -5823,7 +6070,7 @@
         <v>93</v>
       </c>
       <c r="D37" s="99" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E37" s="62" t="s">
         <v>55</v>
@@ -5833,7 +6080,9 @@
       </c>
       <c r="G37" s="126"/>
       <c r="H37" s="126"/>
-      <c r="I37" s="126"/>
+      <c r="I37" s="118" t="s">
+        <v>240</v>
+      </c>
       <c r="J37" s="126"/>
       <c r="K37" s="126"/>
       <c r="L37" s="126"/>
@@ -5863,7 +6112,7 @@
         <v>103</v>
       </c>
       <c r="D38" s="99" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E38" s="62" t="s">
         <v>55</v>
@@ -5873,7 +6122,9 @@
       </c>
       <c r="G38" s="126"/>
       <c r="H38" s="126"/>
-      <c r="I38" s="126"/>
+      <c r="I38" s="118" t="s">
+        <v>240</v>
+      </c>
       <c r="J38" s="126"/>
       <c r="K38" s="126"/>
       <c r="L38" s="126"/>
@@ -5903,7 +6154,7 @@
         <v>107</v>
       </c>
       <c r="D39" s="99" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E39" s="62" t="s">
         <v>55</v>
@@ -5913,7 +6164,9 @@
       </c>
       <c r="G39" s="126"/>
       <c r="H39" s="126"/>
-      <c r="I39" s="126"/>
+      <c r="I39" s="118" t="s">
+        <v>240</v>
+      </c>
       <c r="J39" s="126"/>
       <c r="K39" s="126"/>
       <c r="L39" s="126"/>
@@ -5943,7 +6196,7 @@
         <v>111</v>
       </c>
       <c r="D40" s="99" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E40" s="62" t="s">
         <v>55</v>
@@ -5953,7 +6206,9 @@
       </c>
       <c r="G40" s="126"/>
       <c r="H40" s="126"/>
-      <c r="I40" s="126"/>
+      <c r="I40" s="118" t="s">
+        <v>240</v>
+      </c>
       <c r="J40" s="126"/>
       <c r="K40" s="126"/>
       <c r="L40" s="126"/>
@@ -5983,13 +6238,16 @@
         <v>112</v>
       </c>
       <c r="D41" s="99" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E41" s="62" t="s">
         <v>62</v>
       </c>
       <c r="F41" s="62" t="s">
         <v>62</v>
+      </c>
+      <c r="I41" s="118" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="42" spans="1:26" ht="15.75" customHeight="1">
@@ -6003,13 +6261,16 @@
         <v>113</v>
       </c>
       <c r="D42" s="99" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E42" s="62" t="s">
         <v>62</v>
       </c>
       <c r="F42" s="62" t="s">
         <v>62</v>
+      </c>
+      <c r="I42" s="118" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="43" spans="1:26" ht="15.75" customHeight="1">
@@ -6023,13 +6284,16 @@
         <v>114</v>
       </c>
       <c r="D43" s="99" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E43" s="62" t="s">
         <v>62</v>
       </c>
       <c r="F43" s="62" t="s">
         <v>62</v>
+      </c>
+      <c r="I43" s="118" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="44" spans="1:26" ht="15.75" customHeight="1">
@@ -6043,13 +6307,16 @@
         <v>116</v>
       </c>
       <c r="D44" s="99" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E44" s="62" t="s">
         <v>62</v>
       </c>
       <c r="F44" s="62" t="s">
         <v>62</v>
+      </c>
+      <c r="I44" s="118" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="45" spans="1:26" s="79" customFormat="1">
@@ -7103,8 +7370,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A64" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView topLeftCell="A19" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50:XFD50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -7175,12 +7442,12 @@
     </row>
     <row r="2" spans="1:26" ht="19.5" customHeight="1">
       <c r="A2" s="7"/>
-      <c r="B2" s="141" t="s">
+      <c r="B2" s="135" t="s">
         <v>20</v>
       </c>
       <c r="C2" s="136"/>
       <c r="D2" s="136"/>
-      <c r="E2" s="142"/>
+      <c r="E2" s="137"/>
       <c r="F2" s="13"/>
       <c r="G2" s="15"/>
       <c r="H2" s="7"/>
@@ -7265,7 +7532,9 @@
         <v>52</v>
       </c>
       <c r="G5" s="22"/>
-      <c r="H5" s="22"/>
+      <c r="H5" s="58" t="s">
+        <v>30</v>
+      </c>
       <c r="I5" s="29" t="s">
         <v>26</v>
       </c>
@@ -7311,7 +7580,9 @@
       <c r="G6" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="H6" s="22"/>
+      <c r="H6" s="58" t="s">
+        <v>30</v>
+      </c>
       <c r="I6" s="29" t="s">
         <v>26</v>
       </c>
@@ -7359,7 +7630,9 @@
       <c r="G7" s="34" t="s">
         <v>97</v>
       </c>
-      <c r="H7" s="23"/>
+      <c r="H7" s="58" t="s">
+        <v>30</v>
+      </c>
       <c r="I7" s="16" t="s">
         <v>26</v>
       </c>
@@ -7392,7 +7665,9 @@
       <c r="G8" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="H8" s="14"/>
+      <c r="H8" s="58" t="s">
+        <v>30</v>
+      </c>
       <c r="I8" s="16" t="s">
         <v>26</v>
       </c>
@@ -7449,12 +7724,12 @@
     </row>
     <row r="11" spans="1:26">
       <c r="A11" s="8"/>
-      <c r="B11" s="143" t="s">
+      <c r="B11" s="138" t="s">
         <v>108</v>
       </c>
-      <c r="C11" s="144"/>
-      <c r="D11" s="144"/>
-      <c r="E11" s="145"/>
+      <c r="C11" s="139"/>
+      <c r="D11" s="139"/>
+      <c r="E11" s="140"/>
       <c r="F11" s="9"/>
       <c r="G11" s="9"/>
       <c r="H11" s="10"/>
@@ -7530,7 +7805,9 @@
       <c r="G13" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="H13" s="23"/>
+      <c r="H13" s="58" t="s">
+        <v>30</v>
+      </c>
       <c r="I13" s="16" t="s">
         <v>26</v>
       </c>
@@ -7558,7 +7835,9 @@
       <c r="G14" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="H14" s="23"/>
+      <c r="H14" s="58" t="s">
+        <v>30</v>
+      </c>
       <c r="I14" s="16" t="s">
         <v>26</v>
       </c>
@@ -7657,7 +7936,9 @@
         <v>52</v>
       </c>
       <c r="G18" s="22"/>
-      <c r="H18" s="22"/>
+      <c r="H18" s="58" t="s">
+        <v>30</v>
+      </c>
       <c r="I18" s="29" t="s">
         <v>26</v>
       </c>
@@ -7703,7 +7984,9 @@
       <c r="G19" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="H19" s="22"/>
+      <c r="H19" s="58" t="s">
+        <v>30</v>
+      </c>
       <c r="I19" s="29" t="s">
         <v>26</v>
       </c>
@@ -7751,7 +8034,9 @@
       <c r="G20" s="34" t="s">
         <v>97</v>
       </c>
-      <c r="H20" s="23"/>
+      <c r="H20" s="58" t="s">
+        <v>30</v>
+      </c>
       <c r="I20" s="16" t="s">
         <v>26</v>
       </c>
@@ -7808,12 +8093,12 @@
     </row>
     <row r="23" spans="1:26" ht="15.75" customHeight="1">
       <c r="A23" s="8"/>
-      <c r="B23" s="146" t="s">
+      <c r="B23" s="141" t="s">
         <v>131</v>
       </c>
-      <c r="C23" s="139"/>
-      <c r="D23" s="139"/>
-      <c r="E23" s="140"/>
+      <c r="C23" s="142"/>
+      <c r="D23" s="142"/>
+      <c r="E23" s="143"/>
       <c r="F23" s="9"/>
       <c r="G23" s="9"/>
       <c r="H23" s="10"/>
@@ -7898,7 +8183,9 @@
         <v>132</v>
       </c>
       <c r="G26" s="22"/>
-      <c r="H26" s="22"/>
+      <c r="H26" s="58" t="s">
+        <v>30</v>
+      </c>
       <c r="I26" s="29" t="s">
         <v>26</v>
       </c>
@@ -7944,7 +8231,9 @@
       <c r="G27" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="H27" s="22"/>
+      <c r="H27" s="58" t="s">
+        <v>30</v>
+      </c>
       <c r="I27" s="29" t="s">
         <v>26</v>
       </c>
@@ -7992,7 +8281,9 @@
       <c r="G28" s="34" t="s">
         <v>97</v>
       </c>
-      <c r="H28" s="23"/>
+      <c r="H28" s="58" t="s">
+        <v>30</v>
+      </c>
       <c r="I28" s="16" t="s">
         <v>26</v>
       </c>
@@ -8025,7 +8316,9 @@
       <c r="G29" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="H29" s="14"/>
+      <c r="H29" s="58" t="s">
+        <v>30</v>
+      </c>
       <c r="I29" s="16" t="s">
         <v>26</v>
       </c>
@@ -8082,12 +8375,12 @@
     </row>
     <row r="32" spans="1:26" ht="15.75" customHeight="1">
       <c r="A32" s="38"/>
-      <c r="B32" s="147" t="s">
+      <c r="B32" s="144" t="s">
         <v>133</v>
       </c>
       <c r="C32" s="136"/>
       <c r="D32" s="136"/>
-      <c r="E32" s="137"/>
+      <c r="E32" s="145"/>
       <c r="F32" s="39"/>
       <c r="G32" s="40"/>
       <c r="H32" s="17"/>
@@ -8163,7 +8456,9 @@
       <c r="G34" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="H34" s="23"/>
+      <c r="H34" s="58" t="s">
+        <v>30</v>
+      </c>
       <c r="I34" s="16" t="s">
         <v>26</v>
       </c>
@@ -8191,7 +8486,9 @@
       <c r="G35" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="H35" s="23"/>
+      <c r="H35" s="58" t="s">
+        <v>30</v>
+      </c>
       <c r="I35" s="16" t="s">
         <v>26</v>
       </c>
@@ -8290,7 +8587,9 @@
         <v>132</v>
       </c>
       <c r="G39" s="22"/>
-      <c r="H39" s="22"/>
+      <c r="H39" s="58" t="s">
+        <v>30</v>
+      </c>
       <c r="I39" s="29" t="s">
         <v>26</v>
       </c>
@@ -8336,7 +8635,9 @@
       <c r="G40" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="H40" s="22"/>
+      <c r="H40" s="58" t="s">
+        <v>30</v>
+      </c>
       <c r="I40" s="29" t="s">
         <v>26</v>
       </c>
@@ -8384,7 +8685,9 @@
       <c r="G41" s="34" t="s">
         <v>97</v>
       </c>
-      <c r="H41" s="23"/>
+      <c r="H41" s="58" t="s">
+        <v>30</v>
+      </c>
       <c r="I41" s="16" t="s">
         <v>26</v>
       </c>
@@ -8441,12 +8744,12 @@
     </row>
     <row r="44" spans="1:26" ht="15.75" customHeight="1">
       <c r="A44" s="8"/>
-      <c r="B44" s="138" t="s">
+      <c r="B44" s="147" t="s">
         <v>134</v>
       </c>
-      <c r="C44" s="139"/>
-      <c r="D44" s="139"/>
-      <c r="E44" s="140"/>
+      <c r="C44" s="142"/>
+      <c r="D44" s="142"/>
+      <c r="E44" s="143"/>
       <c r="F44" s="9"/>
       <c r="G44" s="9"/>
       <c r="H44" s="10"/>
@@ -8531,7 +8834,9 @@
         <v>52</v>
       </c>
       <c r="G47" s="22"/>
-      <c r="H47" s="22"/>
+      <c r="H47" s="58" t="s">
+        <v>30</v>
+      </c>
       <c r="I47" s="29" t="s">
         <v>26</v>
       </c>
@@ -8577,7 +8882,9 @@
       <c r="G48" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="H48" s="22"/>
+      <c r="H48" s="58" t="s">
+        <v>30</v>
+      </c>
       <c r="I48" s="29" t="s">
         <v>26</v>
       </c>
@@ -8625,7 +8932,9 @@
       <c r="G49" s="34" t="s">
         <v>97</v>
       </c>
-      <c r="H49" s="23"/>
+      <c r="H49" s="58" t="s">
+        <v>30</v>
+      </c>
       <c r="I49" s="16" t="s">
         <v>26</v>
       </c>
@@ -8636,36 +8945,38 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A50" s="19" t="s">
+    <row r="50" spans="1:26" s="163" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A50" s="155" t="s">
         <v>135</v>
       </c>
-      <c r="B50" s="2">
+      <c r="B50" s="156">
         <v>19</v>
       </c>
-      <c r="C50" s="11" t="s">
+      <c r="C50" s="157" t="s">
         <v>98</v>
       </c>
-      <c r="D50" s="12" t="s">
+      <c r="D50" s="158" t="s">
         <v>99</v>
       </c>
-      <c r="E50" s="14" t="s">
+      <c r="E50" s="159" t="s">
         <v>101</v>
       </c>
-      <c r="F50" s="11" t="s">
+      <c r="F50" s="157" t="s">
         <v>102</v>
       </c>
-      <c r="G50" s="6">
-        <v>0</v>
-      </c>
-      <c r="H50" s="14"/>
-      <c r="I50" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="J50" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="L50">
+      <c r="G50" s="160" t="s">
+        <v>82</v>
+      </c>
+      <c r="H50" s="161" t="s">
+        <v>30</v>
+      </c>
+      <c r="I50" s="162" t="s">
+        <v>26</v>
+      </c>
+      <c r="J50" s="160" t="s">
+        <v>30</v>
+      </c>
+      <c r="L50" s="163">
         <v>0</v>
       </c>
     </row>
@@ -8715,12 +9026,12 @@
     </row>
     <row r="53" spans="1:26" ht="15.75" customHeight="1">
       <c r="A53" s="8"/>
-      <c r="B53" s="138" t="s">
+      <c r="B53" s="147" t="s">
         <v>136</v>
       </c>
-      <c r="C53" s="139"/>
-      <c r="D53" s="139"/>
-      <c r="E53" s="140"/>
+      <c r="C53" s="142"/>
+      <c r="D53" s="142"/>
+      <c r="E53" s="143"/>
       <c r="F53" s="9"/>
       <c r="G53" s="9"/>
       <c r="H53" s="10"/>
@@ -8796,7 +9107,9 @@
       <c r="G55" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="H55" s="23"/>
+      <c r="H55" s="58" t="s">
+        <v>30</v>
+      </c>
       <c r="I55" s="16" t="s">
         <v>26</v>
       </c>
@@ -8824,7 +9137,9 @@
       <c r="G56" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="H56" s="23"/>
+      <c r="H56" s="58" t="s">
+        <v>30</v>
+      </c>
       <c r="I56" s="16" t="s">
         <v>26</v>
       </c>
@@ -8923,7 +9238,9 @@
         <v>52</v>
       </c>
       <c r="G60" s="22"/>
-      <c r="H60" s="22"/>
+      <c r="H60" s="58" t="s">
+        <v>30</v>
+      </c>
       <c r="I60" s="29" t="s">
         <v>26</v>
       </c>
@@ -8969,7 +9286,9 @@
       <c r="G61" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="H61" s="22"/>
+      <c r="H61" s="58" t="s">
+        <v>30</v>
+      </c>
       <c r="I61" s="29" t="s">
         <v>26</v>
       </c>
@@ -9017,7 +9336,9 @@
       <c r="G62" s="34" t="s">
         <v>97</v>
       </c>
-      <c r="H62" s="23"/>
+      <c r="H62" s="58" t="s">
+        <v>30</v>
+      </c>
       <c r="I62" s="16" t="s">
         <v>26</v>
       </c>
@@ -9074,12 +9395,12 @@
     </row>
     <row r="65" spans="1:26" ht="15.75" customHeight="1">
       <c r="A65" s="8"/>
-      <c r="B65" s="138" t="s">
+      <c r="B65" s="147" t="s">
         <v>138</v>
       </c>
-      <c r="C65" s="139"/>
-      <c r="D65" s="139"/>
-      <c r="E65" s="140"/>
+      <c r="C65" s="142"/>
+      <c r="D65" s="142"/>
+      <c r="E65" s="143"/>
       <c r="F65" s="9"/>
       <c r="G65" s="9"/>
       <c r="H65" s="10"/>
@@ -9157,7 +9478,9 @@
       <c r="G67" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="H67" s="23"/>
+      <c r="H67" s="58" t="s">
+        <v>30</v>
+      </c>
       <c r="I67" s="16" t="s">
         <v>26</v>
       </c>
@@ -9187,7 +9510,9 @@
       <c r="G68" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="H68" s="23"/>
+      <c r="H68" s="58" t="s">
+        <v>30</v>
+      </c>
       <c r="I68" s="16" t="s">
         <v>26</v>
       </c>
@@ -9314,7 +9639,9 @@
         <v>52</v>
       </c>
       <c r="G73" s="22"/>
-      <c r="H73" s="22"/>
+      <c r="H73" s="58" t="s">
+        <v>30</v>
+      </c>
       <c r="I73" s="29" t="s">
         <v>26</v>
       </c>
@@ -9360,7 +9687,9 @@
       <c r="G74" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="H74" s="22"/>
+      <c r="H74" s="58" t="s">
+        <v>30</v>
+      </c>
       <c r="I74" s="29" t="s">
         <v>26</v>
       </c>
@@ -9408,7 +9737,9 @@
       <c r="G75" t="s">
         <v>146</v>
       </c>
-      <c r="H75" s="23"/>
+      <c r="H75" s="58" t="s">
+        <v>30</v>
+      </c>
       <c r="I75" s="16" t="s">
         <v>26</v>
       </c>
@@ -9469,12 +9800,12 @@
     </row>
     <row r="78" spans="1:26" ht="15.75" customHeight="1">
       <c r="A78" s="8"/>
-      <c r="B78" s="138" t="s">
+      <c r="B78" s="147" t="s">
         <v>147</v>
       </c>
-      <c r="C78" s="139"/>
-      <c r="D78" s="139"/>
-      <c r="E78" s="140"/>
+      <c r="C78" s="142"/>
+      <c r="D78" s="142"/>
+      <c r="E78" s="143"/>
       <c r="F78" s="9"/>
       <c r="G78" s="9"/>
       <c r="H78" s="10"/>
@@ -9552,7 +9883,9 @@
       <c r="G80" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="H80" s="23"/>
+      <c r="H80" s="58" t="s">
+        <v>30</v>
+      </c>
       <c r="I80" s="16" t="s">
         <v>26</v>
       </c>
@@ -9582,7 +9915,9 @@
       <c r="G81" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="H81" s="23"/>
+      <c r="H81" s="58" t="s">
+        <v>30</v>
+      </c>
       <c r="I81" s="16" t="s">
         <v>26</v>
       </c>
@@ -9709,7 +10044,9 @@
         <v>52</v>
       </c>
       <c r="G86" s="22"/>
-      <c r="H86" s="22"/>
+      <c r="H86" s="58" t="s">
+        <v>30</v>
+      </c>
       <c r="I86" s="29" t="s">
         <v>26</v>
       </c>
@@ -9755,7 +10092,9 @@
       <c r="G87" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="H87" s="22"/>
+      <c r="H87" s="58" t="s">
+        <v>30</v>
+      </c>
       <c r="I87" s="29" t="s">
         <v>26</v>
       </c>
@@ -9803,7 +10142,9 @@
       <c r="G88" t="s">
         <v>151</v>
       </c>
-      <c r="H88" s="23"/>
+      <c r="H88" s="58" t="s">
+        <v>30</v>
+      </c>
       <c r="I88" s="16" t="s">
         <v>26</v>
       </c>
@@ -9864,11 +10205,11 @@
     </row>
     <row r="91" spans="1:26" ht="15.75" customHeight="1">
       <c r="A91" s="55"/>
-      <c r="B91" s="135" t="s">
+      <c r="B91" s="146" t="s">
         <v>152</v>
       </c>
       <c r="C91" s="136"/>
-      <c r="D91" s="137"/>
+      <c r="D91" s="145"/>
       <c r="E91" s="56"/>
       <c r="F91" s="56"/>
       <c r="G91" s="56"/>
@@ -9947,7 +10288,9 @@
       <c r="G93" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="H93" s="23"/>
+      <c r="H93" s="58" t="s">
+        <v>30</v>
+      </c>
       <c r="I93" s="16" t="s">
         <v>26</v>
       </c>
@@ -9977,7 +10320,9 @@
       <c r="G94" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="H94" s="23"/>
+      <c r="H94" s="58" t="s">
+        <v>30</v>
+      </c>
       <c r="I94" s="16" t="s">
         <v>26</v>
       </c>
@@ -10104,7 +10449,9 @@
         <v>132</v>
       </c>
       <c r="G99" s="22"/>
-      <c r="H99" s="22"/>
+      <c r="H99" s="58" t="s">
+        <v>30</v>
+      </c>
       <c r="I99" s="29" t="s">
         <v>26</v>
       </c>
@@ -10150,7 +10497,9 @@
       <c r="G100" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="H100" s="22"/>
+      <c r="H100" s="58" t="s">
+        <v>30</v>
+      </c>
       <c r="I100" s="29" t="s">
         <v>26</v>
       </c>
@@ -10198,7 +10547,9 @@
       <c r="G101" t="s">
         <v>146</v>
       </c>
-      <c r="H101" s="23"/>
+      <c r="H101" s="58" t="s">
+        <v>30</v>
+      </c>
       <c r="I101" s="16" t="s">
         <v>26</v>
       </c>
@@ -10259,11 +10610,11 @@
     </row>
     <row r="104" spans="1:26" ht="15.75" customHeight="1">
       <c r="A104" s="55"/>
-      <c r="B104" s="135" t="s">
+      <c r="B104" s="146" t="s">
         <v>154</v>
       </c>
       <c r="C104" s="136"/>
-      <c r="D104" s="137"/>
+      <c r="D104" s="145"/>
       <c r="E104" s="56"/>
       <c r="F104" s="56"/>
       <c r="G104" s="56"/>
@@ -10342,7 +10693,9 @@
       <c r="G106" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="H106" s="23"/>
+      <c r="H106" s="58" t="s">
+        <v>30</v>
+      </c>
       <c r="I106" s="16" t="s">
         <v>26</v>
       </c>
@@ -10372,7 +10725,9 @@
       <c r="G107" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="H107" s="23"/>
+      <c r="H107" s="58" t="s">
+        <v>30</v>
+      </c>
       <c r="I107" s="16" t="s">
         <v>26</v>
       </c>
@@ -10499,7 +10854,9 @@
         <v>52</v>
       </c>
       <c r="G112" s="22"/>
-      <c r="H112" s="22"/>
+      <c r="H112" s="58" t="s">
+        <v>30</v>
+      </c>
       <c r="I112" s="29" t="s">
         <v>26</v>
       </c>
@@ -10545,7 +10902,9 @@
       <c r="G113" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="H113" s="22"/>
+      <c r="H113" s="58" t="s">
+        <v>30</v>
+      </c>
       <c r="I113" s="29" t="s">
         <v>26</v>
       </c>
@@ -10593,7 +10952,9 @@
       <c r="G114" t="s">
         <v>146</v>
       </c>
-      <c r="H114" s="23"/>
+      <c r="H114" s="58" t="s">
+        <v>30</v>
+      </c>
       <c r="I114" s="16" t="s">
         <v>26</v>
       </c>
@@ -10654,11 +11015,11 @@
     </row>
     <row r="117" spans="1:26" ht="15.75" customHeight="1">
       <c r="A117" s="55"/>
-      <c r="B117" s="135" t="s">
+      <c r="B117" s="146" t="s">
         <v>155</v>
       </c>
       <c r="C117" s="136"/>
-      <c r="D117" s="137"/>
+      <c r="D117" s="145"/>
       <c r="E117" s="56"/>
       <c r="F117" s="56"/>
       <c r="G117" s="56"/>
@@ -10737,7 +11098,9 @@
       <c r="G119" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="H119" s="23"/>
+      <c r="H119" s="58" t="s">
+        <v>30</v>
+      </c>
       <c r="I119" s="16" t="s">
         <v>26</v>
       </c>
@@ -10767,7 +11130,9 @@
       <c r="G120" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="H120" s="23"/>
+      <c r="H120" s="58" t="s">
+        <v>30</v>
+      </c>
       <c r="I120" s="16" t="s">
         <v>26</v>
       </c>
@@ -10894,7 +11259,9 @@
         <v>132</v>
       </c>
       <c r="G125" s="22"/>
-      <c r="H125" s="22"/>
+      <c r="H125" s="58" t="s">
+        <v>30</v>
+      </c>
       <c r="I125" s="29" t="s">
         <v>26</v>
       </c>
@@ -10940,7 +11307,9 @@
       <c r="G126" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="H126" s="22"/>
+      <c r="H126" s="58" t="s">
+        <v>30</v>
+      </c>
       <c r="I126" s="29" t="s">
         <v>26</v>
       </c>
@@ -10988,7 +11357,9 @@
       <c r="G127" t="s">
         <v>151</v>
       </c>
-      <c r="H127" s="23"/>
+      <c r="H127" s="58" t="s">
+        <v>30</v>
+      </c>
       <c r="I127" s="16" t="s">
         <v>26</v>
       </c>
@@ -11049,11 +11420,11 @@
     </row>
     <row r="130" spans="1:26" ht="15.75" customHeight="1">
       <c r="A130" s="55"/>
-      <c r="B130" s="135" t="s">
+      <c r="B130" s="146" t="s">
         <v>156</v>
       </c>
       <c r="C130" s="136"/>
-      <c r="D130" s="137"/>
+      <c r="D130" s="145"/>
       <c r="E130" s="56"/>
       <c r="F130" s="56"/>
       <c r="G130" s="56"/>
@@ -11132,7 +11503,9 @@
       <c r="G132" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="H132" s="23"/>
+      <c r="H132" s="58" t="s">
+        <v>30</v>
+      </c>
       <c r="I132" s="16" t="s">
         <v>26</v>
       </c>
@@ -11162,7 +11535,9 @@
       <c r="G133" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="H133" s="23"/>
+      <c r="H133" s="58" t="s">
+        <v>30</v>
+      </c>
       <c r="I133" s="16" t="s">
         <v>26</v>
       </c>
@@ -11289,7 +11664,9 @@
         <v>52</v>
       </c>
       <c r="G138" s="22"/>
-      <c r="H138" s="22"/>
+      <c r="H138" s="58" t="s">
+        <v>30</v>
+      </c>
       <c r="I138" s="29" t="s">
         <v>26</v>
       </c>
@@ -11335,7 +11712,9 @@
       <c r="G139" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="H139" s="22"/>
+      <c r="H139" s="58" t="s">
+        <v>30</v>
+      </c>
       <c r="I139" s="29" t="s">
         <v>26</v>
       </c>
@@ -11383,7 +11762,9 @@
       <c r="G140" t="s">
         <v>151</v>
       </c>
-      <c r="H140" s="23"/>
+      <c r="H140" s="58" t="s">
+        <v>30</v>
+      </c>
       <c r="I140" s="16" t="s">
         <v>26</v>
       </c>
@@ -14876,11 +15257,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="B32:E32"/>
-    <mergeCell ref="B104:D104"/>
     <mergeCell ref="B117:D117"/>
     <mergeCell ref="B130:D130"/>
     <mergeCell ref="B44:E44"/>
@@ -14888,1139 +15264,1378 @@
     <mergeCell ref="B78:E78"/>
     <mergeCell ref="B65:E65"/>
     <mergeCell ref="B53:E53"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="B32:E32"/>
+    <mergeCell ref="B104:D104"/>
   </mergeCells>
   <conditionalFormatting sqref="H3">
-    <cfRule type="cellIs" dxfId="398" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="419" priority="22" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3">
-    <cfRule type="cellIs" dxfId="397" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="418" priority="23" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3">
-    <cfRule type="cellIs" dxfId="396" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="417" priority="24" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16">
-    <cfRule type="cellIs" dxfId="395" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="416" priority="25" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16">
-    <cfRule type="cellIs" dxfId="394" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="415" priority="26" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16">
-    <cfRule type="cellIs" dxfId="393" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="414" priority="27" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4">
-    <cfRule type="cellIs" dxfId="392" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="413" priority="28" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4">
-    <cfRule type="cellIs" dxfId="391" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="412" priority="29" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4">
-    <cfRule type="cellIs" dxfId="390" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="411" priority="30" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H17">
-    <cfRule type="cellIs" dxfId="389" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="410" priority="31" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H17">
-    <cfRule type="cellIs" dxfId="388" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="409" priority="32" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H17">
-    <cfRule type="cellIs" dxfId="387" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="408" priority="33" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10">
-    <cfRule type="cellIs" dxfId="386" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="407" priority="34" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10">
-    <cfRule type="cellIs" dxfId="385" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="406" priority="35" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10">
-    <cfRule type="cellIs" dxfId="384" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="405" priority="36" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H22">
-    <cfRule type="cellIs" dxfId="383" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="404" priority="37" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H22">
-    <cfRule type="cellIs" dxfId="382" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="403" priority="38" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H22">
-    <cfRule type="cellIs" dxfId="381" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="402" priority="39" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12">
-    <cfRule type="cellIs" dxfId="380" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="401" priority="40" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12">
-    <cfRule type="cellIs" dxfId="379" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="400" priority="41" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12">
-    <cfRule type="cellIs" dxfId="378" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="399" priority="42" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H15">
-    <cfRule type="cellIs" dxfId="377" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="398" priority="43" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H15">
-    <cfRule type="cellIs" dxfId="376" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="397" priority="44" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H15">
-    <cfRule type="cellIs" dxfId="375" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="396" priority="45" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H21">
-    <cfRule type="cellIs" dxfId="374" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="395" priority="46" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H21">
-    <cfRule type="cellIs" dxfId="373" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="394" priority="47" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H21">
-    <cfRule type="cellIs" dxfId="372" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="393" priority="48" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9">
-    <cfRule type="cellIs" dxfId="371" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="392" priority="49" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9">
-    <cfRule type="cellIs" dxfId="370" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="391" priority="50" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9">
-    <cfRule type="cellIs" dxfId="369" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="390" priority="51" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H24">
-    <cfRule type="cellIs" dxfId="368" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="389" priority="52" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H24">
-    <cfRule type="cellIs" dxfId="367" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="388" priority="53" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H24">
-    <cfRule type="cellIs" dxfId="366" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="387" priority="54" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H25">
-    <cfRule type="cellIs" dxfId="365" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="386" priority="55" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H25">
-    <cfRule type="cellIs" dxfId="364" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="385" priority="56" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H25">
-    <cfRule type="cellIs" dxfId="363" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="384" priority="57" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H31:H32">
-    <cfRule type="cellIs" dxfId="362" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="383" priority="58" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H31:H32">
-    <cfRule type="cellIs" dxfId="361" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="382" priority="59" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H31:H32">
-    <cfRule type="cellIs" dxfId="360" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="381" priority="60" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H30">
-    <cfRule type="cellIs" dxfId="359" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="380" priority="61" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H30">
-    <cfRule type="cellIs" dxfId="358" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="379" priority="62" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H30">
-    <cfRule type="cellIs" dxfId="357" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="378" priority="63" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H45">
-    <cfRule type="cellIs" dxfId="356" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="377" priority="64" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H45">
-    <cfRule type="cellIs" dxfId="355" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="376" priority="65" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H45">
-    <cfRule type="cellIs" dxfId="354" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="375" priority="66" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H46">
-    <cfRule type="cellIs" dxfId="353" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="374" priority="67" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H46">
-    <cfRule type="cellIs" dxfId="352" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="373" priority="68" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H46">
-    <cfRule type="cellIs" dxfId="351" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="372" priority="69" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H52">
-    <cfRule type="cellIs" dxfId="350" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="371" priority="70" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H52">
-    <cfRule type="cellIs" dxfId="349" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="370" priority="71" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H52">
-    <cfRule type="cellIs" dxfId="348" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="369" priority="72" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H51">
-    <cfRule type="cellIs" dxfId="347" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="368" priority="73" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H51">
-    <cfRule type="cellIs" dxfId="346" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="367" priority="74" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H51">
-    <cfRule type="cellIs" dxfId="345" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="366" priority="75" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H37">
-    <cfRule type="cellIs" dxfId="344" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="365" priority="76" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H37">
-    <cfRule type="cellIs" dxfId="343" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="364" priority="77" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H37">
-    <cfRule type="cellIs" dxfId="342" priority="57" operator="equal">
+    <cfRule type="cellIs" dxfId="363" priority="78" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H38">
-    <cfRule type="cellIs" dxfId="341" priority="58" operator="equal">
+    <cfRule type="cellIs" dxfId="362" priority="79" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H38">
-    <cfRule type="cellIs" dxfId="340" priority="59" operator="equal">
+    <cfRule type="cellIs" dxfId="361" priority="80" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H38">
-    <cfRule type="cellIs" dxfId="339" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="360" priority="81" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H43">
-    <cfRule type="cellIs" dxfId="338" priority="61" operator="equal">
+    <cfRule type="cellIs" dxfId="359" priority="82" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H43">
-    <cfRule type="cellIs" dxfId="337" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="358" priority="83" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H43">
-    <cfRule type="cellIs" dxfId="336" priority="63" operator="equal">
+    <cfRule type="cellIs" dxfId="357" priority="84" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H33">
-    <cfRule type="cellIs" dxfId="335" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="356" priority="85" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H33">
-    <cfRule type="cellIs" dxfId="334" priority="65" operator="equal">
+    <cfRule type="cellIs" dxfId="355" priority="86" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H33">
-    <cfRule type="cellIs" dxfId="333" priority="66" operator="equal">
+    <cfRule type="cellIs" dxfId="354" priority="87" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H36">
-    <cfRule type="cellIs" dxfId="332" priority="67" operator="equal">
+    <cfRule type="cellIs" dxfId="353" priority="88" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H36">
-    <cfRule type="cellIs" dxfId="331" priority="68" operator="equal">
+    <cfRule type="cellIs" dxfId="352" priority="89" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H36">
-    <cfRule type="cellIs" dxfId="330" priority="69" operator="equal">
+    <cfRule type="cellIs" dxfId="351" priority="90" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H42">
-    <cfRule type="cellIs" dxfId="329" priority="70" operator="equal">
+    <cfRule type="cellIs" dxfId="350" priority="91" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H42">
-    <cfRule type="cellIs" dxfId="328" priority="71" operator="equal">
+    <cfRule type="cellIs" dxfId="349" priority="92" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H42">
-    <cfRule type="cellIs" dxfId="327" priority="72" operator="equal">
+    <cfRule type="cellIs" dxfId="348" priority="93" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H58">
-    <cfRule type="cellIs" dxfId="326" priority="73" operator="equal">
+    <cfRule type="cellIs" dxfId="347" priority="94" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H58">
-    <cfRule type="cellIs" dxfId="325" priority="74" operator="equal">
+    <cfRule type="cellIs" dxfId="346" priority="95" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H58">
-    <cfRule type="cellIs" dxfId="324" priority="75" operator="equal">
+    <cfRule type="cellIs" dxfId="345" priority="96" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H59">
-    <cfRule type="cellIs" dxfId="323" priority="76" operator="equal">
+    <cfRule type="cellIs" dxfId="344" priority="97" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H59">
-    <cfRule type="cellIs" dxfId="322" priority="77" operator="equal">
+    <cfRule type="cellIs" dxfId="343" priority="98" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H59">
-    <cfRule type="cellIs" dxfId="321" priority="78" operator="equal">
+    <cfRule type="cellIs" dxfId="342" priority="99" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H64">
-    <cfRule type="cellIs" dxfId="320" priority="79" operator="equal">
+    <cfRule type="cellIs" dxfId="341" priority="100" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H64">
-    <cfRule type="cellIs" dxfId="319" priority="80" operator="equal">
+    <cfRule type="cellIs" dxfId="340" priority="101" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H64">
-    <cfRule type="cellIs" dxfId="318" priority="81" operator="equal">
+    <cfRule type="cellIs" dxfId="339" priority="102" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H54">
-    <cfRule type="cellIs" dxfId="317" priority="82" operator="equal">
+    <cfRule type="cellIs" dxfId="338" priority="103" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H54">
-    <cfRule type="cellIs" dxfId="316" priority="83" operator="equal">
+    <cfRule type="cellIs" dxfId="337" priority="104" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H54">
-    <cfRule type="cellIs" dxfId="315" priority="84" operator="equal">
+    <cfRule type="cellIs" dxfId="336" priority="105" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H57">
-    <cfRule type="cellIs" dxfId="314" priority="85" operator="equal">
+    <cfRule type="cellIs" dxfId="335" priority="106" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H57">
-    <cfRule type="cellIs" dxfId="313" priority="86" operator="equal">
+    <cfRule type="cellIs" dxfId="334" priority="107" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H57">
-    <cfRule type="cellIs" dxfId="312" priority="87" operator="equal">
+    <cfRule type="cellIs" dxfId="333" priority="108" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H63">
-    <cfRule type="cellIs" dxfId="311" priority="88" operator="equal">
+    <cfRule type="cellIs" dxfId="332" priority="109" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H63">
-    <cfRule type="cellIs" dxfId="310" priority="89" operator="equal">
+    <cfRule type="cellIs" dxfId="331" priority="110" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H63">
-    <cfRule type="cellIs" dxfId="309" priority="90" operator="equal">
+    <cfRule type="cellIs" dxfId="330" priority="111" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H70">
-    <cfRule type="cellIs" dxfId="308" priority="91" operator="equal">
+    <cfRule type="cellIs" dxfId="329" priority="112" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H70">
-    <cfRule type="cellIs" dxfId="307" priority="92" operator="equal">
+    <cfRule type="cellIs" dxfId="328" priority="113" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H70">
-    <cfRule type="cellIs" dxfId="306" priority="93" operator="equal">
+    <cfRule type="cellIs" dxfId="327" priority="114" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H66">
-    <cfRule type="cellIs" dxfId="305" priority="94" operator="equal">
+    <cfRule type="cellIs" dxfId="326" priority="115" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H66">
-    <cfRule type="cellIs" dxfId="304" priority="95" operator="equal">
+    <cfRule type="cellIs" dxfId="325" priority="116" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H66">
-    <cfRule type="cellIs" dxfId="303" priority="96" operator="equal">
+    <cfRule type="cellIs" dxfId="324" priority="117" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H69">
-    <cfRule type="cellIs" dxfId="302" priority="97" operator="equal">
+    <cfRule type="cellIs" dxfId="323" priority="118" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H69">
-    <cfRule type="cellIs" dxfId="301" priority="98" operator="equal">
+    <cfRule type="cellIs" dxfId="322" priority="119" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H69">
-    <cfRule type="cellIs" dxfId="300" priority="99" operator="equal">
+    <cfRule type="cellIs" dxfId="321" priority="120" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H72">
-    <cfRule type="cellIs" dxfId="299" priority="100" operator="equal">
+    <cfRule type="cellIs" dxfId="320" priority="121" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H72">
-    <cfRule type="cellIs" dxfId="298" priority="101" operator="equal">
+    <cfRule type="cellIs" dxfId="319" priority="122" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H72">
-    <cfRule type="cellIs" dxfId="297" priority="102" operator="equal">
+    <cfRule type="cellIs" dxfId="318" priority="123" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H77">
-    <cfRule type="cellIs" dxfId="296" priority="103" operator="equal">
+    <cfRule type="cellIs" dxfId="317" priority="124" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H77">
-    <cfRule type="cellIs" dxfId="295" priority="104" operator="equal">
+    <cfRule type="cellIs" dxfId="316" priority="125" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H77">
-    <cfRule type="cellIs" dxfId="294" priority="105" operator="equal">
+    <cfRule type="cellIs" dxfId="315" priority="126" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H76">
-    <cfRule type="cellIs" dxfId="293" priority="106" operator="equal">
+    <cfRule type="cellIs" dxfId="314" priority="127" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H76">
-    <cfRule type="cellIs" dxfId="292" priority="107" operator="equal">
+    <cfRule type="cellIs" dxfId="313" priority="128" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H76">
-    <cfRule type="cellIs" dxfId="291" priority="108" operator="equal">
+    <cfRule type="cellIs" dxfId="312" priority="129" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H83">
-    <cfRule type="cellIs" dxfId="290" priority="109" operator="equal">
+    <cfRule type="cellIs" dxfId="311" priority="130" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H83">
-    <cfRule type="cellIs" dxfId="289" priority="110" operator="equal">
+    <cfRule type="cellIs" dxfId="310" priority="131" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H83">
-    <cfRule type="cellIs" dxfId="288" priority="111" operator="equal">
+    <cfRule type="cellIs" dxfId="309" priority="132" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H79">
-    <cfRule type="cellIs" dxfId="287" priority="112" operator="equal">
+    <cfRule type="cellIs" dxfId="308" priority="133" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H79">
-    <cfRule type="cellIs" dxfId="286" priority="113" operator="equal">
+    <cfRule type="cellIs" dxfId="307" priority="134" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H79">
-    <cfRule type="cellIs" dxfId="285" priority="114" operator="equal">
+    <cfRule type="cellIs" dxfId="306" priority="135" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H82">
-    <cfRule type="cellIs" dxfId="284" priority="115" operator="equal">
+    <cfRule type="cellIs" dxfId="305" priority="136" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H82">
-    <cfRule type="cellIs" dxfId="283" priority="116" operator="equal">
+    <cfRule type="cellIs" dxfId="304" priority="137" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H82">
-    <cfRule type="cellIs" dxfId="282" priority="117" operator="equal">
+    <cfRule type="cellIs" dxfId="303" priority="138" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H85">
-    <cfRule type="cellIs" dxfId="281" priority="118" operator="equal">
+    <cfRule type="cellIs" dxfId="302" priority="139" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H85">
-    <cfRule type="cellIs" dxfId="280" priority="119" operator="equal">
+    <cfRule type="cellIs" dxfId="301" priority="140" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H85">
-    <cfRule type="cellIs" dxfId="279" priority="120" operator="equal">
+    <cfRule type="cellIs" dxfId="300" priority="141" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H90">
-    <cfRule type="cellIs" dxfId="278" priority="121" operator="equal">
+    <cfRule type="cellIs" dxfId="299" priority="142" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H90">
-    <cfRule type="cellIs" dxfId="277" priority="122" operator="equal">
+    <cfRule type="cellIs" dxfId="298" priority="143" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H90">
-    <cfRule type="cellIs" dxfId="276" priority="123" operator="equal">
+    <cfRule type="cellIs" dxfId="297" priority="144" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H89">
-    <cfRule type="cellIs" dxfId="275" priority="124" operator="equal">
+    <cfRule type="cellIs" dxfId="296" priority="145" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H89">
-    <cfRule type="cellIs" dxfId="274" priority="125" operator="equal">
+    <cfRule type="cellIs" dxfId="295" priority="146" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H89">
-    <cfRule type="cellIs" dxfId="273" priority="126" operator="equal">
+    <cfRule type="cellIs" dxfId="294" priority="147" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H71">
-    <cfRule type="cellIs" dxfId="272" priority="127" operator="equal">
+    <cfRule type="cellIs" dxfId="293" priority="148" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H71">
-    <cfRule type="cellIs" dxfId="271" priority="128" operator="equal">
+    <cfRule type="cellIs" dxfId="292" priority="149" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H71">
-    <cfRule type="cellIs" dxfId="270" priority="129" operator="equal">
+    <cfRule type="cellIs" dxfId="291" priority="150" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H84">
-    <cfRule type="cellIs" dxfId="269" priority="130" operator="equal">
+    <cfRule type="cellIs" dxfId="290" priority="151" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H84">
-    <cfRule type="cellIs" dxfId="268" priority="131" operator="equal">
+    <cfRule type="cellIs" dxfId="289" priority="152" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H84">
-    <cfRule type="cellIs" dxfId="267" priority="132" operator="equal">
+    <cfRule type="cellIs" dxfId="288" priority="153" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H96">
-    <cfRule type="cellIs" dxfId="266" priority="133" operator="equal">
+    <cfRule type="cellIs" dxfId="287" priority="154" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H96">
-    <cfRule type="cellIs" dxfId="265" priority="134" operator="equal">
+    <cfRule type="cellIs" dxfId="286" priority="155" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H96">
-    <cfRule type="cellIs" dxfId="264" priority="135" operator="equal">
+    <cfRule type="cellIs" dxfId="285" priority="156" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H92">
-    <cfRule type="cellIs" dxfId="263" priority="136" operator="equal">
+    <cfRule type="cellIs" dxfId="284" priority="157" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H92">
-    <cfRule type="cellIs" dxfId="262" priority="137" operator="equal">
+    <cfRule type="cellIs" dxfId="283" priority="158" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H92">
-    <cfRule type="cellIs" dxfId="261" priority="138" operator="equal">
+    <cfRule type="cellIs" dxfId="282" priority="159" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H95">
-    <cfRule type="cellIs" dxfId="260" priority="139" operator="equal">
+    <cfRule type="cellIs" dxfId="281" priority="160" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H95">
-    <cfRule type="cellIs" dxfId="259" priority="140" operator="equal">
+    <cfRule type="cellIs" dxfId="280" priority="161" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H95">
-    <cfRule type="cellIs" dxfId="258" priority="141" operator="equal">
+    <cfRule type="cellIs" dxfId="279" priority="162" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H98">
-    <cfRule type="cellIs" dxfId="257" priority="142" operator="equal">
+    <cfRule type="cellIs" dxfId="278" priority="163" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H98">
-    <cfRule type="cellIs" dxfId="256" priority="143" operator="equal">
+    <cfRule type="cellIs" dxfId="277" priority="164" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H98">
-    <cfRule type="cellIs" dxfId="255" priority="144" operator="equal">
+    <cfRule type="cellIs" dxfId="276" priority="165" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H103">
-    <cfRule type="cellIs" dxfId="254" priority="145" operator="equal">
+    <cfRule type="cellIs" dxfId="275" priority="166" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H103">
-    <cfRule type="cellIs" dxfId="253" priority="146" operator="equal">
+    <cfRule type="cellIs" dxfId="274" priority="167" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H103">
-    <cfRule type="cellIs" dxfId="252" priority="147" operator="equal">
+    <cfRule type="cellIs" dxfId="273" priority="168" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H102">
-    <cfRule type="cellIs" dxfId="251" priority="148" operator="equal">
+    <cfRule type="cellIs" dxfId="272" priority="169" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H102">
-    <cfRule type="cellIs" dxfId="250" priority="149" operator="equal">
+    <cfRule type="cellIs" dxfId="271" priority="170" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H102">
-    <cfRule type="cellIs" dxfId="249" priority="150" operator="equal">
+    <cfRule type="cellIs" dxfId="270" priority="171" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H97">
-    <cfRule type="cellIs" dxfId="248" priority="151" operator="equal">
+    <cfRule type="cellIs" dxfId="269" priority="172" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H97">
-    <cfRule type="cellIs" dxfId="247" priority="152" operator="equal">
+    <cfRule type="cellIs" dxfId="268" priority="173" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H97">
-    <cfRule type="cellIs" dxfId="246" priority="153" operator="equal">
+    <cfRule type="cellIs" dxfId="267" priority="174" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H109">
-    <cfRule type="cellIs" dxfId="245" priority="154" operator="equal">
+    <cfRule type="cellIs" dxfId="266" priority="175" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H109">
-    <cfRule type="cellIs" dxfId="244" priority="155" operator="equal">
+    <cfRule type="cellIs" dxfId="265" priority="176" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H109">
-    <cfRule type="cellIs" dxfId="243" priority="156" operator="equal">
+    <cfRule type="cellIs" dxfId="264" priority="177" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H105">
-    <cfRule type="cellIs" dxfId="242" priority="157" operator="equal">
+    <cfRule type="cellIs" dxfId="263" priority="178" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H105">
-    <cfRule type="cellIs" dxfId="241" priority="158" operator="equal">
+    <cfRule type="cellIs" dxfId="262" priority="179" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H105">
-    <cfRule type="cellIs" dxfId="240" priority="159" operator="equal">
+    <cfRule type="cellIs" dxfId="261" priority="180" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H108">
-    <cfRule type="cellIs" dxfId="239" priority="160" operator="equal">
+    <cfRule type="cellIs" dxfId="260" priority="181" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H108">
-    <cfRule type="cellIs" dxfId="238" priority="161" operator="equal">
+    <cfRule type="cellIs" dxfId="259" priority="182" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H108">
-    <cfRule type="cellIs" dxfId="237" priority="162" operator="equal">
+    <cfRule type="cellIs" dxfId="258" priority="183" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H111">
-    <cfRule type="cellIs" dxfId="236" priority="163" operator="equal">
+    <cfRule type="cellIs" dxfId="257" priority="184" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H111">
-    <cfRule type="cellIs" dxfId="235" priority="164" operator="equal">
+    <cfRule type="cellIs" dxfId="256" priority="185" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H111">
-    <cfRule type="cellIs" dxfId="234" priority="165" operator="equal">
+    <cfRule type="cellIs" dxfId="255" priority="186" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H116">
-    <cfRule type="cellIs" dxfId="233" priority="166" operator="equal">
+    <cfRule type="cellIs" dxfId="254" priority="187" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H116">
-    <cfRule type="cellIs" dxfId="232" priority="167" operator="equal">
+    <cfRule type="cellIs" dxfId="253" priority="188" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H116">
-    <cfRule type="cellIs" dxfId="231" priority="168" operator="equal">
+    <cfRule type="cellIs" dxfId="252" priority="189" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H115">
-    <cfRule type="cellIs" dxfId="230" priority="169" operator="equal">
+    <cfRule type="cellIs" dxfId="251" priority="190" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H115">
-    <cfRule type="cellIs" dxfId="229" priority="170" operator="equal">
+    <cfRule type="cellIs" dxfId="250" priority="191" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H115">
-    <cfRule type="cellIs" dxfId="228" priority="171" operator="equal">
+    <cfRule type="cellIs" dxfId="249" priority="192" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H110">
-    <cfRule type="cellIs" dxfId="227" priority="172" operator="equal">
+    <cfRule type="cellIs" dxfId="248" priority="193" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H110">
-    <cfRule type="cellIs" dxfId="226" priority="173" operator="equal">
+    <cfRule type="cellIs" dxfId="247" priority="194" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H110">
-    <cfRule type="cellIs" dxfId="225" priority="174" operator="equal">
+    <cfRule type="cellIs" dxfId="246" priority="195" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H122">
-    <cfRule type="cellIs" dxfId="224" priority="175" operator="equal">
+    <cfRule type="cellIs" dxfId="245" priority="196" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H122">
-    <cfRule type="cellIs" dxfId="223" priority="176" operator="equal">
+    <cfRule type="cellIs" dxfId="244" priority="197" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H122">
-    <cfRule type="cellIs" dxfId="222" priority="177" operator="equal">
+    <cfRule type="cellIs" dxfId="243" priority="198" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H118">
-    <cfRule type="cellIs" dxfId="221" priority="178" operator="equal">
+    <cfRule type="cellIs" dxfId="242" priority="199" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H118">
-    <cfRule type="cellIs" dxfId="220" priority="179" operator="equal">
+    <cfRule type="cellIs" dxfId="241" priority="200" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H118">
-    <cfRule type="cellIs" dxfId="219" priority="180" operator="equal">
+    <cfRule type="cellIs" dxfId="240" priority="201" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H121">
-    <cfRule type="cellIs" dxfId="218" priority="181" operator="equal">
+    <cfRule type="cellIs" dxfId="239" priority="202" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H121">
-    <cfRule type="cellIs" dxfId="217" priority="182" operator="equal">
+    <cfRule type="cellIs" dxfId="238" priority="203" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H121">
-    <cfRule type="cellIs" dxfId="216" priority="183" operator="equal">
+    <cfRule type="cellIs" dxfId="237" priority="204" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H124">
-    <cfRule type="cellIs" dxfId="215" priority="184" operator="equal">
+    <cfRule type="cellIs" dxfId="236" priority="205" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H124">
-    <cfRule type="cellIs" dxfId="214" priority="185" operator="equal">
+    <cfRule type="cellIs" dxfId="235" priority="206" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H124">
-    <cfRule type="cellIs" dxfId="213" priority="186" operator="equal">
+    <cfRule type="cellIs" dxfId="234" priority="207" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H129">
-    <cfRule type="cellIs" dxfId="212" priority="187" operator="equal">
+    <cfRule type="cellIs" dxfId="233" priority="208" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H129">
-    <cfRule type="cellIs" dxfId="211" priority="188" operator="equal">
+    <cfRule type="cellIs" dxfId="232" priority="209" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H129">
-    <cfRule type="cellIs" dxfId="210" priority="189" operator="equal">
+    <cfRule type="cellIs" dxfId="231" priority="210" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H128">
-    <cfRule type="cellIs" dxfId="209" priority="190" operator="equal">
+    <cfRule type="cellIs" dxfId="230" priority="211" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H128">
-    <cfRule type="cellIs" dxfId="208" priority="191" operator="equal">
+    <cfRule type="cellIs" dxfId="229" priority="212" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H128">
-    <cfRule type="cellIs" dxfId="207" priority="192" operator="equal">
+    <cfRule type="cellIs" dxfId="228" priority="213" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H123">
-    <cfRule type="cellIs" dxfId="206" priority="193" operator="equal">
+    <cfRule type="cellIs" dxfId="227" priority="214" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H123">
-    <cfRule type="cellIs" dxfId="205" priority="194" operator="equal">
+    <cfRule type="cellIs" dxfId="226" priority="215" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H123">
-    <cfRule type="cellIs" dxfId="204" priority="195" operator="equal">
+    <cfRule type="cellIs" dxfId="225" priority="216" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H135">
-    <cfRule type="cellIs" dxfId="203" priority="196" operator="equal">
+    <cfRule type="cellIs" dxfId="224" priority="217" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H135">
-    <cfRule type="cellIs" dxfId="202" priority="197" operator="equal">
+    <cfRule type="cellIs" dxfId="223" priority="218" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H135">
-    <cfRule type="cellIs" dxfId="201" priority="198" operator="equal">
+    <cfRule type="cellIs" dxfId="222" priority="219" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H131">
-    <cfRule type="cellIs" dxfId="200" priority="199" operator="equal">
+    <cfRule type="cellIs" dxfId="221" priority="220" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H131">
-    <cfRule type="cellIs" dxfId="199" priority="200" operator="equal">
+    <cfRule type="cellIs" dxfId="220" priority="221" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H131">
-    <cfRule type="cellIs" dxfId="198" priority="201" operator="equal">
+    <cfRule type="cellIs" dxfId="219" priority="222" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H134">
-    <cfRule type="cellIs" dxfId="197" priority="202" operator="equal">
+    <cfRule type="cellIs" dxfId="218" priority="223" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H134">
-    <cfRule type="cellIs" dxfId="196" priority="203" operator="equal">
+    <cfRule type="cellIs" dxfId="217" priority="224" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H134">
-    <cfRule type="cellIs" dxfId="195" priority="204" operator="equal">
+    <cfRule type="cellIs" dxfId="216" priority="225" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H137">
-    <cfRule type="cellIs" dxfId="194" priority="205" operator="equal">
+    <cfRule type="cellIs" dxfId="215" priority="226" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H137">
-    <cfRule type="cellIs" dxfId="193" priority="206" operator="equal">
+    <cfRule type="cellIs" dxfId="214" priority="227" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H137">
-    <cfRule type="cellIs" dxfId="192" priority="207" operator="equal">
+    <cfRule type="cellIs" dxfId="213" priority="228" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H142">
-    <cfRule type="cellIs" dxfId="191" priority="208" operator="equal">
+    <cfRule type="cellIs" dxfId="212" priority="229" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H142">
-    <cfRule type="cellIs" dxfId="190" priority="209" operator="equal">
+    <cfRule type="cellIs" dxfId="211" priority="230" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H142">
-    <cfRule type="cellIs" dxfId="189" priority="210" operator="equal">
+    <cfRule type="cellIs" dxfId="210" priority="231" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H141">
-    <cfRule type="cellIs" dxfId="188" priority="211" operator="equal">
+    <cfRule type="cellIs" dxfId="209" priority="232" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H141">
-    <cfRule type="cellIs" dxfId="187" priority="212" operator="equal">
+    <cfRule type="cellIs" dxfId="208" priority="233" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H141">
-    <cfRule type="cellIs" dxfId="186" priority="213" operator="equal">
+    <cfRule type="cellIs" dxfId="207" priority="234" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H136">
-    <cfRule type="cellIs" dxfId="185" priority="214" operator="equal">
+    <cfRule type="cellIs" dxfId="206" priority="235" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H136">
-    <cfRule type="cellIs" dxfId="184" priority="215" operator="equal">
+    <cfRule type="cellIs" dxfId="205" priority="236" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H136">
-    <cfRule type="cellIs" dxfId="183" priority="216" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H8">
-    <cfRule type="cellIs" dxfId="182" priority="217" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H8">
-    <cfRule type="cellIs" dxfId="181" priority="218" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H8">
-    <cfRule type="cellIs" dxfId="180" priority="219" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H29">
-    <cfRule type="cellIs" dxfId="179" priority="220" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H29">
-    <cfRule type="cellIs" dxfId="178" priority="221" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H29">
-    <cfRule type="cellIs" dxfId="177" priority="222" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H50">
-    <cfRule type="cellIs" dxfId="176" priority="223" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H50">
-    <cfRule type="cellIs" dxfId="175" priority="224" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H50">
-    <cfRule type="cellIs" dxfId="174" priority="225" operator="equal">
+    <cfRule type="cellIs" dxfId="204" priority="237" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H3:H4 H8:H10 H12 H15:H17 H21:H22 H24:H25 H29:H33 H36:H38 H42:H43 H45:H46 H50:H52 H54 H57:H59 H63:H64 H66 H69:H72 H76:H77 H79 H82:H85 H89:H90 H92 H95:H98 H102:H103 H105 H108:H111 H115:H116 H118 H121:H124 H128:H129 H131 H134:H137 H141:H142">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H3:H4 H30:H33 H12 H15:H17 H21:H22 H24:H25 H51:H52 H36:H38 H42:H43 H45:H46 H141:H142 H54 H57:H59 H63:H64 H66 H69:H72 H76:H77 H79 H82:H85 H89:H90 H92 H95:H98 H102:H103 H105 H108:H111 H115:H116 H118 H121:H124 H128:H129 H131 H134:H137 H9:H10">
       <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="21" operator="equal" id="{0F88A3A9-7741-499D-8553-E9ADB4798D1B}">
+            <xm:f>'C:\Users\DSi\Documents\Users\DSi\Desktop\backuo\src\main\resources\modules\[sample.xlsx]Controller'!#REF!</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="5" tint="0.39994506668294322"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>H47:H50</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="20" operator="equal" id="{BC21F9FA-1C54-489B-A95A-4AFBF20911CA}">
+            <xm:f>'C:\Users\DSi\Documents\Users\DSi\Desktop\backuo\src\main\resources\modules\[sample.xlsx]Controller'!#REF!</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="5" tint="0.39994506668294322"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>H39:H41</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="19" operator="equal" id="{CD5B42B5-F495-4292-AEBD-7166B3D8C54B}">
+            <xm:f>'C:\Users\DSi\Documents\Users\DSi\Desktop\backuo\src\main\resources\modules\[sample.xlsx]Controller'!#REF!</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="5" tint="0.39994506668294322"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>H34:H35</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="18" operator="equal" id="{815E18FC-B86D-42DB-9B25-99AC6A766975}">
+            <xm:f>'C:\Users\DSi\Documents\Users\DSi\Desktop\backuo\src\main\resources\modules\[sample.xlsx]Controller'!#REF!</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="5" tint="0.39994506668294322"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>H26:H29</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="17" operator="equal" id="{FB67F097-4A16-4591-9EBB-5B14C49D1FF6}">
+            <xm:f>'C:\Users\DSi\Documents\Users\DSi\Desktop\backuo\src\main\resources\modules\[sample.xlsx]Controller'!#REF!</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="5" tint="0.39994506668294322"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>H5:H8</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="16" operator="equal" id="{C79AB38D-FDD1-415C-A421-235230524200}">
+            <xm:f>'C:\Users\DSi\Documents\Users\DSi\Desktop\backuo\src\main\resources\modules\[sample.xlsx]Controller'!#REF!</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="5" tint="0.39994506668294322"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>H13:H14</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="15" operator="equal" id="{63FB0488-7C8A-43B4-B573-A51F49890029}">
+            <xm:f>'C:\Users\DSi\Documents\Users\DSi\Desktop\backuo\src\main\resources\modules\[sample.xlsx]Controller'!#REF!</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="5" tint="0.39994506668294322"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>H18:H20</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="14" operator="equal" id="{1458C84B-2631-4458-9297-1F2DBCD96F42}">
+            <xm:f>'C:\Users\DSi\Documents\Users\DSi\Desktop\backuo\src\main\resources\modules\[sample.xlsx]Controller'!#REF!</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="5" tint="0.39994506668294322"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>H55:H56</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="13" operator="equal" id="{424E64FB-9A6D-43F3-82B6-3D30201DC771}">
+            <xm:f>'C:\Users\DSi\Documents\Users\DSi\Desktop\backuo\src\main\resources\modules\[sample.xlsx]Controller'!#REF!</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="5" tint="0.39994506668294322"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>H60:H62</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="12" operator="equal" id="{E66A4116-0E17-4933-A353-EC2689CB72CE}">
+            <xm:f>'C:\Users\DSi\Documents\Users\DSi\Desktop\backuo\src\main\resources\modules\[sample.xlsx]Controller'!#REF!</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="5" tint="0.39994506668294322"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>H67:H68</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="11" operator="equal" id="{91793D95-13C5-4517-A376-CD2166E458E7}">
+            <xm:f>'C:\Users\DSi\Documents\Users\DSi\Desktop\backuo\src\main\resources\modules\[sample.xlsx]Controller'!#REF!</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="5" tint="0.39994506668294322"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>H73:H75</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="10" operator="equal" id="{AA55BDD3-A369-441F-8323-639D3B95D969}">
+            <xm:f>'C:\Users\DSi\Documents\Users\DSi\Desktop\backuo\src\main\resources\modules\[sample.xlsx]Controller'!#REF!</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="5" tint="0.39994506668294322"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>H80:H81</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="9" operator="equal" id="{1E905747-D560-49D7-B09A-B416B7DB5C1A}">
+            <xm:f>'C:\Users\DSi\Documents\Users\DSi\Desktop\backuo\src\main\resources\modules\[sample.xlsx]Controller'!#REF!</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="5" tint="0.39994506668294322"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>H86:H88</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="8" operator="equal" id="{638DFABC-5B8E-40EA-BE49-5C2317F62E63}">
+            <xm:f>'C:\Users\DSi\Documents\Users\DSi\Desktop\backuo\src\main\resources\modules\[sample.xlsx]Controller'!#REF!</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="5" tint="0.39994506668294322"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>H93:H94</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="7" operator="equal" id="{3533E3C6-7DB0-42F7-8C84-BAEB3838E1A4}">
+            <xm:f>'C:\Users\DSi\Documents\Users\DSi\Desktop\backuo\src\main\resources\modules\[sample.xlsx]Controller'!#REF!</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="5" tint="0.39994506668294322"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>H99:H101</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="6" operator="equal" id="{6F4C3F67-7C3B-445F-AF41-EC8E69B77AAA}">
+            <xm:f>'C:\Users\DSi\Documents\Users\DSi\Desktop\backuo\src\main\resources\modules\[sample.xlsx]Controller'!#REF!</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="5" tint="0.39994506668294322"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>H106:H107</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="5" operator="equal" id="{330AA708-A92A-4765-B80D-0220EFC828FA}">
+            <xm:f>'C:\Users\DSi\Documents\Users\DSi\Desktop\backuo\src\main\resources\modules\[sample.xlsx]Controller'!#REF!</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="5" tint="0.39994506668294322"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>H112:H114</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="4" operator="equal" id="{A29F1A29-DD31-4213-8B64-931A4014B1E9}">
+            <xm:f>'C:\Users\DSi\Documents\Users\DSi\Desktop\backuo\src\main\resources\modules\[sample.xlsx]Controller'!#REF!</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="5" tint="0.39994506668294322"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>H119:H120</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="3" operator="equal" id="{43B8262E-A1A8-4BF0-8058-3A478B5B54A6}">
+            <xm:f>'C:\Users\DSi\Documents\Users\DSi\Desktop\backuo\src\main\resources\modules\[sample.xlsx]Controller'!#REF!</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="5" tint="0.39994506668294322"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>H125:H127</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="2" operator="equal" id="{3B300F48-7AAF-4CAF-B913-A92670FAC57B}">
+            <xm:f>'C:\Users\DSi\Documents\Users\DSi\Desktop\backuo\src\main\resources\modules\[sample.xlsx]Controller'!#REF!</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="5" tint="0.39994506668294322"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>H132:H133</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="1" operator="equal" id="{194FB7D5-1C8A-4201-9DD0-D4D503D4B1E8}">
+            <xm:f>'C:\Users\DSi\Documents\Users\DSi\Desktop\backuo\src\main\resources\modules\[sample.xlsx]Controller'!#REF!</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="5" tint="0.39994506668294322"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>H138:H140</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -21196,362 +21811,362 @@
     <mergeCell ref="B34:D34"/>
   </mergeCells>
   <conditionalFormatting sqref="H8">
-    <cfRule type="cellIs" dxfId="173" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="194" priority="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H8">
-    <cfRule type="cellIs" dxfId="172" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="193" priority="2" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H8">
-    <cfRule type="cellIs" dxfId="171" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="192" priority="3" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6">
-    <cfRule type="cellIs" dxfId="170" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="191" priority="4" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6">
-    <cfRule type="cellIs" dxfId="169" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="190" priority="5" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6">
-    <cfRule type="cellIs" dxfId="168" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="189" priority="6" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7">
-    <cfRule type="cellIs" dxfId="167" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="188" priority="7" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7">
-    <cfRule type="cellIs" dxfId="166" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="187" priority="8" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7">
-    <cfRule type="cellIs" dxfId="165" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="186" priority="9" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16">
-    <cfRule type="cellIs" dxfId="164" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="185" priority="10" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16">
-    <cfRule type="cellIs" dxfId="163" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="184" priority="11" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16">
-    <cfRule type="cellIs" dxfId="162" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="183" priority="12" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H14">
-    <cfRule type="cellIs" dxfId="161" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="182" priority="13" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H14">
-    <cfRule type="cellIs" dxfId="160" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="181" priority="14" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H14">
-    <cfRule type="cellIs" dxfId="159" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="180" priority="15" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H15">
-    <cfRule type="cellIs" dxfId="158" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="179" priority="16" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H15">
-    <cfRule type="cellIs" dxfId="157" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="178" priority="17" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H15">
-    <cfRule type="cellIs" dxfId="156" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="177" priority="18" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H24">
-    <cfRule type="cellIs" dxfId="155" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="176" priority="19" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H24">
-    <cfRule type="cellIs" dxfId="154" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="175" priority="20" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H24">
-    <cfRule type="cellIs" dxfId="153" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="174" priority="21" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H22">
-    <cfRule type="cellIs" dxfId="152" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="173" priority="22" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H22">
-    <cfRule type="cellIs" dxfId="151" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="172" priority="23" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H22">
-    <cfRule type="cellIs" dxfId="150" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="171" priority="24" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H23">
-    <cfRule type="cellIs" dxfId="149" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="170" priority="25" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H23">
-    <cfRule type="cellIs" dxfId="148" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="169" priority="26" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H23">
-    <cfRule type="cellIs" dxfId="147" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="168" priority="27" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H32">
-    <cfRule type="cellIs" dxfId="146" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="167" priority="28" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H32">
-    <cfRule type="cellIs" dxfId="145" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="166" priority="29" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H32">
-    <cfRule type="cellIs" dxfId="144" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="165" priority="30" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H30">
-    <cfRule type="cellIs" dxfId="143" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="164" priority="31" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H30">
-    <cfRule type="cellIs" dxfId="142" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="163" priority="32" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H30">
-    <cfRule type="cellIs" dxfId="141" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="162" priority="33" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H31">
-    <cfRule type="cellIs" dxfId="140" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="161" priority="34" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H31">
-    <cfRule type="cellIs" dxfId="139" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="160" priority="35" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H31">
-    <cfRule type="cellIs" dxfId="138" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="159" priority="36" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H40">
-    <cfRule type="cellIs" dxfId="137" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="158" priority="37" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H40">
-    <cfRule type="cellIs" dxfId="136" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="157" priority="38" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H40">
-    <cfRule type="cellIs" dxfId="135" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="156" priority="39" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H38">
-    <cfRule type="cellIs" dxfId="134" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="155" priority="40" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H38">
-    <cfRule type="cellIs" dxfId="133" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="154" priority="41" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H38">
-    <cfRule type="cellIs" dxfId="132" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="153" priority="42" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H39">
-    <cfRule type="cellIs" dxfId="131" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="152" priority="43" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H39">
-    <cfRule type="cellIs" dxfId="130" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="151" priority="44" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H39">
-    <cfRule type="cellIs" dxfId="129" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="150" priority="45" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H48">
-    <cfRule type="cellIs" dxfId="128" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="149" priority="46" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H48">
-    <cfRule type="cellIs" dxfId="127" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="148" priority="47" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H48">
-    <cfRule type="cellIs" dxfId="126" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="147" priority="48" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H46">
-    <cfRule type="cellIs" dxfId="125" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="146" priority="49" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H46">
-    <cfRule type="cellIs" dxfId="124" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="145" priority="50" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H46">
-    <cfRule type="cellIs" dxfId="123" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="144" priority="51" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H47">
-    <cfRule type="cellIs" dxfId="122" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="143" priority="52" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H47">
-    <cfRule type="cellIs" dxfId="121" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="142" priority="53" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H47">
-    <cfRule type="cellIs" dxfId="120" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="141" priority="54" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H13">
-    <cfRule type="cellIs" dxfId="119" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="140" priority="55" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H13">
-    <cfRule type="cellIs" dxfId="118" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="139" priority="56" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H13">
-    <cfRule type="cellIs" dxfId="117" priority="57" operator="equal">
+    <cfRule type="cellIs" dxfId="138" priority="57" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H21">
-    <cfRule type="cellIs" dxfId="116" priority="58" operator="equal">
+    <cfRule type="cellIs" dxfId="137" priority="58" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H21">
-    <cfRule type="cellIs" dxfId="115" priority="59" operator="equal">
+    <cfRule type="cellIs" dxfId="136" priority="59" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H21">
-    <cfRule type="cellIs" dxfId="114" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="135" priority="60" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H29">
-    <cfRule type="cellIs" dxfId="113" priority="61" operator="equal">
+    <cfRule type="cellIs" dxfId="134" priority="61" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H29">
-    <cfRule type="cellIs" dxfId="112" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="133" priority="62" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H29">
-    <cfRule type="cellIs" dxfId="111" priority="63" operator="equal">
+    <cfRule type="cellIs" dxfId="132" priority="63" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H37">
-    <cfRule type="cellIs" dxfId="110" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="131" priority="64" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H37">
-    <cfRule type="cellIs" dxfId="109" priority="65" operator="equal">
+    <cfRule type="cellIs" dxfId="130" priority="65" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H37">
-    <cfRule type="cellIs" dxfId="108" priority="66" operator="equal">
+    <cfRule type="cellIs" dxfId="129" priority="66" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H45">
-    <cfRule type="cellIs" dxfId="107" priority="67" operator="equal">
+    <cfRule type="cellIs" dxfId="128" priority="67" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H45">
-    <cfRule type="cellIs" dxfId="106" priority="68" operator="equal">
+    <cfRule type="cellIs" dxfId="127" priority="68" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H45">
-    <cfRule type="cellIs" dxfId="105" priority="69" operator="equal">
+    <cfRule type="cellIs" dxfId="126" priority="69" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5">
-    <cfRule type="cellIs" dxfId="104" priority="70" operator="equal">
+    <cfRule type="cellIs" dxfId="125" priority="70" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5">
-    <cfRule type="cellIs" dxfId="103" priority="71" operator="equal">
+    <cfRule type="cellIs" dxfId="124" priority="71" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5">
-    <cfRule type="cellIs" dxfId="102" priority="72" operator="equal">
+    <cfRule type="cellIs" dxfId="123" priority="72" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21570,7 +22185,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -21651,7 +22266,7 @@
       <c r="G2" s="136"/>
       <c r="H2" s="136"/>
       <c r="I2" s="136"/>
-      <c r="J2" s="142"/>
+      <c r="J2" s="137"/>
       <c r="K2" s="45"/>
       <c r="L2" s="46"/>
       <c r="M2" s="47"/>
@@ -21835,7 +22450,7 @@
       <c r="G7" s="136"/>
       <c r="H7" s="136"/>
       <c r="I7" s="136"/>
-      <c r="J7" s="142"/>
+      <c r="J7" s="137"/>
       <c r="K7" s="45"/>
       <c r="L7" s="46"/>
       <c r="M7" s="47"/>
@@ -22019,7 +22634,7 @@
       <c r="G12" s="136"/>
       <c r="H12" s="136"/>
       <c r="I12" s="136"/>
-      <c r="J12" s="142"/>
+      <c r="J12" s="137"/>
       <c r="K12" s="45"/>
       <c r="L12" s="46"/>
       <c r="M12" s="47"/>
@@ -22203,7 +22818,7 @@
       <c r="G17" s="136"/>
       <c r="H17" s="136"/>
       <c r="I17" s="136"/>
-      <c r="J17" s="142"/>
+      <c r="J17" s="137"/>
       <c r="K17" s="45"/>
       <c r="L17" s="46"/>
       <c r="M17" s="47"/>
@@ -22387,7 +23002,7 @@
       <c r="G22" s="136"/>
       <c r="H22" s="136"/>
       <c r="I22" s="136"/>
-      <c r="J22" s="142"/>
+      <c r="J22" s="137"/>
       <c r="K22" s="45"/>
       <c r="L22" s="46"/>
       <c r="M22" s="47"/>
@@ -22561,7 +23176,7 @@
       <c r="G27" s="136"/>
       <c r="H27" s="136"/>
       <c r="I27" s="136"/>
-      <c r="J27" s="142"/>
+      <c r="J27" s="137"/>
       <c r="K27" s="45"/>
       <c r="L27" s="46"/>
       <c r="M27" s="47"/>
@@ -22745,7 +23360,7 @@
       <c r="G32" s="136"/>
       <c r="H32" s="136"/>
       <c r="I32" s="136"/>
-      <c r="J32" s="142"/>
+      <c r="J32" s="137"/>
       <c r="K32" s="45"/>
       <c r="L32" s="46"/>
       <c r="M32" s="47"/>
@@ -22929,7 +23544,7 @@
       <c r="G37" s="136"/>
       <c r="H37" s="136"/>
       <c r="I37" s="136"/>
-      <c r="J37" s="142"/>
+      <c r="J37" s="137"/>
       <c r="K37" s="45"/>
       <c r="L37" s="46"/>
       <c r="M37" s="47"/>
@@ -23113,7 +23728,7 @@
       <c r="G42" s="136"/>
       <c r="H42" s="136"/>
       <c r="I42" s="136"/>
-      <c r="J42" s="142"/>
+      <c r="J42" s="137"/>
       <c r="K42" s="45"/>
       <c r="L42" s="46"/>
       <c r="M42" s="47"/>
@@ -23297,7 +23912,7 @@
       <c r="G47" s="136"/>
       <c r="H47" s="136"/>
       <c r="I47" s="136"/>
-      <c r="J47" s="142"/>
+      <c r="J47" s="137"/>
       <c r="K47" s="45"/>
       <c r="L47" s="46"/>
       <c r="M47" s="47"/>
@@ -23481,7 +24096,7 @@
       <c r="G52" s="136"/>
       <c r="H52" s="136"/>
       <c r="I52" s="136"/>
-      <c r="J52" s="142"/>
+      <c r="J52" s="137"/>
       <c r="K52" s="45"/>
       <c r="L52" s="46"/>
       <c r="M52" s="47"/>
@@ -23665,7 +24280,7 @@
       <c r="G57" s="136"/>
       <c r="H57" s="136"/>
       <c r="I57" s="136"/>
-      <c r="J57" s="142"/>
+      <c r="J57" s="137"/>
       <c r="K57" s="45"/>
       <c r="L57" s="46"/>
       <c r="M57" s="47"/>
@@ -50131,11 +50746,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="C37:J37"/>
-    <mergeCell ref="C47:J47"/>
-    <mergeCell ref="C52:J52"/>
-    <mergeCell ref="C57:J57"/>
-    <mergeCell ref="C42:J42"/>
     <mergeCell ref="C22:J22"/>
     <mergeCell ref="C27:J27"/>
     <mergeCell ref="C32:J32"/>
@@ -50143,109 +50753,114 @@
     <mergeCell ref="C7:J7"/>
     <mergeCell ref="C12:J12"/>
     <mergeCell ref="C17:J17"/>
+    <mergeCell ref="C37:J37"/>
+    <mergeCell ref="C47:J47"/>
+    <mergeCell ref="C52:J52"/>
+    <mergeCell ref="C57:J57"/>
+    <mergeCell ref="C42:J42"/>
   </mergeCells>
   <conditionalFormatting sqref="H65">
-    <cfRule type="cellIs" dxfId="101" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="122" priority="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H65">
-    <cfRule type="cellIs" dxfId="100" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="121" priority="2" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H65">
-    <cfRule type="cellIs" dxfId="99" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="120" priority="3" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H63">
-    <cfRule type="cellIs" dxfId="98" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="119" priority="4" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H63">
-    <cfRule type="cellIs" dxfId="97" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="118" priority="5" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H63">
-    <cfRule type="cellIs" dxfId="96" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="117" priority="6" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H64">
-    <cfRule type="cellIs" dxfId="95" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="116" priority="7" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H64">
-    <cfRule type="cellIs" dxfId="94" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="115" priority="8" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H64">
-    <cfRule type="cellIs" dxfId="93" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="114" priority="9" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H61">
-    <cfRule type="cellIs" dxfId="92" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="113" priority="10" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H61">
-    <cfRule type="cellIs" dxfId="91" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="112" priority="11" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H61">
-    <cfRule type="cellIs" dxfId="90" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="111" priority="12" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H62">
-    <cfRule type="cellIs" dxfId="89" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="110" priority="13" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H62">
-    <cfRule type="cellIs" dxfId="88" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="109" priority="14" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H62">
-    <cfRule type="cellIs" dxfId="87" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="108" priority="15" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6">
-    <cfRule type="cellIs" dxfId="86" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="107" priority="16" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6">
-    <cfRule type="cellIs" dxfId="85" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="106" priority="17" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6">
-    <cfRule type="cellIs" dxfId="84" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="105" priority="18" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H26">
-    <cfRule type="cellIs" dxfId="83" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="19" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H26">
-    <cfRule type="cellIs" dxfId="82" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="103" priority="20" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H26">
-    <cfRule type="cellIs" dxfId="81" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="102" priority="21" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
@@ -62478,18 +63093,18 @@
     <row r="470" spans="1:10" ht="12.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="C395:J395"/>
+    <mergeCell ref="C142:J142"/>
+    <mergeCell ref="C431:J431"/>
+    <mergeCell ref="C213:J213"/>
+    <mergeCell ref="C250:J250"/>
+    <mergeCell ref="C359:J359"/>
     <mergeCell ref="C2:J2"/>
     <mergeCell ref="C36:J36"/>
     <mergeCell ref="C177:J177"/>
     <mergeCell ref="C323:J323"/>
     <mergeCell ref="C70:J70"/>
     <mergeCell ref="C106:J106"/>
-    <mergeCell ref="C395:J395"/>
-    <mergeCell ref="C142:J142"/>
-    <mergeCell ref="C431:J431"/>
-    <mergeCell ref="C213:J213"/>
-    <mergeCell ref="C250:J250"/>
-    <mergeCell ref="C359:J359"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add deleteRPR method and configure xlsx file for execution of test cases in App
</commit_message>
<xml_diff>
--- a/src/main/resources/modules/SMOKE.xlsx
+++ b/src/main/resources/modules/SMOKE.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="9000" windowWidth="20490" windowHeight="3450" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="9450" windowWidth="20490" windowHeight="3450"/>
   </bookViews>
   <sheets>
     <sheet name="Controller" sheetId="1" r:id="rId1"/>
@@ -740,15 +740,6 @@
     <t>13th Period - Lessor - Operating - Validate user is able to Add Revision</t>
   </si>
   <si>
-    <t>TCEnv107</t>
-  </si>
-  <si>
-    <t>TCEnv108</t>
-  </si>
-  <si>
-    <t>TCEnv109</t>
-  </si>
-  <si>
     <t>Homepage</t>
   </si>
   <si>
@@ -756,6 +747,15 @@
   </si>
   <si>
     <t>UIBase.VerifyPageLoadedTrue</t>
+  </si>
+  <si>
+    <t>TCEnv101</t>
+  </si>
+  <si>
+    <t>TCEnv105</t>
+  </si>
+  <si>
+    <t>TCEnv106</t>
   </si>
 </sst>
 </file>
@@ -1610,46 +1610,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1672,19 +1632,52 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="420">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2993,6 +2986,13 @@
         <patternFill patternType="solid">
           <fgColor rgb="FFF4B083"/>
           <bgColor rgb="FFF4B083"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5235,8 +5235,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1005"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:D6"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -5349,7 +5349,7 @@
         <v>27</v>
       </c>
       <c r="I3" s="118" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="25.5" customHeight="1">
@@ -5372,7 +5372,7 @@
         <v>27</v>
       </c>
       <c r="I4" s="118" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="S4" s="68" t="s">
         <v>26</v>
@@ -5398,7 +5398,7 @@
         <v>55</v>
       </c>
       <c r="I5" s="118" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
     </row>
     <row r="6" spans="1:26">
@@ -5421,7 +5421,7 @@
         <v>55</v>
       </c>
       <c r="I6" s="118" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
     </row>
     <row r="7" spans="1:26">
@@ -5444,7 +5444,7 @@
         <v>55</v>
       </c>
       <c r="I7" s="118" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
     </row>
     <row r="8" spans="1:26">
@@ -5467,7 +5467,7 @@
         <v>55</v>
       </c>
       <c r="I8" s="118" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
     </row>
     <row r="9" spans="1:26">
@@ -5490,7 +5490,7 @@
         <v>62</v>
       </c>
       <c r="I9" s="118" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
     </row>
     <row r="10" spans="1:26">
@@ -5513,7 +5513,7 @@
         <v>62</v>
       </c>
       <c r="I10" s="118" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
     </row>
     <row r="11" spans="1:26">
@@ -5536,7 +5536,7 @@
         <v>62</v>
       </c>
       <c r="I11" s="118" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
     </row>
     <row r="12" spans="1:26">
@@ -5559,7 +5559,7 @@
         <v>62</v>
       </c>
       <c r="I12" s="118" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
     </row>
     <row r="13" spans="1:26" s="79" customFormat="1">
@@ -5582,7 +5582,7 @@
         <v>210</v>
       </c>
       <c r="I13" s="118" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
     </row>
     <row r="14" spans="1:26" s="79" customFormat="1">
@@ -5605,7 +5605,7 @@
         <v>210</v>
       </c>
       <c r="I14" s="118" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="15" customHeight="1">
@@ -5630,7 +5630,7 @@
       <c r="G15" s="79"/>
       <c r="H15" s="79"/>
       <c r="I15" s="118" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="15" customHeight="1">
@@ -5655,7 +5655,7 @@
       <c r="G16" s="79"/>
       <c r="H16" s="79"/>
       <c r="I16" s="118" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
     </row>
     <row r="18" spans="1:26">
@@ -5708,7 +5708,7 @@
         <v>27</v>
       </c>
       <c r="I19" s="118" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
     </row>
     <row r="20" spans="1:26">
@@ -5731,7 +5731,7 @@
         <v>27</v>
       </c>
       <c r="I20" s="118" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
     </row>
     <row r="21" spans="1:26">
@@ -5754,7 +5754,7 @@
         <v>55</v>
       </c>
       <c r="I21" s="118" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
     </row>
     <row r="22" spans="1:26">
@@ -5777,7 +5777,7 @@
         <v>55</v>
       </c>
       <c r="I22" s="118" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
     </row>
     <row r="23" spans="1:26">
@@ -5800,7 +5800,7 @@
         <v>55</v>
       </c>
       <c r="I23" s="118" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
     </row>
     <row r="24" spans="1:26" ht="15.75" customHeight="1">
@@ -5823,7 +5823,7 @@
         <v>55</v>
       </c>
       <c r="I24" s="118" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
     </row>
     <row r="25" spans="1:26" ht="15.75" customHeight="1">
@@ -5846,7 +5846,7 @@
         <v>62</v>
       </c>
       <c r="I25" s="118" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
     </row>
     <row r="26" spans="1:26" ht="15.75" customHeight="1">
@@ -5869,7 +5869,7 @@
         <v>62</v>
       </c>
       <c r="I26" s="118" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
     </row>
     <row r="27" spans="1:26" ht="15.75" customHeight="1">
@@ -5892,7 +5892,7 @@
         <v>62</v>
       </c>
       <c r="I27" s="118" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
     </row>
     <row r="28" spans="1:26" ht="15.75" customHeight="1">
@@ -5915,7 +5915,7 @@
         <v>62</v>
       </c>
       <c r="I28" s="118" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
     </row>
     <row r="29" spans="1:26" s="79" customFormat="1">
@@ -5938,7 +5938,7 @@
         <v>210</v>
       </c>
       <c r="I29" s="118" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
     </row>
     <row r="30" spans="1:26" s="79" customFormat="1">
@@ -5961,7 +5961,7 @@
         <v>210</v>
       </c>
       <c r="I30" s="118" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
     </row>
     <row r="31" spans="1:26" s="79" customFormat="1">
@@ -5984,7 +5984,7 @@
         <v>210</v>
       </c>
       <c r="I31" s="118" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
     </row>
     <row r="32" spans="1:26" s="79" customFormat="1">
@@ -6007,7 +6007,7 @@
         <v>210</v>
       </c>
       <c r="I32" s="118" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
     </row>
     <row r="33" spans="1:26" s="133" customFormat="1" ht="15.75" customHeight="1">
@@ -6065,7 +6065,7 @@
         <v>27</v>
       </c>
       <c r="I35" s="118" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
     </row>
     <row r="36" spans="1:26" ht="15.75" customHeight="1">
@@ -6088,7 +6088,7 @@
         <v>27</v>
       </c>
       <c r="I36" s="118" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
     </row>
     <row r="37" spans="1:26" ht="15.75" customHeight="1">
@@ -6113,7 +6113,7 @@
       <c r="G37" s="126"/>
       <c r="H37" s="126"/>
       <c r="I37" s="118" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="J37" s="126"/>
       <c r="K37" s="126"/>
@@ -6155,7 +6155,7 @@
       <c r="G38" s="126"/>
       <c r="H38" s="126"/>
       <c r="I38" s="118" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="J38" s="126"/>
       <c r="K38" s="126"/>
@@ -6197,7 +6197,7 @@
       <c r="G39" s="126"/>
       <c r="H39" s="126"/>
       <c r="I39" s="118" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="J39" s="126"/>
       <c r="K39" s="126"/>
@@ -6239,7 +6239,7 @@
       <c r="G40" s="126"/>
       <c r="H40" s="126"/>
       <c r="I40" s="118" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="J40" s="126"/>
       <c r="K40" s="126"/>
@@ -6279,7 +6279,7 @@
         <v>62</v>
       </c>
       <c r="I41" s="118" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
     </row>
     <row r="42" spans="1:26" ht="15.75" customHeight="1">
@@ -6302,7 +6302,7 @@
         <v>62</v>
       </c>
       <c r="I42" s="118" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
     </row>
     <row r="43" spans="1:26" ht="15.75" customHeight="1">
@@ -6325,7 +6325,7 @@
         <v>62</v>
       </c>
       <c r="I43" s="118" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
     </row>
     <row r="44" spans="1:26" ht="15.75" customHeight="1">
@@ -6348,7 +6348,7 @@
         <v>62</v>
       </c>
       <c r="I44" s="118" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
     </row>
     <row r="45" spans="1:26" s="79" customFormat="1">
@@ -7402,7 +7402,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1009"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="A112" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="A139" sqref="A139"/>
     </sheetView>
   </sheetViews>
@@ -7474,12 +7474,12 @@
     </row>
     <row r="2" spans="1:26" ht="19.5" customHeight="1">
       <c r="A2" s="7"/>
-      <c r="B2" s="150" t="s">
+      <c r="B2" s="152" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="145"/>
-      <c r="D2" s="145"/>
-      <c r="E2" s="151"/>
+      <c r="C2" s="153"/>
+      <c r="D2" s="153"/>
+      <c r="E2" s="154"/>
       <c r="F2" s="13"/>
       <c r="G2" s="15"/>
       <c r="H2" s="7"/>
@@ -7756,12 +7756,12 @@
     </row>
     <row r="11" spans="1:26">
       <c r="A11" s="8"/>
-      <c r="B11" s="152" t="s">
+      <c r="B11" s="155" t="s">
         <v>108</v>
       </c>
-      <c r="C11" s="153"/>
-      <c r="D11" s="153"/>
-      <c r="E11" s="154"/>
+      <c r="C11" s="156"/>
+      <c r="D11" s="156"/>
+      <c r="E11" s="157"/>
       <c r="F11" s="9"/>
       <c r="G11" s="9"/>
       <c r="H11" s="10"/>
@@ -7784,36 +7784,36 @@
       <c r="Y11" s="9"/>
       <c r="Z11" s="9"/>
     </row>
-    <row r="12" spans="1:26" s="171" customFormat="1">
+    <row r="12" spans="1:26" s="151" customFormat="1">
       <c r="A12" s="6">
         <v>6530956</v>
       </c>
       <c r="B12" s="59">
         <v>1</v>
       </c>
-      <c r="C12" s="164" t="s">
-        <v>240</v>
-      </c>
-      <c r="D12" s="165" t="s">
-        <v>241</v>
-      </c>
-      <c r="E12" s="166" t="s">
-        <v>242</v>
-      </c>
-      <c r="F12" s="167" t="s">
+      <c r="C12" s="144" t="s">
+        <v>237</v>
+      </c>
+      <c r="D12" s="145" t="s">
+        <v>238</v>
+      </c>
+      <c r="E12" s="146" t="s">
+        <v>239</v>
+      </c>
+      <c r="F12" s="147" t="s">
         <v>119</v>
       </c>
-      <c r="G12" s="168"/>
+      <c r="G12" s="148"/>
       <c r="H12" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="I12" s="169" t="s">
-        <v>26</v>
-      </c>
-      <c r="J12" s="170" t="s">
-        <v>30</v>
-      </c>
-      <c r="L12" s="171">
+      <c r="I12" s="149" t="s">
+        <v>26</v>
+      </c>
+      <c r="J12" s="150" t="s">
+        <v>30</v>
+      </c>
+      <c r="L12" s="151">
         <v>0</v>
       </c>
     </row>
@@ -8158,12 +8158,12 @@
     </row>
     <row r="24" spans="1:26" ht="15.75" customHeight="1">
       <c r="A24" s="8"/>
-      <c r="B24" s="155" t="s">
+      <c r="B24" s="158" t="s">
         <v>131</v>
       </c>
-      <c r="C24" s="148"/>
-      <c r="D24" s="148"/>
-      <c r="E24" s="149"/>
+      <c r="C24" s="159"/>
+      <c r="D24" s="159"/>
+      <c r="E24" s="160"/>
       <c r="F24" s="9"/>
       <c r="G24" s="9"/>
       <c r="H24" s="10"/>
@@ -8440,12 +8440,12 @@
     </row>
     <row r="33" spans="1:26" ht="15.75" customHeight="1">
       <c r="A33" s="38"/>
-      <c r="B33" s="156" t="s">
+      <c r="B33" s="161" t="s">
         <v>133</v>
       </c>
-      <c r="C33" s="145"/>
-      <c r="D33" s="145"/>
-      <c r="E33" s="146"/>
+      <c r="C33" s="153"/>
+      <c r="D33" s="153"/>
+      <c r="E33" s="162"/>
       <c r="F33" s="39"/>
       <c r="G33" s="40"/>
       <c r="H33" s="17"/>
@@ -8468,36 +8468,36 @@
       <c r="Y33" s="9"/>
       <c r="Z33" s="9"/>
     </row>
-    <row r="34" spans="1:26" s="171" customFormat="1">
+    <row r="34" spans="1:26" s="151" customFormat="1">
       <c r="A34" s="6">
         <v>6530968</v>
       </c>
       <c r="B34" s="59">
         <v>1</v>
       </c>
-      <c r="C34" s="164" t="s">
-        <v>240</v>
-      </c>
-      <c r="D34" s="165" t="s">
-        <v>241</v>
-      </c>
-      <c r="E34" s="166" t="s">
-        <v>242</v>
-      </c>
-      <c r="F34" s="167" t="s">
+      <c r="C34" s="144" t="s">
+        <v>237</v>
+      </c>
+      <c r="D34" s="145" t="s">
+        <v>238</v>
+      </c>
+      <c r="E34" s="146" t="s">
+        <v>239</v>
+      </c>
+      <c r="F34" s="147" t="s">
         <v>119</v>
       </c>
-      <c r="G34" s="168"/>
+      <c r="G34" s="148"/>
       <c r="H34" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="I34" s="169" t="s">
-        <v>26</v>
-      </c>
-      <c r="J34" s="170" t="s">
-        <v>30</v>
-      </c>
-      <c r="L34" s="171">
+      <c r="I34" s="149" t="s">
+        <v>26</v>
+      </c>
+      <c r="J34" s="150" t="s">
+        <v>30</v>
+      </c>
+      <c r="L34" s="151">
         <v>0</v>
       </c>
     </row>
@@ -8842,12 +8842,12 @@
     </row>
     <row r="46" spans="1:26" ht="15.75" customHeight="1">
       <c r="A46" s="8"/>
-      <c r="B46" s="147" t="s">
+      <c r="B46" s="164" t="s">
         <v>134</v>
       </c>
-      <c r="C46" s="148"/>
-      <c r="D46" s="148"/>
-      <c r="E46" s="149"/>
+      <c r="C46" s="159"/>
+      <c r="D46" s="159"/>
+      <c r="E46" s="160"/>
       <c r="F46" s="9"/>
       <c r="G46" s="9"/>
       <c r="H46" s="10"/>
@@ -9124,12 +9124,12 @@
     </row>
     <row r="55" spans="1:26" ht="15.75" customHeight="1">
       <c r="A55" s="8"/>
-      <c r="B55" s="147" t="s">
+      <c r="B55" s="164" t="s">
         <v>136</v>
       </c>
-      <c r="C55" s="148"/>
-      <c r="D55" s="148"/>
-      <c r="E55" s="149"/>
+      <c r="C55" s="159"/>
+      <c r="D55" s="159"/>
+      <c r="E55" s="160"/>
       <c r="F55" s="9"/>
       <c r="G55" s="9"/>
       <c r="H55" s="10"/>
@@ -9152,36 +9152,36 @@
       <c r="Y55" s="9"/>
       <c r="Z55" s="9"/>
     </row>
-    <row r="56" spans="1:26" s="171" customFormat="1">
+    <row r="56" spans="1:26" s="151" customFormat="1">
       <c r="A56" s="6">
         <v>6530966</v>
       </c>
       <c r="B56" s="59">
         <v>1</v>
       </c>
-      <c r="C56" s="164" t="s">
-        <v>240</v>
-      </c>
-      <c r="D56" s="165" t="s">
-        <v>241</v>
-      </c>
-      <c r="E56" s="166" t="s">
-        <v>242</v>
-      </c>
-      <c r="F56" s="167" t="s">
+      <c r="C56" s="144" t="s">
+        <v>237</v>
+      </c>
+      <c r="D56" s="145" t="s">
+        <v>238</v>
+      </c>
+      <c r="E56" s="146" t="s">
+        <v>239</v>
+      </c>
+      <c r="F56" s="147" t="s">
         <v>119</v>
       </c>
-      <c r="G56" s="168"/>
+      <c r="G56" s="148"/>
       <c r="H56" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="I56" s="169" t="s">
-        <v>26</v>
-      </c>
-      <c r="J56" s="170" t="s">
-        <v>30</v>
-      </c>
-      <c r="L56" s="171">
+      <c r="I56" s="149" t="s">
+        <v>26</v>
+      </c>
+      <c r="J56" s="150" t="s">
+        <v>30</v>
+      </c>
+      <c r="L56" s="151">
         <v>0</v>
       </c>
     </row>
@@ -9526,12 +9526,12 @@
     </row>
     <row r="68" spans="1:26" ht="15.75" customHeight="1">
       <c r="A68" s="8"/>
-      <c r="B68" s="147" t="s">
+      <c r="B68" s="164" t="s">
         <v>138</v>
       </c>
-      <c r="C68" s="148"/>
-      <c r="D68" s="148"/>
-      <c r="E68" s="149"/>
+      <c r="C68" s="159"/>
+      <c r="D68" s="159"/>
+      <c r="E68" s="160"/>
       <c r="F68" s="9"/>
       <c r="G68" s="9"/>
       <c r="H68" s="10"/>
@@ -9554,36 +9554,36 @@
       <c r="Y68" s="9"/>
       <c r="Z68" s="9"/>
     </row>
-    <row r="69" spans="1:26" s="171" customFormat="1">
+    <row r="69" spans="1:26" s="151" customFormat="1">
       <c r="A69" s="6">
         <v>6530957</v>
       </c>
       <c r="B69" s="59">
         <v>1</v>
       </c>
-      <c r="C69" s="164" t="s">
-        <v>240</v>
-      </c>
-      <c r="D69" s="165" t="s">
-        <v>241</v>
-      </c>
-      <c r="E69" s="166" t="s">
-        <v>242</v>
-      </c>
-      <c r="F69" s="167" t="s">
+      <c r="C69" s="144" t="s">
+        <v>237</v>
+      </c>
+      <c r="D69" s="145" t="s">
+        <v>238</v>
+      </c>
+      <c r="E69" s="146" t="s">
+        <v>239</v>
+      </c>
+      <c r="F69" s="147" t="s">
         <v>119</v>
       </c>
-      <c r="G69" s="168"/>
+      <c r="G69" s="148"/>
       <c r="H69" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="I69" s="169" t="s">
-        <v>26</v>
-      </c>
-      <c r="J69" s="170" t="s">
-        <v>30</v>
-      </c>
-      <c r="L69" s="171">
+      <c r="I69" s="149" t="s">
+        <v>26</v>
+      </c>
+      <c r="J69" s="150" t="s">
+        <v>30</v>
+      </c>
+      <c r="L69" s="151">
         <v>0</v>
       </c>
     </row>
@@ -9964,12 +9964,12 @@
     </row>
     <row r="82" spans="1:26" ht="15.75" customHeight="1">
       <c r="A82" s="8"/>
-      <c r="B82" s="147" t="s">
+      <c r="B82" s="164" t="s">
         <v>147</v>
       </c>
-      <c r="C82" s="148"/>
-      <c r="D82" s="148"/>
-      <c r="E82" s="149"/>
+      <c r="C82" s="159"/>
+      <c r="D82" s="159"/>
+      <c r="E82" s="160"/>
       <c r="F82" s="9"/>
       <c r="G82" s="9"/>
       <c r="H82" s="10"/>
@@ -9992,36 +9992,36 @@
       <c r="Y82" s="9"/>
       <c r="Z82" s="9"/>
     </row>
-    <row r="83" spans="1:26" s="171" customFormat="1">
+    <row r="83" spans="1:26" s="151" customFormat="1">
       <c r="A83" s="6">
         <v>6530958</v>
       </c>
       <c r="B83" s="59">
         <v>1</v>
       </c>
-      <c r="C83" s="164" t="s">
-        <v>240</v>
-      </c>
-      <c r="D83" s="165" t="s">
-        <v>241</v>
-      </c>
-      <c r="E83" s="166" t="s">
-        <v>242</v>
-      </c>
-      <c r="F83" s="167" t="s">
+      <c r="C83" s="144" t="s">
+        <v>237</v>
+      </c>
+      <c r="D83" s="145" t="s">
+        <v>238</v>
+      </c>
+      <c r="E83" s="146" t="s">
+        <v>239</v>
+      </c>
+      <c r="F83" s="147" t="s">
         <v>119</v>
       </c>
-      <c r="G83" s="168"/>
+      <c r="G83" s="148"/>
       <c r="H83" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="I83" s="169" t="s">
-        <v>26</v>
-      </c>
-      <c r="J83" s="170" t="s">
-        <v>30</v>
-      </c>
-      <c r="L83" s="171">
+      <c r="I83" s="149" t="s">
+        <v>26</v>
+      </c>
+      <c r="J83" s="150" t="s">
+        <v>30</v>
+      </c>
+      <c r="L83" s="151">
         <v>0</v>
       </c>
     </row>
@@ -10402,11 +10402,11 @@
     </row>
     <row r="96" spans="1:26" ht="15.75" customHeight="1">
       <c r="A96" s="55"/>
-      <c r="B96" s="144" t="s">
+      <c r="B96" s="163" t="s">
         <v>152</v>
       </c>
-      <c r="C96" s="145"/>
-      <c r="D96" s="146"/>
+      <c r="C96" s="153"/>
+      <c r="D96" s="162"/>
       <c r="E96" s="56"/>
       <c r="F96" s="56"/>
       <c r="G96" s="56"/>
@@ -10430,36 +10430,36 @@
       <c r="Y96" s="56"/>
       <c r="Z96" s="56"/>
     </row>
-    <row r="97" spans="1:26" s="171" customFormat="1">
+    <row r="97" spans="1:26" s="151" customFormat="1">
       <c r="A97" s="6">
         <v>6530962</v>
       </c>
       <c r="B97" s="59">
         <v>1</v>
       </c>
-      <c r="C97" s="164" t="s">
-        <v>240</v>
-      </c>
-      <c r="D97" s="165" t="s">
-        <v>241</v>
-      </c>
-      <c r="E97" s="166" t="s">
-        <v>242</v>
-      </c>
-      <c r="F97" s="167" t="s">
+      <c r="C97" s="144" t="s">
+        <v>237</v>
+      </c>
+      <c r="D97" s="145" t="s">
+        <v>238</v>
+      </c>
+      <c r="E97" s="146" t="s">
+        <v>239</v>
+      </c>
+      <c r="F97" s="147" t="s">
         <v>119</v>
       </c>
-      <c r="G97" s="168"/>
+      <c r="G97" s="148"/>
       <c r="H97" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="I97" s="169" t="s">
-        <v>26</v>
-      </c>
-      <c r="J97" s="170" t="s">
-        <v>30</v>
-      </c>
-      <c r="L97" s="171">
+      <c r="I97" s="149" t="s">
+        <v>26</v>
+      </c>
+      <c r="J97" s="150" t="s">
+        <v>30</v>
+      </c>
+      <c r="L97" s="151">
         <v>0</v>
       </c>
     </row>
@@ -10840,11 +10840,11 @@
     </row>
     <row r="110" spans="1:26" ht="15.75" customHeight="1">
       <c r="A110" s="55"/>
-      <c r="B110" s="144" t="s">
+      <c r="B110" s="163" t="s">
         <v>154</v>
       </c>
-      <c r="C110" s="145"/>
-      <c r="D110" s="146"/>
+      <c r="C110" s="153"/>
+      <c r="D110" s="162"/>
       <c r="E110" s="56"/>
       <c r="F110" s="56"/>
       <c r="G110" s="56"/>
@@ -10868,36 +10868,36 @@
       <c r="Y110" s="56"/>
       <c r="Z110" s="56"/>
     </row>
-    <row r="111" spans="1:26" s="171" customFormat="1">
+    <row r="111" spans="1:26" s="151" customFormat="1">
       <c r="A111" s="6">
         <v>6530960</v>
       </c>
       <c r="B111" s="59">
         <v>1</v>
       </c>
-      <c r="C111" s="164" t="s">
-        <v>240</v>
-      </c>
-      <c r="D111" s="165" t="s">
-        <v>241</v>
-      </c>
-      <c r="E111" s="166" t="s">
-        <v>242</v>
-      </c>
-      <c r="F111" s="167" t="s">
+      <c r="C111" s="144" t="s">
+        <v>237</v>
+      </c>
+      <c r="D111" s="145" t="s">
+        <v>238</v>
+      </c>
+      <c r="E111" s="146" t="s">
+        <v>239</v>
+      </c>
+      <c r="F111" s="147" t="s">
         <v>119</v>
       </c>
-      <c r="G111" s="168"/>
+      <c r="G111" s="148"/>
       <c r="H111" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="I111" s="169" t="s">
-        <v>26</v>
-      </c>
-      <c r="J111" s="170" t="s">
-        <v>30</v>
-      </c>
-      <c r="L111" s="171">
+      <c r="I111" s="149" t="s">
+        <v>26</v>
+      </c>
+      <c r="J111" s="150" t="s">
+        <v>30</v>
+      </c>
+      <c r="L111" s="151">
         <v>0</v>
       </c>
     </row>
@@ -11278,11 +11278,11 @@
     </row>
     <row r="124" spans="1:26" ht="15.75" customHeight="1">
       <c r="A124" s="55"/>
-      <c r="B124" s="144" t="s">
+      <c r="B124" s="163" t="s">
         <v>155</v>
       </c>
-      <c r="C124" s="145"/>
-      <c r="D124" s="146"/>
+      <c r="C124" s="153"/>
+      <c r="D124" s="162"/>
       <c r="E124" s="56"/>
       <c r="F124" s="56"/>
       <c r="G124" s="56"/>
@@ -11306,36 +11306,36 @@
       <c r="Y124" s="56"/>
       <c r="Z124" s="56"/>
     </row>
-    <row r="125" spans="1:26" s="171" customFormat="1">
+    <row r="125" spans="1:26" s="151" customFormat="1">
       <c r="A125" s="6">
         <v>6530964</v>
       </c>
       <c r="B125" s="59">
         <v>1</v>
       </c>
-      <c r="C125" s="164" t="s">
-        <v>240</v>
-      </c>
-      <c r="D125" s="165" t="s">
-        <v>241</v>
-      </c>
-      <c r="E125" s="166" t="s">
-        <v>242</v>
-      </c>
-      <c r="F125" s="167" t="s">
+      <c r="C125" s="144" t="s">
+        <v>237</v>
+      </c>
+      <c r="D125" s="145" t="s">
+        <v>238</v>
+      </c>
+      <c r="E125" s="146" t="s">
+        <v>239</v>
+      </c>
+      <c r="F125" s="147" t="s">
         <v>119</v>
       </c>
-      <c r="G125" s="168"/>
+      <c r="G125" s="148"/>
       <c r="H125" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="I125" s="169" t="s">
-        <v>26</v>
-      </c>
-      <c r="J125" s="170" t="s">
-        <v>30</v>
-      </c>
-      <c r="L125" s="171">
+      <c r="I125" s="149" t="s">
+        <v>26</v>
+      </c>
+      <c r="J125" s="150" t="s">
+        <v>30</v>
+      </c>
+      <c r="L125" s="151">
         <v>0</v>
       </c>
     </row>
@@ -11716,11 +11716,11 @@
     </row>
     <row r="138" spans="1:26" ht="15.75" customHeight="1">
       <c r="A138" s="55"/>
-      <c r="B138" s="144" t="s">
+      <c r="B138" s="163" t="s">
         <v>156</v>
       </c>
-      <c r="C138" s="145"/>
-      <c r="D138" s="146"/>
+      <c r="C138" s="153"/>
+      <c r="D138" s="162"/>
       <c r="E138" s="56"/>
       <c r="F138" s="56"/>
       <c r="G138" s="56"/>
@@ -11744,36 +11744,36 @@
       <c r="Y138" s="56"/>
       <c r="Z138" s="56"/>
     </row>
-    <row r="139" spans="1:26" s="171" customFormat="1">
+    <row r="139" spans="1:26" s="151" customFormat="1">
       <c r="A139" s="6">
         <v>6530959</v>
       </c>
       <c r="B139" s="59">
         <v>1</v>
       </c>
-      <c r="C139" s="164" t="s">
-        <v>240</v>
-      </c>
-      <c r="D139" s="165" t="s">
-        <v>241</v>
-      </c>
-      <c r="E139" s="166" t="s">
-        <v>242</v>
-      </c>
-      <c r="F139" s="167" t="s">
+      <c r="C139" s="144" t="s">
+        <v>237</v>
+      </c>
+      <c r="D139" s="145" t="s">
+        <v>238</v>
+      </c>
+      <c r="E139" s="146" t="s">
+        <v>239</v>
+      </c>
+      <c r="F139" s="147" t="s">
         <v>119</v>
       </c>
-      <c r="G139" s="168"/>
+      <c r="G139" s="148"/>
       <c r="H139" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="I139" s="169" t="s">
-        <v>26</v>
-      </c>
-      <c r="J139" s="170" t="s">
-        <v>30</v>
-      </c>
-      <c r="L139" s="171">
+      <c r="I139" s="149" t="s">
+        <v>26</v>
+      </c>
+      <c r="J139" s="150" t="s">
+        <v>30</v>
+      </c>
+      <c r="L139" s="151">
         <v>0</v>
       </c>
     </row>
@@ -15586,11 +15586,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="B33:E33"/>
-    <mergeCell ref="B110:D110"/>
     <mergeCell ref="B124:D124"/>
     <mergeCell ref="B138:D138"/>
     <mergeCell ref="B46:E46"/>
@@ -15598,6 +15593,11 @@
     <mergeCell ref="B82:E82"/>
     <mergeCell ref="B68:E68"/>
     <mergeCell ref="B55:E55"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="B33:E33"/>
+    <mergeCell ref="B110:D110"/>
   </mergeCells>
   <conditionalFormatting sqref="H3">
     <cfRule type="cellIs" dxfId="419" priority="31" operator="equal">
@@ -17161,11 +17161,11 @@
     </row>
     <row r="2" spans="1:26">
       <c r="A2" s="8"/>
-      <c r="B2" s="157" t="s">
+      <c r="B2" s="165" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="158"/>
-      <c r="D2" s="159"/>
+      <c r="C2" s="166"/>
+      <c r="D2" s="167"/>
       <c r="E2" s="9"/>
       <c r="F2" s="9"/>
       <c r="G2" s="9"/>
@@ -17377,11 +17377,11 @@
     </row>
     <row r="10" spans="1:26">
       <c r="A10" s="8"/>
-      <c r="B10" s="157" t="s">
+      <c r="B10" s="165" t="s">
         <v>49</v>
       </c>
-      <c r="C10" s="158"/>
-      <c r="D10" s="159"/>
+      <c r="C10" s="166"/>
+      <c r="D10" s="167"/>
       <c r="E10" s="9"/>
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
@@ -17593,11 +17593,11 @@
     </row>
     <row r="18" spans="1:26">
       <c r="A18" s="8"/>
-      <c r="B18" s="157" t="s">
+      <c r="B18" s="165" t="s">
         <v>64</v>
       </c>
-      <c r="C18" s="158"/>
-      <c r="D18" s="159"/>
+      <c r="C18" s="166"/>
+      <c r="D18" s="167"/>
       <c r="E18" s="9"/>
       <c r="F18" s="9"/>
       <c r="G18" s="9"/>
@@ -17809,11 +17809,11 @@
     </row>
     <row r="26" spans="1:26" ht="15.75" customHeight="1">
       <c r="A26" s="8"/>
-      <c r="B26" s="157" t="s">
+      <c r="B26" s="165" t="s">
         <v>70</v>
       </c>
-      <c r="C26" s="158"/>
-      <c r="D26" s="159"/>
+      <c r="C26" s="166"/>
+      <c r="D26" s="167"/>
       <c r="E26" s="9"/>
       <c r="F26" s="9"/>
       <c r="G26" s="9"/>
@@ -18025,11 +18025,11 @@
     </row>
     <row r="34" spans="1:26" ht="15.75" customHeight="1">
       <c r="A34" s="8"/>
-      <c r="B34" s="157" t="s">
+      <c r="B34" s="165" t="s">
         <v>95</v>
       </c>
-      <c r="C34" s="158"/>
-      <c r="D34" s="159"/>
+      <c r="C34" s="166"/>
+      <c r="D34" s="167"/>
       <c r="E34" s="9"/>
       <c r="F34" s="9"/>
       <c r="G34" s="9"/>
@@ -18235,11 +18235,11 @@
     </row>
     <row r="42" spans="1:26" ht="15.75" customHeight="1">
       <c r="A42" s="8"/>
-      <c r="B42" s="157" t="s">
+      <c r="B42" s="165" t="s">
         <v>110</v>
       </c>
-      <c r="C42" s="158"/>
-      <c r="D42" s="159"/>
+      <c r="C42" s="166"/>
+      <c r="D42" s="167"/>
       <c r="E42" s="9"/>
       <c r="F42" s="9"/>
       <c r="G42" s="9"/>
@@ -22257,362 +22257,362 @@
     <mergeCell ref="B34:D34"/>
   </mergeCells>
   <conditionalFormatting sqref="H8">
-    <cfRule type="cellIs" dxfId="174" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="173" priority="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H8">
-    <cfRule type="cellIs" dxfId="173" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="172" priority="2" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H8">
-    <cfRule type="cellIs" dxfId="172" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="171" priority="3" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6">
-    <cfRule type="cellIs" dxfId="171" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="170" priority="4" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6">
-    <cfRule type="cellIs" dxfId="170" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="169" priority="5" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6">
-    <cfRule type="cellIs" dxfId="169" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="168" priority="6" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7">
-    <cfRule type="cellIs" dxfId="168" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="167" priority="7" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7">
-    <cfRule type="cellIs" dxfId="167" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="166" priority="8" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7">
-    <cfRule type="cellIs" dxfId="166" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="165" priority="9" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16">
-    <cfRule type="cellIs" dxfId="165" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="164" priority="10" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16">
-    <cfRule type="cellIs" dxfId="164" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="163" priority="11" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16">
-    <cfRule type="cellIs" dxfId="163" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="162" priority="12" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H14">
-    <cfRule type="cellIs" dxfId="162" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="161" priority="13" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H14">
-    <cfRule type="cellIs" dxfId="161" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="160" priority="14" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H14">
-    <cfRule type="cellIs" dxfId="160" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="159" priority="15" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H15">
-    <cfRule type="cellIs" dxfId="159" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="158" priority="16" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H15">
-    <cfRule type="cellIs" dxfId="158" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="157" priority="17" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H15">
-    <cfRule type="cellIs" dxfId="157" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="156" priority="18" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H24">
-    <cfRule type="cellIs" dxfId="156" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="155" priority="19" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H24">
-    <cfRule type="cellIs" dxfId="155" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="154" priority="20" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H24">
-    <cfRule type="cellIs" dxfId="154" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="153" priority="21" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H22">
-    <cfRule type="cellIs" dxfId="153" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="152" priority="22" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H22">
-    <cfRule type="cellIs" dxfId="152" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="151" priority="23" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H22">
-    <cfRule type="cellIs" dxfId="151" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="150" priority="24" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H23">
-    <cfRule type="cellIs" dxfId="150" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="149" priority="25" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H23">
-    <cfRule type="cellIs" dxfId="149" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="148" priority="26" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H23">
-    <cfRule type="cellIs" dxfId="148" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="147" priority="27" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H32">
-    <cfRule type="cellIs" dxfId="147" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="146" priority="28" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H32">
-    <cfRule type="cellIs" dxfId="146" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="145" priority="29" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H32">
-    <cfRule type="cellIs" dxfId="145" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="144" priority="30" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H30">
-    <cfRule type="cellIs" dxfId="144" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="143" priority="31" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H30">
-    <cfRule type="cellIs" dxfId="143" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="142" priority="32" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H30">
-    <cfRule type="cellIs" dxfId="142" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="141" priority="33" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H31">
-    <cfRule type="cellIs" dxfId="141" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="140" priority="34" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H31">
-    <cfRule type="cellIs" dxfId="140" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="139" priority="35" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H31">
-    <cfRule type="cellIs" dxfId="139" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="138" priority="36" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H40">
-    <cfRule type="cellIs" dxfId="138" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="137" priority="37" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H40">
-    <cfRule type="cellIs" dxfId="137" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="136" priority="38" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H40">
-    <cfRule type="cellIs" dxfId="136" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="135" priority="39" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H38">
-    <cfRule type="cellIs" dxfId="135" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="134" priority="40" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H38">
-    <cfRule type="cellIs" dxfId="134" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="133" priority="41" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H38">
-    <cfRule type="cellIs" dxfId="133" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="132" priority="42" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H39">
-    <cfRule type="cellIs" dxfId="132" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="131" priority="43" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H39">
-    <cfRule type="cellIs" dxfId="131" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="130" priority="44" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H39">
-    <cfRule type="cellIs" dxfId="130" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="129" priority="45" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H48">
-    <cfRule type="cellIs" dxfId="129" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="128" priority="46" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H48">
-    <cfRule type="cellIs" dxfId="128" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="127" priority="47" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H48">
-    <cfRule type="cellIs" dxfId="127" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="126" priority="48" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H46">
-    <cfRule type="cellIs" dxfId="126" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="125" priority="49" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H46">
-    <cfRule type="cellIs" dxfId="125" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="124" priority="50" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H46">
-    <cfRule type="cellIs" dxfId="124" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="123" priority="51" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H47">
-    <cfRule type="cellIs" dxfId="123" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="122" priority="52" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H47">
-    <cfRule type="cellIs" dxfId="122" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="121" priority="53" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H47">
-    <cfRule type="cellIs" dxfId="121" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="120" priority="54" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H13">
-    <cfRule type="cellIs" dxfId="120" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="119" priority="55" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H13">
-    <cfRule type="cellIs" dxfId="119" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="118" priority="56" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H13">
-    <cfRule type="cellIs" dxfId="118" priority="57" operator="equal">
+    <cfRule type="cellIs" dxfId="117" priority="57" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H21">
-    <cfRule type="cellIs" dxfId="117" priority="58" operator="equal">
+    <cfRule type="cellIs" dxfId="116" priority="58" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H21">
-    <cfRule type="cellIs" dxfId="116" priority="59" operator="equal">
+    <cfRule type="cellIs" dxfId="115" priority="59" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H21">
-    <cfRule type="cellIs" dxfId="115" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="114" priority="60" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H29">
-    <cfRule type="cellIs" dxfId="114" priority="61" operator="equal">
+    <cfRule type="cellIs" dxfId="113" priority="61" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H29">
-    <cfRule type="cellIs" dxfId="113" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="112" priority="62" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H29">
-    <cfRule type="cellIs" dxfId="112" priority="63" operator="equal">
+    <cfRule type="cellIs" dxfId="111" priority="63" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H37">
-    <cfRule type="cellIs" dxfId="111" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="110" priority="64" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H37">
-    <cfRule type="cellIs" dxfId="110" priority="65" operator="equal">
+    <cfRule type="cellIs" dxfId="109" priority="65" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H37">
-    <cfRule type="cellIs" dxfId="109" priority="66" operator="equal">
+    <cfRule type="cellIs" dxfId="108" priority="66" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H45">
-    <cfRule type="cellIs" dxfId="108" priority="67" operator="equal">
+    <cfRule type="cellIs" dxfId="107" priority="67" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H45">
-    <cfRule type="cellIs" dxfId="107" priority="68" operator="equal">
+    <cfRule type="cellIs" dxfId="106" priority="68" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H45">
-    <cfRule type="cellIs" dxfId="106" priority="69" operator="equal">
+    <cfRule type="cellIs" dxfId="105" priority="69" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5">
-    <cfRule type="cellIs" dxfId="105" priority="70" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="70" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5">
-    <cfRule type="cellIs" dxfId="104" priority="71" operator="equal">
+    <cfRule type="cellIs" dxfId="103" priority="71" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5">
-    <cfRule type="cellIs" dxfId="103" priority="72" operator="equal">
+    <cfRule type="cellIs" dxfId="102" priority="72" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
@@ -22703,16 +22703,16 @@
     <row r="2" spans="1:26">
       <c r="A2" s="44"/>
       <c r="B2" s="45"/>
-      <c r="C2" s="160" t="s">
+      <c r="C2" s="168" t="s">
         <v>61</v>
       </c>
-      <c r="D2" s="145"/>
-      <c r="E2" s="145"/>
-      <c r="F2" s="145"/>
-      <c r="G2" s="145"/>
-      <c r="H2" s="145"/>
-      <c r="I2" s="145"/>
-      <c r="J2" s="151"/>
+      <c r="D2" s="153"/>
+      <c r="E2" s="153"/>
+      <c r="F2" s="153"/>
+      <c r="G2" s="153"/>
+      <c r="H2" s="153"/>
+      <c r="I2" s="153"/>
+      <c r="J2" s="154"/>
       <c r="K2" s="45"/>
       <c r="L2" s="46"/>
       <c r="M2" s="47"/>
@@ -22887,16 +22887,16 @@
     <row r="7" spans="1:26">
       <c r="A7" s="44"/>
       <c r="B7" s="45"/>
-      <c r="C7" s="160" t="s">
+      <c r="C7" s="168" t="s">
         <v>65</v>
       </c>
-      <c r="D7" s="145"/>
-      <c r="E7" s="145"/>
-      <c r="F7" s="145"/>
-      <c r="G7" s="145"/>
-      <c r="H7" s="145"/>
-      <c r="I7" s="145"/>
-      <c r="J7" s="151"/>
+      <c r="D7" s="153"/>
+      <c r="E7" s="153"/>
+      <c r="F7" s="153"/>
+      <c r="G7" s="153"/>
+      <c r="H7" s="153"/>
+      <c r="I7" s="153"/>
+      <c r="J7" s="154"/>
       <c r="K7" s="45"/>
       <c r="L7" s="46"/>
       <c r="M7" s="47"/>
@@ -23071,16 +23071,16 @@
     <row r="12" spans="1:26">
       <c r="A12" s="44"/>
       <c r="B12" s="45"/>
-      <c r="C12" s="160" t="s">
+      <c r="C12" s="168" t="s">
         <v>66</v>
       </c>
-      <c r="D12" s="145"/>
-      <c r="E12" s="145"/>
-      <c r="F12" s="145"/>
-      <c r="G12" s="145"/>
-      <c r="H12" s="145"/>
-      <c r="I12" s="145"/>
-      <c r="J12" s="151"/>
+      <c r="D12" s="153"/>
+      <c r="E12" s="153"/>
+      <c r="F12" s="153"/>
+      <c r="G12" s="153"/>
+      <c r="H12" s="153"/>
+      <c r="I12" s="153"/>
+      <c r="J12" s="154"/>
       <c r="K12" s="45"/>
       <c r="L12" s="46"/>
       <c r="M12" s="47"/>
@@ -23255,16 +23255,16 @@
     <row r="17" spans="1:26">
       <c r="A17" s="44"/>
       <c r="B17" s="45"/>
-      <c r="C17" s="160" t="s">
+      <c r="C17" s="168" t="s">
         <v>69</v>
       </c>
-      <c r="D17" s="145"/>
-      <c r="E17" s="145"/>
-      <c r="F17" s="145"/>
-      <c r="G17" s="145"/>
-      <c r="H17" s="145"/>
-      <c r="I17" s="145"/>
-      <c r="J17" s="151"/>
+      <c r="D17" s="153"/>
+      <c r="E17" s="153"/>
+      <c r="F17" s="153"/>
+      <c r="G17" s="153"/>
+      <c r="H17" s="153"/>
+      <c r="I17" s="153"/>
+      <c r="J17" s="154"/>
       <c r="K17" s="45"/>
       <c r="L17" s="46"/>
       <c r="M17" s="47"/>
@@ -23439,16 +23439,16 @@
     <row r="22" spans="1:26" ht="15.75" customHeight="1">
       <c r="A22" s="44"/>
       <c r="B22" s="45"/>
-      <c r="C22" s="160" t="s">
+      <c r="C22" s="168" t="s">
         <v>79</v>
       </c>
-      <c r="D22" s="145"/>
-      <c r="E22" s="145"/>
-      <c r="F22" s="145"/>
-      <c r="G22" s="145"/>
-      <c r="H22" s="145"/>
-      <c r="I22" s="145"/>
-      <c r="J22" s="151"/>
+      <c r="D22" s="153"/>
+      <c r="E22" s="153"/>
+      <c r="F22" s="153"/>
+      <c r="G22" s="153"/>
+      <c r="H22" s="153"/>
+      <c r="I22" s="153"/>
+      <c r="J22" s="154"/>
       <c r="K22" s="45"/>
       <c r="L22" s="46"/>
       <c r="M22" s="47"/>
@@ -23613,16 +23613,16 @@
     <row r="27" spans="1:26" ht="15.75" customHeight="1">
       <c r="A27" s="44"/>
       <c r="B27" s="45"/>
-      <c r="C27" s="160" t="s">
+      <c r="C27" s="168" t="s">
         <v>83</v>
       </c>
-      <c r="D27" s="145"/>
-      <c r="E27" s="145"/>
-      <c r="F27" s="145"/>
-      <c r="G27" s="145"/>
-      <c r="H27" s="145"/>
-      <c r="I27" s="145"/>
-      <c r="J27" s="151"/>
+      <c r="D27" s="153"/>
+      <c r="E27" s="153"/>
+      <c r="F27" s="153"/>
+      <c r="G27" s="153"/>
+      <c r="H27" s="153"/>
+      <c r="I27" s="153"/>
+      <c r="J27" s="154"/>
       <c r="K27" s="45"/>
       <c r="L27" s="46"/>
       <c r="M27" s="47"/>
@@ -23797,16 +23797,16 @@
     <row r="32" spans="1:26" ht="15.75" customHeight="1">
       <c r="A32" s="44"/>
       <c r="B32" s="45"/>
-      <c r="C32" s="160" t="s">
+      <c r="C32" s="168" t="s">
         <v>84</v>
       </c>
-      <c r="D32" s="145"/>
-      <c r="E32" s="145"/>
-      <c r="F32" s="145"/>
-      <c r="G32" s="145"/>
-      <c r="H32" s="145"/>
-      <c r="I32" s="145"/>
-      <c r="J32" s="151"/>
+      <c r="D32" s="153"/>
+      <c r="E32" s="153"/>
+      <c r="F32" s="153"/>
+      <c r="G32" s="153"/>
+      <c r="H32" s="153"/>
+      <c r="I32" s="153"/>
+      <c r="J32" s="154"/>
       <c r="K32" s="45"/>
       <c r="L32" s="46"/>
       <c r="M32" s="47"/>
@@ -23981,16 +23981,16 @@
     <row r="37" spans="1:26" ht="15.75" customHeight="1">
       <c r="A37" s="44"/>
       <c r="B37" s="45"/>
-      <c r="C37" s="160" t="s">
+      <c r="C37" s="168" t="s">
         <v>87</v>
       </c>
-      <c r="D37" s="145"/>
-      <c r="E37" s="145"/>
-      <c r="F37" s="145"/>
-      <c r="G37" s="145"/>
-      <c r="H37" s="145"/>
-      <c r="I37" s="145"/>
-      <c r="J37" s="151"/>
+      <c r="D37" s="153"/>
+      <c r="E37" s="153"/>
+      <c r="F37" s="153"/>
+      <c r="G37" s="153"/>
+      <c r="H37" s="153"/>
+      <c r="I37" s="153"/>
+      <c r="J37" s="154"/>
       <c r="K37" s="45"/>
       <c r="L37" s="46"/>
       <c r="M37" s="47"/>
@@ -24165,16 +24165,16 @@
     <row r="42" spans="1:26" ht="15.75" customHeight="1">
       <c r="A42" s="44"/>
       <c r="B42" s="45"/>
-      <c r="C42" s="160" t="s">
+      <c r="C42" s="168" t="s">
         <v>112</v>
       </c>
-      <c r="D42" s="145"/>
-      <c r="E42" s="145"/>
-      <c r="F42" s="145"/>
-      <c r="G42" s="145"/>
-      <c r="H42" s="145"/>
-      <c r="I42" s="145"/>
-      <c r="J42" s="151"/>
+      <c r="D42" s="153"/>
+      <c r="E42" s="153"/>
+      <c r="F42" s="153"/>
+      <c r="G42" s="153"/>
+      <c r="H42" s="153"/>
+      <c r="I42" s="153"/>
+      <c r="J42" s="154"/>
       <c r="K42" s="45"/>
       <c r="L42" s="46"/>
       <c r="M42" s="47"/>
@@ -24349,16 +24349,16 @@
     <row r="47" spans="1:26" ht="15.75" customHeight="1">
       <c r="A47" s="44"/>
       <c r="B47" s="45"/>
-      <c r="C47" s="160" t="s">
+      <c r="C47" s="168" t="s">
         <v>113</v>
       </c>
-      <c r="D47" s="145"/>
-      <c r="E47" s="145"/>
-      <c r="F47" s="145"/>
-      <c r="G47" s="145"/>
-      <c r="H47" s="145"/>
-      <c r="I47" s="145"/>
-      <c r="J47" s="151"/>
+      <c r="D47" s="153"/>
+      <c r="E47" s="153"/>
+      <c r="F47" s="153"/>
+      <c r="G47" s="153"/>
+      <c r="H47" s="153"/>
+      <c r="I47" s="153"/>
+      <c r="J47" s="154"/>
       <c r="K47" s="45"/>
       <c r="L47" s="46"/>
       <c r="M47" s="47"/>
@@ -24533,16 +24533,16 @@
     <row r="52" spans="1:26" ht="15.75" customHeight="1">
       <c r="A52" s="44"/>
       <c r="B52" s="45"/>
-      <c r="C52" s="160" t="s">
+      <c r="C52" s="168" t="s">
         <v>114</v>
       </c>
-      <c r="D52" s="145"/>
-      <c r="E52" s="145"/>
-      <c r="F52" s="145"/>
-      <c r="G52" s="145"/>
-      <c r="H52" s="145"/>
-      <c r="I52" s="145"/>
-      <c r="J52" s="151"/>
+      <c r="D52" s="153"/>
+      <c r="E52" s="153"/>
+      <c r="F52" s="153"/>
+      <c r="G52" s="153"/>
+      <c r="H52" s="153"/>
+      <c r="I52" s="153"/>
+      <c r="J52" s="154"/>
       <c r="K52" s="45"/>
       <c r="L52" s="46"/>
       <c r="M52" s="47"/>
@@ -24717,16 +24717,16 @@
     <row r="57" spans="1:26" ht="15.75" customHeight="1">
       <c r="A57" s="44"/>
       <c r="B57" s="45"/>
-      <c r="C57" s="160" t="s">
+      <c r="C57" s="168" t="s">
         <v>116</v>
       </c>
-      <c r="D57" s="145"/>
-      <c r="E57" s="145"/>
-      <c r="F57" s="145"/>
-      <c r="G57" s="145"/>
-      <c r="H57" s="145"/>
-      <c r="I57" s="145"/>
-      <c r="J57" s="151"/>
+      <c r="D57" s="153"/>
+      <c r="E57" s="153"/>
+      <c r="F57" s="153"/>
+      <c r="G57" s="153"/>
+      <c r="H57" s="153"/>
+      <c r="I57" s="153"/>
+      <c r="J57" s="154"/>
       <c r="K57" s="45"/>
       <c r="L57" s="46"/>
       <c r="M57" s="47"/>
@@ -51192,11 +51192,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="C37:J37"/>
-    <mergeCell ref="C47:J47"/>
-    <mergeCell ref="C52:J52"/>
-    <mergeCell ref="C57:J57"/>
-    <mergeCell ref="C42:J42"/>
     <mergeCell ref="C22:J22"/>
     <mergeCell ref="C27:J27"/>
     <mergeCell ref="C32:J32"/>
@@ -51204,109 +51199,114 @@
     <mergeCell ref="C7:J7"/>
     <mergeCell ref="C12:J12"/>
     <mergeCell ref="C17:J17"/>
+    <mergeCell ref="C37:J37"/>
+    <mergeCell ref="C47:J47"/>
+    <mergeCell ref="C52:J52"/>
+    <mergeCell ref="C57:J57"/>
+    <mergeCell ref="C42:J42"/>
   </mergeCells>
   <conditionalFormatting sqref="H65">
-    <cfRule type="cellIs" dxfId="102" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="101" priority="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H65">
-    <cfRule type="cellIs" dxfId="101" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="100" priority="2" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H65">
-    <cfRule type="cellIs" dxfId="100" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="99" priority="3" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H63">
-    <cfRule type="cellIs" dxfId="99" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="98" priority="4" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H63">
-    <cfRule type="cellIs" dxfId="98" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="97" priority="5" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H63">
-    <cfRule type="cellIs" dxfId="97" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="6" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H64">
-    <cfRule type="cellIs" dxfId="96" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="7" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H64">
-    <cfRule type="cellIs" dxfId="95" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="8" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H64">
-    <cfRule type="cellIs" dxfId="94" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="93" priority="9" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H61">
-    <cfRule type="cellIs" dxfId="93" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="10" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H61">
-    <cfRule type="cellIs" dxfId="92" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="11" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H61">
-    <cfRule type="cellIs" dxfId="91" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="90" priority="12" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H62">
-    <cfRule type="cellIs" dxfId="90" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="13" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H62">
-    <cfRule type="cellIs" dxfId="89" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="14" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H62">
-    <cfRule type="cellIs" dxfId="88" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="15" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6">
-    <cfRule type="cellIs" dxfId="87" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="16" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6">
-    <cfRule type="cellIs" dxfId="86" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="17" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6">
-    <cfRule type="cellIs" dxfId="85" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="18" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H26">
-    <cfRule type="cellIs" dxfId="84" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="19" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H26">
-    <cfRule type="cellIs" dxfId="83" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="20" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H26">
-    <cfRule type="cellIs" dxfId="82" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="21" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
@@ -51384,16 +51384,16 @@
     <row r="2" spans="1:26" s="99" customFormat="1">
       <c r="A2" s="94"/>
       <c r="B2" s="95"/>
-      <c r="C2" s="161" t="s">
+      <c r="C2" s="169" t="s">
         <v>209</v>
       </c>
-      <c r="D2" s="162"/>
-      <c r="E2" s="162"/>
-      <c r="F2" s="162"/>
-      <c r="G2" s="162"/>
-      <c r="H2" s="162"/>
-      <c r="I2" s="162"/>
-      <c r="J2" s="162"/>
+      <c r="D2" s="170"/>
+      <c r="E2" s="170"/>
+      <c r="F2" s="170"/>
+      <c r="G2" s="170"/>
+      <c r="H2" s="170"/>
+      <c r="I2" s="170"/>
+      <c r="J2" s="170"/>
       <c r="K2" s="96"/>
       <c r="L2" s="97"/>
       <c r="M2" s="98"/>
@@ -52374,16 +52374,16 @@
     <row r="36" spans="1:12" ht="15" customHeight="1">
       <c r="A36" s="94"/>
       <c r="B36" s="95"/>
-      <c r="C36" s="161" t="s">
+      <c r="C36" s="169" t="s">
         <v>212</v>
       </c>
-      <c r="D36" s="162"/>
-      <c r="E36" s="162"/>
-      <c r="F36" s="162"/>
-      <c r="G36" s="162"/>
-      <c r="H36" s="162"/>
-      <c r="I36" s="162"/>
-      <c r="J36" s="162"/>
+      <c r="D36" s="170"/>
+      <c r="E36" s="170"/>
+      <c r="F36" s="170"/>
+      <c r="G36" s="170"/>
+      <c r="H36" s="170"/>
+      <c r="I36" s="170"/>
+      <c r="J36" s="170"/>
       <c r="K36" s="96"/>
       <c r="L36" s="97"/>
     </row>
@@ -53391,16 +53391,16 @@
     <row r="70" spans="1:26" ht="15" customHeight="1">
       <c r="A70" s="94"/>
       <c r="B70" s="95"/>
-      <c r="C70" s="161" t="s">
+      <c r="C70" s="169" t="s">
         <v>223</v>
       </c>
-      <c r="D70" s="162"/>
-      <c r="E70" s="162"/>
-      <c r="F70" s="162"/>
-      <c r="G70" s="162"/>
-      <c r="H70" s="162"/>
-      <c r="I70" s="162"/>
-      <c r="J70" s="162"/>
+      <c r="D70" s="170"/>
+      <c r="E70" s="170"/>
+      <c r="F70" s="170"/>
+      <c r="G70" s="170"/>
+      <c r="H70" s="170"/>
+      <c r="I70" s="170"/>
+      <c r="J70" s="170"/>
       <c r="K70" s="96"/>
       <c r="L70" s="97"/>
     </row>
@@ -54442,16 +54442,16 @@
     <row r="106" spans="1:26" ht="15" customHeight="1">
       <c r="A106" s="94"/>
       <c r="B106" s="95"/>
-      <c r="C106" s="161" t="s">
+      <c r="C106" s="169" t="s">
         <v>227</v>
       </c>
-      <c r="D106" s="162"/>
-      <c r="E106" s="162"/>
-      <c r="F106" s="162"/>
-      <c r="G106" s="162"/>
-      <c r="H106" s="162"/>
-      <c r="I106" s="162"/>
-      <c r="J106" s="162"/>
+      <c r="D106" s="170"/>
+      <c r="E106" s="170"/>
+      <c r="F106" s="170"/>
+      <c r="G106" s="170"/>
+      <c r="H106" s="170"/>
+      <c r="I106" s="170"/>
+      <c r="J106" s="170"/>
       <c r="K106" s="96"/>
       <c r="L106" s="97"/>
     </row>
@@ -55493,16 +55493,16 @@
     <row r="142" spans="1:12" ht="15" customHeight="1">
       <c r="A142" s="94"/>
       <c r="B142" s="95"/>
-      <c r="C142" s="163" t="s">
+      <c r="C142" s="171" t="s">
         <v>217</v>
       </c>
-      <c r="D142" s="162"/>
-      <c r="E142" s="162"/>
-      <c r="F142" s="162"/>
-      <c r="G142" s="162"/>
-      <c r="H142" s="162"/>
-      <c r="I142" s="162"/>
-      <c r="J142" s="162"/>
+      <c r="D142" s="170"/>
+      <c r="E142" s="170"/>
+      <c r="F142" s="170"/>
+      <c r="G142" s="170"/>
+      <c r="H142" s="170"/>
+      <c r="I142" s="170"/>
+      <c r="J142" s="170"/>
       <c r="K142" s="96"/>
       <c r="L142" s="97"/>
     </row>
@@ -56467,16 +56467,16 @@
     <row r="177" spans="1:12" ht="15" customHeight="1">
       <c r="A177" s="94"/>
       <c r="B177" s="95"/>
-      <c r="C177" s="163" t="s">
+      <c r="C177" s="171" t="s">
         <v>219</v>
       </c>
-      <c r="D177" s="162"/>
-      <c r="E177" s="162"/>
-      <c r="F177" s="162"/>
-      <c r="G177" s="162"/>
-      <c r="H177" s="162"/>
-      <c r="I177" s="162"/>
-      <c r="J177" s="162"/>
+      <c r="D177" s="170"/>
+      <c r="E177" s="170"/>
+      <c r="F177" s="170"/>
+      <c r="G177" s="170"/>
+      <c r="H177" s="170"/>
+      <c r="I177" s="170"/>
+      <c r="J177" s="170"/>
       <c r="K177" s="96"/>
       <c r="L177" s="97"/>
     </row>
@@ -57439,16 +57439,16 @@
     <row r="213" spans="1:12" ht="15" customHeight="1">
       <c r="A213" s="94"/>
       <c r="B213" s="95"/>
-      <c r="C213" s="161" t="s">
+      <c r="C213" s="169" t="s">
         <v>232</v>
       </c>
-      <c r="D213" s="162"/>
-      <c r="E213" s="162"/>
-      <c r="F213" s="162"/>
-      <c r="G213" s="162"/>
-      <c r="H213" s="162"/>
-      <c r="I213" s="162"/>
-      <c r="J213" s="162"/>
+      <c r="D213" s="170"/>
+      <c r="E213" s="170"/>
+      <c r="F213" s="170"/>
+      <c r="G213" s="170"/>
+      <c r="H213" s="170"/>
+      <c r="I213" s="170"/>
+      <c r="J213" s="170"/>
       <c r="K213" s="96"/>
       <c r="L213" s="97"/>
     </row>
@@ -58477,16 +58477,16 @@
     <row r="250" spans="1:12" ht="15" customHeight="1">
       <c r="A250" s="94"/>
       <c r="B250" s="95"/>
-      <c r="C250" s="161" t="s">
+      <c r="C250" s="169" t="s">
         <v>233</v>
       </c>
-      <c r="D250" s="162"/>
-      <c r="E250" s="162"/>
-      <c r="F250" s="162"/>
-      <c r="G250" s="162"/>
-      <c r="H250" s="162"/>
-      <c r="I250" s="162"/>
-      <c r="J250" s="162"/>
+      <c r="D250" s="170"/>
+      <c r="E250" s="170"/>
+      <c r="F250" s="170"/>
+      <c r="G250" s="170"/>
+      <c r="H250" s="170"/>
+      <c r="I250" s="170"/>
+      <c r="J250" s="170"/>
       <c r="K250" s="96"/>
       <c r="L250" s="97"/>
     </row>
@@ -59520,16 +59520,16 @@
     <row r="323" spans="1:12" ht="15" customHeight="1">
       <c r="A323" s="94"/>
       <c r="B323" s="95"/>
-      <c r="C323" s="163" t="s">
+      <c r="C323" s="171" t="s">
         <v>220</v>
       </c>
-      <c r="D323" s="162"/>
-      <c r="E323" s="162"/>
-      <c r="F323" s="162"/>
-      <c r="G323" s="162"/>
-      <c r="H323" s="162"/>
-      <c r="I323" s="162"/>
-      <c r="J323" s="162"/>
+      <c r="D323" s="170"/>
+      <c r="E323" s="170"/>
+      <c r="F323" s="170"/>
+      <c r="G323" s="170"/>
+      <c r="H323" s="170"/>
+      <c r="I323" s="170"/>
+      <c r="J323" s="170"/>
       <c r="K323" s="96"/>
       <c r="L323" s="97"/>
     </row>
@@ -60494,16 +60494,16 @@
     <row r="359" spans="1:12" ht="15" customHeight="1">
       <c r="A359" s="94"/>
       <c r="B359" s="95"/>
-      <c r="C359" s="163" t="s">
+      <c r="C359" s="171" t="s">
         <v>221</v>
       </c>
-      <c r="D359" s="162"/>
-      <c r="E359" s="162"/>
-      <c r="F359" s="162"/>
-      <c r="G359" s="162"/>
-      <c r="H359" s="162"/>
-      <c r="I359" s="162"/>
-      <c r="J359" s="162"/>
+      <c r="D359" s="170"/>
+      <c r="E359" s="170"/>
+      <c r="F359" s="170"/>
+      <c r="G359" s="170"/>
+      <c r="H359" s="170"/>
+      <c r="I359" s="170"/>
+      <c r="J359" s="170"/>
       <c r="K359" s="96"/>
       <c r="L359" s="97"/>
     </row>
@@ -61465,16 +61465,16 @@
     <row r="395" spans="1:12" ht="15" customHeight="1">
       <c r="A395" s="94"/>
       <c r="B395" s="95"/>
-      <c r="C395" s="161" t="s">
+      <c r="C395" s="169" t="s">
         <v>230</v>
       </c>
-      <c r="D395" s="162"/>
-      <c r="E395" s="162"/>
-      <c r="F395" s="162"/>
-      <c r="G395" s="162"/>
-      <c r="H395" s="162"/>
-      <c r="I395" s="162"/>
-      <c r="J395" s="162"/>
+      <c r="D395" s="170"/>
+      <c r="E395" s="170"/>
+      <c r="F395" s="170"/>
+      <c r="G395" s="170"/>
+      <c r="H395" s="170"/>
+      <c r="I395" s="170"/>
+      <c r="J395" s="170"/>
       <c r="K395" s="96"/>
       <c r="L395" s="97"/>
     </row>
@@ -62502,16 +62502,16 @@
     <row r="431" spans="1:12" ht="15" customHeight="1">
       <c r="A431" s="94"/>
       <c r="B431" s="95"/>
-      <c r="C431" s="161" t="s">
+      <c r="C431" s="169" t="s">
         <v>231</v>
       </c>
-      <c r="D431" s="162"/>
-      <c r="E431" s="162"/>
-      <c r="F431" s="162"/>
-      <c r="G431" s="162"/>
-      <c r="H431" s="162"/>
-      <c r="I431" s="162"/>
-      <c r="J431" s="162"/>
+      <c r="D431" s="170"/>
+      <c r="E431" s="170"/>
+      <c r="F431" s="170"/>
+      <c r="G431" s="170"/>
+      <c r="H431" s="170"/>
+      <c r="I431" s="170"/>
+      <c r="J431" s="170"/>
       <c r="K431" s="96"/>
       <c r="L431" s="97"/>
     </row>
@@ -63539,18 +63539,18 @@
     <row r="470" spans="1:10" ht="12.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="C395:J395"/>
+    <mergeCell ref="C142:J142"/>
+    <mergeCell ref="C431:J431"/>
+    <mergeCell ref="C213:J213"/>
+    <mergeCell ref="C250:J250"/>
+    <mergeCell ref="C359:J359"/>
     <mergeCell ref="C2:J2"/>
     <mergeCell ref="C36:J36"/>
     <mergeCell ref="C177:J177"/>
     <mergeCell ref="C323:J323"/>
     <mergeCell ref="C70:J70"/>
     <mergeCell ref="C106:J106"/>
-    <mergeCell ref="C395:J395"/>
-    <mergeCell ref="C142:J142"/>
-    <mergeCell ref="C431:J431"/>
-    <mergeCell ref="C213:J213"/>
-    <mergeCell ref="C250:J250"/>
-    <mergeCell ref="C359:J359"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>